<commit_message>
Complete constrained alignment tree structure with all EVEs incorporated (references+curated)
</commit_message>
<xml_diff>
--- a/tabular/eve/ehbv-refseqs-side-data.xlsx
+++ b/tabular/eve/ehbv-refseqs-side-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C788DCA-DCA8-ED43-938A-8FC4A1CAD341}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3034E04A-8CAB-9945-9F3A-E570D1F63457}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
   <si>
     <t>host_sci_name</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Endogenous snake hepatitis B virus 1</t>
   </si>
   <si>
-    <t>eSNHBV1-con</t>
-  </si>
-  <si>
     <t>Crocodylus</t>
   </si>
   <si>
@@ -63,18 +60,9 @@
     <t>Chrysemys</t>
   </si>
   <si>
-    <t>eCRHBV-con</t>
-  </si>
-  <si>
     <t xml:space="preserve">Endogenous crocodile hepatitis B virus </t>
   </si>
   <si>
-    <t>eDRHPV</t>
-  </si>
-  <si>
-    <t>eTHBV-con</t>
-  </si>
-  <si>
     <t>Endogenous turtle hepatitis B virus</t>
   </si>
   <si>
@@ -84,9 +72,6 @@
     <t>Sphenodon</t>
   </si>
   <si>
-    <t>Fish</t>
-  </si>
-  <si>
     <t>tuatara</t>
   </si>
   <si>
@@ -96,9 +81,6 @@
     <t>Varanus komodoensis</t>
   </si>
   <si>
-    <t>eAVHBV1-con</t>
-  </si>
-  <si>
     <t>Endogenous avian hepatitis B virus 1</t>
   </si>
   <si>
@@ -111,36 +93,12 @@
     <t>birds</t>
   </si>
   <si>
-    <t>virus_name</t>
-  </si>
-  <si>
-    <t>virus_full_name</t>
-  </si>
-  <si>
-    <t>virus_genus</t>
-  </si>
-  <si>
     <t>clade</t>
   </si>
   <si>
-    <t>SphHBV-con</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
-    <t>eAvHBV1-con</t>
-  </si>
-  <si>
-    <t>eDrHPV-con</t>
-  </si>
-  <si>
-    <t>eCrHBV2-con</t>
-  </si>
-  <si>
-    <t>eSnHBV1-con</t>
-  </si>
-  <si>
     <t>eAVHBV2-con</t>
   </si>
   <si>
@@ -163,6 +121,69 @@
   </si>
   <si>
     <t>Ticks</t>
+  </si>
+  <si>
+    <t>full_name</t>
+  </si>
+  <si>
+    <t>locus_id</t>
+  </si>
+  <si>
+    <t>genus</t>
+  </si>
+  <si>
+    <t>EHBV-Avi.1-Aves-con</t>
+  </si>
+  <si>
+    <t>EHBV-Avi.2-Psittaciformes-con</t>
+  </si>
+  <si>
+    <t>EHBV-Avi.2-Psittaciformes</t>
+  </si>
+  <si>
+    <t>EHBV-Avi.1-Aves</t>
+  </si>
+  <si>
+    <t>EHBV-Herpeto.5-Testudines-con</t>
+  </si>
+  <si>
+    <t>EHBV-Herpeto.5-Testudines</t>
+  </si>
+  <si>
+    <t>EHBV-Meta.1-Sphenodon</t>
+  </si>
+  <si>
+    <t>EHBV-Herpeto.3-Crocodilia-con</t>
+  </si>
+  <si>
+    <t>EHBV-Herpeto.3-Crocodilia</t>
+  </si>
+  <si>
+    <t>EHBV-Herpeto.6-Varanus-con</t>
+  </si>
+  <si>
+    <t>EHBV-Herpeto.6-Varanus</t>
+  </si>
+  <si>
+    <t>EHBV-Herpeto.1-Serpentes-con</t>
+  </si>
+  <si>
+    <t>EHBV-Herpeto.1-Serpentes</t>
+  </si>
+  <si>
+    <t>EHBV-Herpeto.2-Serpentes-con</t>
+  </si>
+  <si>
+    <t>EHBV-Herpeto.2-Serpentes</t>
+  </si>
+  <si>
+    <t>Endogenous snake hepatitis B virus 2</t>
+  </si>
+  <si>
+    <t>Serpentes</t>
+  </si>
+  <si>
+    <t>Metahepadnavirus</t>
   </si>
 </sst>
 </file>
@@ -1471,16 +1492,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D7" sqref="A1:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="32.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="47.5" style="2" customWidth="1"/>
     <col min="4" max="5" width="23.5" style="2" customWidth="1"/>
     <col min="6" max="6" width="28.5" style="2" customWidth="1"/>
@@ -1490,19 +1511,19 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
@@ -1513,111 +1534,111 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>
@@ -1635,47 +1656,68 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>8</v>
+        <v>50</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="A9" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="B9" s="6" t="s">
         <v>42</v>
       </c>
+      <c r="C9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="5"/>
       <c r="F9" s="2" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E15" s="8"/>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E16" s="8"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G6" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Correcting alignment tree definition / updating side-data
</commit_message>
<xml_diff>
--- a/tabular/eve/ehbv-refseqs-side-data.xlsx
+++ b/tabular/eve/ehbv-refseqs-side-data.xlsx
@@ -1,18 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/eve/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99ADB10E-A1B2-FA4E-AC25-8FABDB83AE89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="3200" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$12</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
   <si>
     <t>host_sci_name</t>
   </si>
@@ -60,9 +66,6 @@
     <t>Endogenous turtle hepatitis B virus</t>
   </si>
   <si>
-    <t>Sphenodon hepatitis B virus</t>
-  </si>
-  <si>
     <t>Sphenodon</t>
   </si>
   <si>
@@ -93,9 +96,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>eAVHBV2-con</t>
-  </si>
-  <si>
     <t>Endogenous komodo dragon hepatitis B virus</t>
   </si>
   <si>
@@ -178,12 +178,45 @@
   </si>
   <si>
     <t>Metahepadnavirus</t>
+  </si>
+  <si>
+    <t>HVe1-MelUnd</t>
+  </si>
+  <si>
+    <t>EHBV-Herpeto.7-Paroedura</t>
+  </si>
+  <si>
+    <t>Melopsittacus</t>
+  </si>
+  <si>
+    <t>EHBV-Avi.3-Psittaciformes</t>
+  </si>
+  <si>
+    <t>budgerigar</t>
+  </si>
+  <si>
+    <t>Endogenous gekko hepatitis B virus</t>
+  </si>
+  <si>
+    <t>Paroedura</t>
+  </si>
+  <si>
+    <t>ocelot gekko</t>
+  </si>
+  <si>
+    <t>Endogenous tuatara hepatitis B virus</t>
+  </si>
+  <si>
+    <t>family</t>
+  </si>
+  <si>
+    <t>Hepadnaviridae</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -237,7 +270,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -274,6 +307,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAB82FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -711,7 +762,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -723,6 +774,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="425">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1153,6 +1207,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFAB82FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1485,236 +1544,323 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="A1:G10"/>
+      <selection activeCell="D8" sqref="A1:H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="32.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="47.5" style="2" customWidth="1"/>
-    <col min="4" max="5" width="23.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="28.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="25.83203125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="25" style="2" customWidth="1"/>
+    <col min="5" max="6" width="23.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="28.5" style="2" customWidth="1"/>
+    <col min="8" max="8" width="25.83203125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="D6" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="F6" s="5"/>
       <c r="G6" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="H6" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="5"/>
+      <c r="G7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="D8" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="5"/>
+      <c r="G9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="E12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="H12" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="E16" s="8"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F15" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G6"/>
+  <autoFilter ref="A1:H5" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H11">
+    <sortCondition ref="E2:E11"/>
+  </sortState>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Refactoring associated with discovery of new avian EVEs
</commit_message>
<xml_diff>
--- a/tabular/eve/ehbv-refseqs-side-data.xlsx
+++ b/tabular/eve/ehbv-refseqs-side-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99ADB10E-A1B2-FA4E-AC25-8FABDB83AE89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33315A78-B12D-E34D-B57A-90997DE53CF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$2</definedName>
   </definedNames>
   <calcPr calcId="140000"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="84">
   <si>
     <t>host_sci_name</t>
   </si>
@@ -39,66 +39,21 @@
     <t>Herpetohepadnavirus</t>
   </si>
   <si>
-    <t>Colubroidea</t>
-  </si>
-  <si>
-    <t>snakes</t>
-  </si>
-  <si>
-    <t>Endogenous snake hepatitis B virus 1</t>
-  </si>
-  <si>
-    <t>Crocodylus</t>
-  </si>
-  <si>
-    <t>crocodiles and gharial</t>
-  </si>
-  <si>
-    <t>turtles</t>
-  </si>
-  <si>
-    <t>Chrysemys</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endogenous crocodile hepatitis B virus </t>
-  </si>
-  <si>
-    <t>Endogenous turtle hepatitis B virus</t>
-  </si>
-  <si>
     <t>Sphenodon</t>
   </si>
   <si>
-    <t>tuatara</t>
-  </si>
-  <si>
-    <t>Komodo dragon</t>
-  </si>
-  <si>
-    <t>Varanus komodoensis</t>
-  </si>
-  <si>
-    <t>Endogenous avian hepatitis B virus 1</t>
-  </si>
-  <si>
     <t>Avihepadnavirus</t>
   </si>
   <si>
     <t>Neognathae</t>
   </si>
   <si>
-    <t>birds</t>
-  </si>
-  <si>
     <t>clade</t>
   </si>
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>Endogenous komodo dragon hepatitis B virus</t>
-  </si>
-  <si>
     <t>HEART-con</t>
   </si>
   <si>
@@ -126,91 +81,205 @@
     <t>genus</t>
   </si>
   <si>
-    <t>EHBV-Avi.1-Aves-con</t>
-  </si>
-  <si>
-    <t>EHBV-Avi.2-Psittaciformes-con</t>
-  </si>
-  <si>
-    <t>EHBV-Avi.2-Psittaciformes</t>
-  </si>
-  <si>
-    <t>EHBV-Avi.1-Aves</t>
-  </si>
-  <si>
-    <t>EHBV-Herpeto.5-Testudines-con</t>
-  </si>
-  <si>
-    <t>EHBV-Herpeto.5-Testudines</t>
-  </si>
-  <si>
-    <t>EHBV-Meta.1-Sphenodon</t>
-  </si>
-  <si>
-    <t>EHBV-Herpeto.3-Crocodilia-con</t>
-  </si>
-  <si>
-    <t>EHBV-Herpeto.3-Crocodilia</t>
-  </si>
-  <si>
-    <t>EHBV-Herpeto.6-Varanus-con</t>
-  </si>
-  <si>
-    <t>EHBV-Herpeto.6-Varanus</t>
-  </si>
-  <si>
-    <t>EHBV-Herpeto.1-Serpentes-con</t>
-  </si>
-  <si>
-    <t>EHBV-Herpeto.1-Serpentes</t>
-  </si>
-  <si>
-    <t>EHBV-Herpeto.2-Serpentes-con</t>
-  </si>
-  <si>
-    <t>EHBV-Herpeto.2-Serpentes</t>
-  </si>
-  <si>
-    <t>Endogenous snake hepatitis B virus 2</t>
-  </si>
-  <si>
     <t>Serpentes</t>
   </si>
   <si>
     <t>Metahepadnavirus</t>
   </si>
   <si>
-    <t>HVe1-MelUnd</t>
-  </si>
-  <si>
-    <t>EHBV-Herpeto.7-Paroedura</t>
-  </si>
-  <si>
     <t>Melopsittacus</t>
   </si>
   <si>
-    <t>EHBV-Avi.3-Psittaciformes</t>
-  </si>
-  <si>
-    <t>budgerigar</t>
-  </si>
-  <si>
-    <t>Endogenous gekko hepatitis B virus</t>
-  </si>
-  <si>
     <t>Paroedura</t>
   </si>
   <si>
-    <t>ocelot gekko</t>
-  </si>
-  <si>
-    <t>Endogenous tuatara hepatitis B virus</t>
-  </si>
-  <si>
     <t>family</t>
   </si>
   <si>
     <t>Hepadnaviridae</t>
+  </si>
+  <si>
+    <t>ehbv-ave.1-neognathea</t>
+  </si>
+  <si>
+    <t>ehbv-ave.2-passeriformes</t>
+  </si>
+  <si>
+    <t>ehbv-ave.3-passeriformes</t>
+  </si>
+  <si>
+    <t>ehbv-ave.5-passeriformes</t>
+  </si>
+  <si>
+    <t>ehbv-ave.6-passeriformes</t>
+  </si>
+  <si>
+    <t>ehbv-ave.7-passeriformes</t>
+  </si>
+  <si>
+    <t>ehbv-ave.8-passeriformes</t>
+  </si>
+  <si>
+    <t>ehbv-ave.9-melopsittacus</t>
+  </si>
+  <si>
+    <t>ehbv-ave.10-melopsittacus</t>
+  </si>
+  <si>
+    <t>ehbv-ave.11-tyto</t>
+  </si>
+  <si>
+    <t>ehbv-ave.12-anser</t>
+  </si>
+  <si>
+    <t>ehbv-ave.13-paleognathae-con</t>
+  </si>
+  <si>
+    <t>ehbv-ave.14-gaviiformes</t>
+  </si>
+  <si>
+    <t>ehbv-ave.16-accipter</t>
+  </si>
+  <si>
+    <t>ehbv-ave.17-passeriformes-con</t>
+  </si>
+  <si>
+    <t>ehbv-ave.18-calypte</t>
+  </si>
+  <si>
+    <t>ehbv-ave.19-buceros</t>
+  </si>
+  <si>
+    <t>ehbv-ave.20-cariama</t>
+  </si>
+  <si>
+    <t>ehbv-herpeto.1-serpentes-con</t>
+  </si>
+  <si>
+    <t>ehbv-herpeto.3-crocodilia-con</t>
+  </si>
+  <si>
+    <t>ehbv-herpeto.5-testudines-con</t>
+  </si>
+  <si>
+    <t>ehbv-herpeto.6-varanus-con</t>
+  </si>
+  <si>
+    <t>ehbv-herpeto.7-paroedura</t>
+  </si>
+  <si>
+    <t>ehbv-meta.1-sphenodon</t>
+  </si>
+  <si>
+    <t>Passeriformes</t>
+  </si>
+  <si>
+    <t>Endogenous avehepadnairus 1</t>
+  </si>
+  <si>
+    <t>Endogenous avehepadnairus 2</t>
+  </si>
+  <si>
+    <t>Endogenous avehepadnairus 3</t>
+  </si>
+  <si>
+    <t>Endogenous avehepadnairus 4</t>
+  </si>
+  <si>
+    <t>Endogenous avehepadnairus 6</t>
+  </si>
+  <si>
+    <t>Endogenous avehepadnairus 7</t>
+  </si>
+  <si>
+    <t>Endogenous avehepadnairus 8</t>
+  </si>
+  <si>
+    <t>Endogenous avehepadnairus 9</t>
+  </si>
+  <si>
+    <t>Endogenous avehepadnairus 10</t>
+  </si>
+  <si>
+    <t>Endogenous avehepadnairus 11</t>
+  </si>
+  <si>
+    <t>Endogenous avehepadnairus 12</t>
+  </si>
+  <si>
+    <t>Endogenous avehepadnairus 13</t>
+  </si>
+  <si>
+    <t>Endogenous avehepadnairus 14</t>
+  </si>
+  <si>
+    <t>Endogenous avehepadnairus 16</t>
+  </si>
+  <si>
+    <t>Endogenous avehepadnairus 17</t>
+  </si>
+  <si>
+    <t>Endogenous avehepadnairus 18</t>
+  </si>
+  <si>
+    <t>Endogenous avehepadnairus 19</t>
+  </si>
+  <si>
+    <t>Endogenous avehepadnairus 20</t>
+  </si>
+  <si>
+    <t>Endogenous herpetohepadnairus 1</t>
+  </si>
+  <si>
+    <t>Endogenous herpetohepadnairus 3</t>
+  </si>
+  <si>
+    <t>Endogenous herpetohepadnairus 5</t>
+  </si>
+  <si>
+    <t>Endogenous herpetohepadnairus 6</t>
+  </si>
+  <si>
+    <t>Endogenous herpetohepadnairus 7</t>
+  </si>
+  <si>
+    <t>Endogenous metahepadnairus 1</t>
+  </si>
+  <si>
+    <t>Tyto</t>
+  </si>
+  <si>
+    <t>Anser</t>
+  </si>
+  <si>
+    <t>Paleognathae</t>
+  </si>
+  <si>
+    <t>Gaviiformes</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Accipiter</t>
+  </si>
+  <si>
+    <t>Calypte</t>
+  </si>
+  <si>
+    <t>Buceros</t>
+  </si>
+  <si>
+    <t>Cariama</t>
+  </si>
+  <si>
+    <t>Crocodilia</t>
+  </si>
+  <si>
+    <t>Testudines</t>
+  </si>
+  <si>
+    <t>Varanus</t>
   </si>
 </sst>
 </file>
@@ -270,7 +339,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -309,18 +378,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFAB82FF"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -762,21 +819,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="425">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1545,10 +1599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="A1:H12"/>
+      <selection activeCell="E13" sqref="A1:H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1557,7 +1611,8 @@
     <col min="2" max="2" width="32.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="47.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="25" style="2" customWidth="1"/>
-    <col min="5" max="6" width="23.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="7.83203125" style="2" customWidth="1"/>
     <col min="7" max="7" width="28.5" style="2" customWidth="1"/>
     <col min="8" max="8" width="25.83203125" style="2" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="2"/>
@@ -1565,22 +1620,22 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
@@ -1590,277 +1645,584 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>19</v>
+      <c r="A2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="7"/>
+      <c r="A3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="G3" s="2" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>17</v>
+        <v>24</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="D7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" s="4" t="s">
+      <c r="D9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="G9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="H9" s="2" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="D15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F15" s="8"/>
+      <c r="G21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H5" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H11">
-    <sortCondition ref="E2:E11"/>
-  </sortState>
+  <autoFilter ref="A1:H1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Updated refcon side data
</commit_message>
<xml_diff>
--- a/tabular/eve/ehbv-refseqs-side-data.xlsx
+++ b/tabular/eve/ehbv-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A545F9BE-41DF-974C-8DCA-D5A4F2100ABA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5267815-86AD-0E45-9619-F7CBF69230D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="93">
   <si>
     <t>host_sci_name</t>
   </si>
@@ -174,78 +174,6 @@
     <t>Passeriformes</t>
   </si>
   <si>
-    <t>Endogenous avehepadnairus 1</t>
-  </si>
-  <si>
-    <t>Endogenous avehepadnairus 2</t>
-  </si>
-  <si>
-    <t>Endogenous avehepadnairus 3</t>
-  </si>
-  <si>
-    <t>Endogenous avehepadnairus 4</t>
-  </si>
-  <si>
-    <t>Endogenous avehepadnairus 6</t>
-  </si>
-  <si>
-    <t>Endogenous avehepadnairus 7</t>
-  </si>
-  <si>
-    <t>Endogenous avehepadnairus 8</t>
-  </si>
-  <si>
-    <t>Endogenous avehepadnairus 9</t>
-  </si>
-  <si>
-    <t>Endogenous avehepadnairus 10</t>
-  </si>
-  <si>
-    <t>Endogenous avehepadnairus 11</t>
-  </si>
-  <si>
-    <t>Endogenous avehepadnairus 12</t>
-  </si>
-  <si>
-    <t>Endogenous avehepadnairus 13</t>
-  </si>
-  <si>
-    <t>Endogenous avehepadnairus 14</t>
-  </si>
-  <si>
-    <t>Endogenous avehepadnairus 16</t>
-  </si>
-  <si>
-    <t>Endogenous avehepadnairus 17</t>
-  </si>
-  <si>
-    <t>Endogenous avehepadnairus 18</t>
-  </si>
-  <si>
-    <t>Endogenous avehepadnairus 19</t>
-  </si>
-  <si>
-    <t>Endogenous avehepadnairus 20</t>
-  </si>
-  <si>
-    <t>Endogenous herpetohepadnairus 1</t>
-  </si>
-  <si>
-    <t>Endogenous herpetohepadnairus 3</t>
-  </si>
-  <si>
-    <t>Endogenous herpetohepadnairus 5</t>
-  </si>
-  <si>
-    <t>Endogenous herpetohepadnairus 6</t>
-  </si>
-  <si>
-    <t>Endogenous herpetohepadnairus 7</t>
-  </si>
-  <si>
-    <t>Endogenous metahepadnairus 1</t>
-  </si>
-  <si>
     <t>Tyto</t>
   </si>
   <si>
@@ -283,6 +211,102 @@
   </si>
   <si>
     <t>ehbv-ave.1-neognathae-con</t>
+  </si>
+  <si>
+    <t>ehbv-meta.5-neoaves</t>
+  </si>
+  <si>
+    <t>Endogenous x 1</t>
+  </si>
+  <si>
+    <t>Endogenous herpetohepadnavirus 3</t>
+  </si>
+  <si>
+    <t>Endogenous herpetohepadnavirus 5</t>
+  </si>
+  <si>
+    <t>Endogenous herpetohepadnavirus 6</t>
+  </si>
+  <si>
+    <t>Endogenous herpetohepadnavirus 7</t>
+  </si>
+  <si>
+    <t>Endogenous metahepadnavirus 1</t>
+  </si>
+  <si>
+    <t>Endogenous metahepadnavirus 2</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 1</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 2</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 3</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 4</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 6</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 7</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 8</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 9</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 10</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 11</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 12</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 13</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 14</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 16</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 17</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 18</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 19</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 20</t>
+  </si>
+  <si>
+    <t>ehbv-meta.2-paroedura</t>
+  </si>
+  <si>
+    <t>ehbv-meta.3-pelusios</t>
+  </si>
+  <si>
+    <t>ehbv-meta.4-pelusios</t>
+  </si>
+  <si>
+    <t>paroedura</t>
+  </si>
+  <si>
+    <t>pelusios</t>
+  </si>
+  <si>
+    <t>neoaves</t>
   </si>
 </sst>
 </file>
@@ -1602,10 +1626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G13" sqref="A1:H26"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1672,245 +1696,244 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>4</v>
+      <c r="A3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="7"/>
+      <c r="A4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>2</v>
+      </c>
       <c r="G4" s="2" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>4</v>
+      <c r="A5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>4</v>
+      <c r="A6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>4</v>
+      <c r="A7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>4</v>
+      <c r="A8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>4</v>
+      <c r="A9" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>4</v>
+      <c r="A10" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>19</v>
+        <v>91</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>4</v>
+      <c r="A11" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>19</v>
+        <v>91</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>4</v>
+      <c r="A12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>22</v>
@@ -1919,21 +1942,21 @@
         <v>4</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>73</v>
+        <v>5</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>22</v>
@@ -1941,22 +1964,23 @@
       <c r="E14" s="6" t="s">
         <v>4</v>
       </c>
+      <c r="F14" s="7"/>
       <c r="G14" s="2" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>22</v>
@@ -1965,21 +1989,21 @@
         <v>4</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>22</v>
@@ -1988,21 +2012,21 @@
         <v>4</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>22</v>
@@ -2014,18 +2038,18 @@
         <v>47</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>22</v>
@@ -2034,21 +2058,21 @@
         <v>4</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>22</v>
@@ -2057,21 +2081,21 @@
         <v>4</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>22</v>
@@ -2080,148 +2104,240 @@
         <v>4</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>2</v>
+      <c r="E21" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>2</v>
+      <c r="E22" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>2</v>
+      <c r="E23" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>2</v>
+      <c r="E24" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>70</v>
+        <v>35</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>81</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>2</v>
+      <c r="E25" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>18</v>
+      <c r="E26" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected typo in genus name
</commit_message>
<xml_diff>
--- a/tabular/eve/ehbv-refseqs-side-data.xlsx
+++ b/tabular/eve/ehbv-refseqs-side-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/eve/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anna/Projects/virus/Hepadnaviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5267815-86AD-0E45-9619-F7CBF69230D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AA28D4-5ADF-2044-B235-E56F1DF329B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="111">
   <si>
     <t>host_sci_name</t>
   </si>
@@ -210,9 +210,6 @@
     <t>Varanus</t>
   </si>
   <si>
-    <t>ehbv-ave.1-neognathae-con</t>
-  </si>
-  <si>
     <t>ehbv-meta.5-neoaves</t>
   </si>
   <si>
@@ -307,6 +304,63 @@
   </si>
   <si>
     <t>neoaves</t>
+  </si>
+  <si>
+    <t>ehbv-meta.5-neoavis</t>
+  </si>
+  <si>
+    <t>ehbv-avi.1-neognathae-con</t>
+  </si>
+  <si>
+    <t>ehbv-avi.2-passeriformes</t>
+  </si>
+  <si>
+    <t>ehbv-avi.3-passeriformes</t>
+  </si>
+  <si>
+    <t>ehbv-avi.5-passeriformes</t>
+  </si>
+  <si>
+    <t>ehbv-avi.6-passeriformes</t>
+  </si>
+  <si>
+    <t>ehbv-avi.7-passeriformes</t>
+  </si>
+  <si>
+    <t>ehbv-avi.8-passeriformes</t>
+  </si>
+  <si>
+    <t>ehbv-avi.9-melopsittacus</t>
+  </si>
+  <si>
+    <t>ehbv-avi.10-melopsittacus</t>
+  </si>
+  <si>
+    <t>ehbv-avi.11-tyto</t>
+  </si>
+  <si>
+    <t>ehbv-avi.12-anser</t>
+  </si>
+  <si>
+    <t>ehbv-avi.13-paleognathae-con</t>
+  </si>
+  <si>
+    <t>ehbv-avi.14-gaviiformes</t>
+  </si>
+  <si>
+    <t>ehbv-avi.16-accipter</t>
+  </si>
+  <si>
+    <t>ehbv-avi.17-passeriformes-con</t>
+  </si>
+  <si>
+    <t>ehbv-avi.18-calypte</t>
+  </si>
+  <si>
+    <t>ehbv-avi.19-buceros</t>
+  </si>
+  <si>
+    <t>ehbv-avi.20-cariama</t>
   </si>
 </sst>
 </file>
@@ -1628,8 +1682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C18" sqref="A1:H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1703,7 +1757,7 @@
         <v>41</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>22</v>
@@ -1726,7 +1780,7 @@
         <v>42</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>22</v>
@@ -1749,7 +1803,7 @@
         <v>43</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>22</v>
@@ -1772,7 +1826,7 @@
         <v>44</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>22</v>
@@ -1795,7 +1849,7 @@
         <v>45</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>22</v>
@@ -1818,7 +1872,7 @@
         <v>46</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>22</v>
@@ -1835,13 +1889,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>22</v>
@@ -1850,7 +1904,7 @@
         <v>18</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>52</v>
@@ -1858,13 +1912,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>22</v>
@@ -1873,7 +1927,7 @@
         <v>18</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>52</v>
@@ -1881,13 +1935,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>22</v>
@@ -1896,7 +1950,7 @@
         <v>18</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>52</v>
@@ -1904,13 +1958,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>22</v>
@@ -1919,7 +1973,7 @@
         <v>18</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>52</v>
@@ -1927,13 +1981,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>22</v>
@@ -1950,13 +2004,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>24</v>
+        <v>94</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>22</v>
@@ -1974,13 +2028,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>25</v>
+        <v>95</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>22</v>
@@ -1997,13 +2051,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>26</v>
+        <v>96</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>22</v>
@@ -2020,13 +2074,13 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>27</v>
+        <v>97</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>22</v>
@@ -2043,13 +2097,13 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>28</v>
+        <v>98</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>22</v>
@@ -2066,13 +2120,13 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>22</v>
@@ -2089,13 +2143,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>22</v>
@@ -2112,13 +2166,13 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>31</v>
+        <v>101</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>22</v>
@@ -2135,13 +2189,13 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>22</v>
@@ -2158,13 +2212,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>33</v>
+        <v>103</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>22</v>
@@ -2181,13 +2235,13 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>34</v>
+        <v>104</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>22</v>
@@ -2204,13 +2258,13 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>35</v>
+        <v>105</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>22</v>
@@ -2227,13 +2281,13 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>22</v>
@@ -2250,13 +2304,13 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>37</v>
+        <v>107</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>22</v>
@@ -2273,13 +2327,13 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>38</v>
+        <v>108</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>22</v>
@@ -2296,13 +2350,13 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>22</v>
@@ -2319,13 +2373,13 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>40</v>
+        <v>110</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Updated data in line with AAV-GLUE template
</commit_message>
<xml_diff>
--- a/tabular/eve/ehbv-refseqs-side-data.xlsx
+++ b/tabular/eve/ehbv-refseqs-side-data.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anna/Projects/virus/Hepadnaviridae-GLUE/tabular/eve/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AA28D4-5ADF-2044-B235-E56F1DF329B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FE14D7-5380-8B41-88BD-358B93E1BC3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="460" windowWidth="32720" windowHeight="17000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$14</definedName>
   </definedNames>
   <calcPr calcId="140000"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="151">
   <si>
     <t>host_sci_name</t>
   </si>
@@ -63,9 +63,6 @@
     <t>HEART consensus DS633349</t>
   </si>
   <si>
-    <t>HEART</t>
-  </si>
-  <si>
     <t>Ixodes</t>
   </si>
   <si>
@@ -99,60 +96,6 @@
     <t>Hepadnaviridae</t>
   </si>
   <si>
-    <t>ehbv-ave.1-neognathea</t>
-  </si>
-  <si>
-    <t>ehbv-ave.2-passeriformes</t>
-  </si>
-  <si>
-    <t>ehbv-ave.3-passeriformes</t>
-  </si>
-  <si>
-    <t>ehbv-ave.5-passeriformes</t>
-  </si>
-  <si>
-    <t>ehbv-ave.6-passeriformes</t>
-  </si>
-  <si>
-    <t>ehbv-ave.7-passeriformes</t>
-  </si>
-  <si>
-    <t>ehbv-ave.8-passeriformes</t>
-  </si>
-  <si>
-    <t>ehbv-ave.9-melopsittacus</t>
-  </si>
-  <si>
-    <t>ehbv-ave.10-melopsittacus</t>
-  </si>
-  <si>
-    <t>ehbv-ave.11-tyto</t>
-  </si>
-  <si>
-    <t>ehbv-ave.12-anser</t>
-  </si>
-  <si>
-    <t>ehbv-ave.13-paleognathae-con</t>
-  </si>
-  <si>
-    <t>ehbv-ave.14-gaviiformes</t>
-  </si>
-  <si>
-    <t>ehbv-ave.16-accipter</t>
-  </si>
-  <si>
-    <t>ehbv-ave.17-passeriformes-con</t>
-  </si>
-  <si>
-    <t>ehbv-ave.18-calypte</t>
-  </si>
-  <si>
-    <t>ehbv-ave.19-buceros</t>
-  </si>
-  <si>
-    <t>ehbv-ave.20-cariama</t>
-  </si>
-  <si>
     <t>ehbv-herpeto.1-serpentes-con</t>
   </si>
   <si>
@@ -165,9 +108,6 @@
     <t>ehbv-herpeto.6-varanus-con</t>
   </si>
   <si>
-    <t>ehbv-herpeto.7-paroedura</t>
-  </si>
-  <si>
     <t>ehbv-meta.1-sphenodon</t>
   </si>
   <si>
@@ -210,9 +150,6 @@
     <t>Varanus</t>
   </si>
   <si>
-    <t>ehbv-meta.5-neoaves</t>
-  </si>
-  <si>
     <t>Endogenous x 1</t>
   </si>
   <si>
@@ -225,9 +162,6 @@
     <t>Endogenous herpetohepadnavirus 6</t>
   </si>
   <si>
-    <t>Endogenous herpetohepadnavirus 7</t>
-  </si>
-  <si>
     <t>Endogenous metahepadnavirus 1</t>
   </si>
   <si>
@@ -288,12 +222,6 @@
     <t>Endogenous avihepadnavirus 20</t>
   </si>
   <si>
-    <t>ehbv-meta.2-paroedura</t>
-  </si>
-  <si>
-    <t>ehbv-meta.3-pelusios</t>
-  </si>
-  <si>
     <t>ehbv-meta.4-pelusios</t>
   </si>
   <si>
@@ -306,30 +234,15 @@
     <t>neoaves</t>
   </si>
   <si>
-    <t>ehbv-meta.5-neoavis</t>
-  </si>
-  <si>
-    <t>ehbv-avi.1-neognathae-con</t>
-  </si>
-  <si>
-    <t>ehbv-avi.2-passeriformes</t>
-  </si>
-  <si>
     <t>ehbv-avi.3-passeriformes</t>
   </si>
   <si>
-    <t>ehbv-avi.5-passeriformes</t>
-  </si>
-  <si>
     <t>ehbv-avi.6-passeriformes</t>
   </si>
   <si>
     <t>ehbv-avi.7-passeriformes</t>
   </si>
   <si>
-    <t>ehbv-avi.8-passeriformes</t>
-  </si>
-  <si>
     <t>ehbv-avi.9-melopsittacus</t>
   </si>
   <si>
@@ -339,35 +252,242 @@
     <t>ehbv-avi.11-tyto</t>
   </si>
   <si>
-    <t>ehbv-avi.12-anser</t>
-  </si>
-  <si>
-    <t>ehbv-avi.13-paleognathae-con</t>
-  </si>
-  <si>
     <t>ehbv-avi.14-gaviiformes</t>
   </si>
   <si>
     <t>ehbv-avi.16-accipter</t>
   </si>
   <si>
-    <t>ehbv-avi.17-passeriformes-con</t>
-  </si>
-  <si>
-    <t>ehbv-avi.18-calypte</t>
-  </si>
-  <si>
-    <t>ehbv-avi.19-buceros</t>
-  </si>
-  <si>
-    <t>ehbv-avi.20-cariama</t>
+    <t>included_msa</t>
+  </si>
+  <si>
+    <t>nearest_upstream_orf</t>
+  </si>
+  <si>
+    <t>nearest_downstream_orf</t>
+  </si>
+  <si>
+    <t>locus_numeric_id</t>
+  </si>
+  <si>
+    <t>num_seqs</t>
+  </si>
+  <si>
+    <t>minimum_age_ortho</t>
+  </si>
+  <si>
+    <t>host_group_taxlevel</t>
+  </si>
+  <si>
+    <t>host_group_name</t>
+  </si>
+  <si>
+    <t>ehbv-avi.15-gaviiformes</t>
+  </si>
+  <si>
+    <t>TSHZ1</t>
+  </si>
+  <si>
+    <t>ZNF516</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>ehbv-hepadna.1-paroedura</t>
+  </si>
+  <si>
+    <t>ehbv-meta.6-neoaves</t>
+  </si>
+  <si>
+    <t>ehbv-meta.3-paroedura</t>
+  </si>
+  <si>
+    <t>ehbv-meta.5-pelusios</t>
+  </si>
+  <si>
+    <t>ehbv-meta.2-varanus</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 15</t>
+  </si>
+  <si>
+    <t>Endogenous metahepadnavirus 3</t>
+  </si>
+  <si>
+    <t>Endogenous metahepadnavirus 4</t>
+  </si>
+  <si>
+    <t>Endogenous metahepadnavirus 5</t>
+  </si>
+  <si>
+    <t>ehbv-meta.6-neoavis</t>
+  </si>
+  <si>
+    <t>Endogenous metahepadnavirus 6</t>
+  </si>
+  <si>
+    <t>E2F7</t>
+  </si>
+  <si>
+    <t>neuron navigator 3</t>
+  </si>
+  <si>
+    <t>TIMM21/FBXO15</t>
+  </si>
+  <si>
+    <t>NETO1/CBLN2/lncRNA</t>
+  </si>
+  <si>
+    <t>Orthohepadnavirus</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>TE</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 5</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 21</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 22</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 23</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 24</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 25</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 26</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 27</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 28</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 29</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 30</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 31</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 32</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 33</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 34</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 35</t>
+  </si>
+  <si>
+    <t>ehbv-avi.17-Passeriformes</t>
+  </si>
+  <si>
+    <t>ehbv-avi.18-Calypte</t>
+  </si>
+  <si>
+    <t>ehbv-avi.19-Buceros</t>
+  </si>
+  <si>
+    <t>ehbv-avi.20-Cariama</t>
+  </si>
+  <si>
+    <t>ehbv-avi.21-Paleognathea</t>
+  </si>
+  <si>
+    <t>ehbv-avi.22-Tyto</t>
+  </si>
+  <si>
+    <t>ehbv-avi.23-Nothoprocta</t>
+  </si>
+  <si>
+    <t>ehbv-avi.24-Apaloderma</t>
+  </si>
+  <si>
+    <t>ehbv-avi.25-Sphenisciformes</t>
+  </si>
+  <si>
+    <t>ehbv-avi.26-Psittaciformes</t>
+  </si>
+  <si>
+    <t>ehbv-avi.27-Suliformes</t>
+  </si>
+  <si>
+    <t>ehbv-avi.28-Amazona</t>
+  </si>
+  <si>
+    <t>ehbv-avi.29-Psittacula</t>
+  </si>
+  <si>
+    <t>ehbv-avi.30-Anser</t>
+  </si>
+  <si>
+    <t>ehbv-avi.31-Passeriformes</t>
+  </si>
+  <si>
+    <t>ehbv-avi.32-Tinamiformes</t>
+  </si>
+  <si>
+    <t>ehbv-avi.33-Psittaciformes</t>
+  </si>
+  <si>
+    <t>ehbv-avi.34-Gallirallus</t>
+  </si>
+  <si>
+    <t>ehbv-avi.35-Chaetura</t>
+  </si>
+  <si>
+    <t>ehbv-avi.1-neoaves</t>
+  </si>
+  <si>
+    <t>ehbv-avi.2-estrildidae</t>
+  </si>
+  <si>
+    <t>ehbv-avi.4-passeriformes</t>
+  </si>
+  <si>
+    <t>ehbv-avi.8-australiaves</t>
+  </si>
+  <si>
+    <t>ehbv-avi.12-anatidae</t>
+  </si>
+  <si>
+    <t>ehbv-avi.13-paleognathea</t>
+  </si>
+  <si>
+    <t>ehbv-avi.5-unranked</t>
+  </si>
+  <si>
+    <t>Endogenous hepadnavirus 1</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -419,8 +539,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -463,6 +615,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFAFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -900,7 +1070,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -912,6 +1082,41 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="425">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1344,6 +1549,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFAFFF"/>
       <color rgb="FFAB82FF"/>
     </mruColors>
   </colors>
@@ -1680,722 +1886,1747 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C18" sqref="A1:H30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="A1:P48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="47.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="25" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="7.83203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="28.5" style="2" customWidth="1"/>
-    <col min="8" max="8" width="25.83203125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="47.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="21.5" style="7" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="25.5" style="2" customWidth="1"/>
+    <col min="9" max="9" width="27.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="25" style="2" customWidth="1"/>
+    <col min="11" max="11" width="23.5" style="2" customWidth="1"/>
+    <col min="12" max="12" width="16" style="2" customWidth="1"/>
+    <col min="13" max="13" width="32.5" style="10" customWidth="1"/>
+    <col min="14" max="14" width="32.5" style="2" customWidth="1"/>
+    <col min="15" max="15" width="28.5" style="2" customWidth="1"/>
+    <col min="16" max="16" width="25.83203125" style="2" customWidth="1"/>
+    <col min="17" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="D1" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="M1" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="22">
+        <v>1</v>
+      </c>
+      <c r="E3" s="22"/>
+      <c r="F3" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="J3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" s="4"/>
+      <c r="O3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="22">
+        <v>2</v>
+      </c>
+      <c r="E4" s="22"/>
+      <c r="F4" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="22">
+        <v>5</v>
+      </c>
+      <c r="E5" s="22"/>
+      <c r="F5" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="J5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="22">
+        <v>6</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="N6" s="4"/>
+      <c r="O6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="23">
+        <v>1</v>
+      </c>
+      <c r="E7" s="23">
+        <v>1</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="N7" s="3"/>
+      <c r="O7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="23">
+        <v>2</v>
+      </c>
+      <c r="E8" s="23">
+        <v>1</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="N8" s="3"/>
+      <c r="O8" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="23">
+        <v>3</v>
+      </c>
+      <c r="E9" s="23">
+        <v>1</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="N9" s="3"/>
+      <c r="O9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="23">
+        <v>4</v>
+      </c>
+      <c r="E10" s="23">
+        <v>1</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="N10" s="3"/>
+      <c r="O10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="23">
+        <v>5</v>
+      </c>
+      <c r="E11" s="23">
+        <v>1</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="N11" s="3"/>
+      <c r="O11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="23">
+        <v>6</v>
+      </c>
+      <c r="E12" s="23"/>
+      <c r="F12" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="24">
+        <v>1</v>
+      </c>
+      <c r="E13" s="24"/>
+      <c r="F13" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D14" s="25">
+        <v>1</v>
+      </c>
+      <c r="E14" s="25"/>
+      <c r="F14" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D15" s="25">
+        <v>2</v>
+      </c>
+      <c r="E15" s="25"/>
+      <c r="F15" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="25">
+        <v>3</v>
+      </c>
+      <c r="E16" s="25"/>
+      <c r="F16" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="D17" s="25">
+        <v>4</v>
+      </c>
+      <c r="E17" s="25"/>
+      <c r="F17" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D18" s="25">
+        <v>5</v>
+      </c>
+      <c r="E18" s="25"/>
+      <c r="F18" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="25">
+        <v>6</v>
+      </c>
+      <c r="E19" s="25"/>
+      <c r="F19" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K19" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="25">
+        <v>7</v>
+      </c>
+      <c r="E20" s="25"/>
+      <c r="F20" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D21" s="25">
+        <v>8</v>
+      </c>
+      <c r="E21" s="25"/>
+      <c r="F21" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="25">
+        <v>9</v>
+      </c>
+      <c r="E22" s="25"/>
+      <c r="F22" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="25">
         <v>10</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E23" s="25"/>
+      <c r="F23" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="I23" s="5"/>
+      <c r="J23" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="25">
         <v>11</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8" t="s">
+      <c r="E24" s="25"/>
+      <c r="F24" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D25" s="25">
         <v>12</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="E25" s="25"/>
+      <c r="F25" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K25" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D26" s="25">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="E26" s="25"/>
+      <c r="F26" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K26" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="25">
+        <v>14</v>
+      </c>
+      <c r="E27" s="25"/>
+      <c r="F27" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K27" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="25">
+        <v>15</v>
+      </c>
+      <c r="E28" s="25"/>
+      <c r="F28" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K28" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" s="25">
+        <v>16</v>
+      </c>
+      <c r="E29" s="25"/>
+      <c r="F29" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="I29" s="5"/>
+      <c r="J29" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K29" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D30" s="25">
+        <v>17</v>
+      </c>
+      <c r="E30" s="25"/>
+      <c r="F30" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K30" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="C31" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D31" s="25">
+        <v>18</v>
+      </c>
+      <c r="E31" s="25"/>
+      <c r="F31" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K31" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D32" s="25">
+        <v>19</v>
+      </c>
+      <c r="E32" s="25"/>
+      <c r="F32" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K32" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D33" s="25">
+        <v>20</v>
+      </c>
+      <c r="E33" s="25"/>
+      <c r="F33" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K33" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D34" s="25">
+        <v>21</v>
+      </c>
+      <c r="E34" s="25"/>
+      <c r="F34" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K34" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D35" s="25">
         <v>22</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="E35" s="25"/>
+      <c r="F35" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K35" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D36" s="25">
         <v>23</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="6" t="s">
+      <c r="E36" s="25"/>
+      <c r="F36" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K36" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D37" s="25">
         <v>24</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="6" t="s">
+      <c r="E37" s="25"/>
+      <c r="F37" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K37" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B15" s="2" t="s">
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D38" s="25">
         <v>25</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="6" t="s">
+      <c r="E38" s="25"/>
+      <c r="F38" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K38" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B16" s="2" t="s">
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D39" s="25">
         <v>26</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="6" t="s">
+      <c r="E39" s="25"/>
+      <c r="F39" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K39" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D40" s="25">
         <v>27</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="6" t="s">
+      <c r="E40" s="25"/>
+      <c r="F40" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K40" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B18" s="2" t="s">
+      <c r="L40" s="6"/>
+      <c r="M40" s="6"/>
+      <c r="N40" s="6"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41" s="25">
         <v>28</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="6" t="s">
+      <c r="E41" s="25"/>
+      <c r="F41" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K41" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B19" s="2" t="s">
+      <c r="L41" s="6"/>
+      <c r="M41" s="6"/>
+      <c r="N41" s="6"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D42" s="25">
         <v>29</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="6" t="s">
+      <c r="E42" s="25"/>
+      <c r="F42" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K42" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B20" s="2" t="s">
+      <c r="L42" s="6"/>
+      <c r="M42" s="6"/>
+      <c r="N42" s="6"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D43" s="25">
         <v>30</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="6" t="s">
+      <c r="E43" s="25"/>
+      <c r="F43" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K43" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B21" s="2" t="s">
+      <c r="L43" s="6"/>
+      <c r="M43" s="6"/>
+      <c r="N43" s="6"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D44" s="25">
         <v>31</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="6" t="s">
+      <c r="E44" s="25"/>
+      <c r="F44" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K44" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="6" t="s">
+      <c r="L44" s="6"/>
+      <c r="M44" s="6"/>
+      <c r="N44" s="6"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D45" s="25">
+        <v>32</v>
+      </c>
+      <c r="E45" s="25"/>
+      <c r="F45" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K45" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B23" s="2" t="s">
+      <c r="L45" s="6"/>
+      <c r="M45" s="6"/>
+      <c r="N45" s="6"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D46" s="25">
         <v>33</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="6" t="s">
+      <c r="E46" s="25"/>
+      <c r="F46" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K46" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B24" s="2" t="s">
+      <c r="L46" s="6"/>
+      <c r="M46" s="6"/>
+      <c r="N46" s="6"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D47" s="25">
         <v>34</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="6" t="s">
+      <c r="E47" s="25"/>
+      <c r="F47" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K47" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B25" s="2" t="s">
+      <c r="L47" s="6"/>
+      <c r="M47" s="6"/>
+      <c r="N47" s="6"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="D48" s="25">
         <v>35</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E25" s="6" t="s">
+      <c r="E48" s="25"/>
+      <c r="F48" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K48" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G25" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>52</v>
-      </c>
+      <c r="L48" s="6"/>
+      <c r="M48" s="6"/>
+      <c r="N48" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:P1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P13">
+    <sortCondition ref="K3:K13"/>
+    <sortCondition ref="D3:D13"/>
+  </sortState>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Updated EHBV side data
</commit_message>
<xml_diff>
--- a/tabular/eve/ehbv-refseqs-side-data.xlsx
+++ b/tabular/eve/ehbv-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FE14D7-5380-8B41-88BD-358B93E1BC3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAC3FB6-F1E6-AD41-9EFE-6B2909781BE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="460" windowWidth="32720" windowHeight="17000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="152">
   <si>
     <t>host_sci_name</t>
   </si>
@@ -481,6 +481,9 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -1889,7 +1892,7 @@
   <dimension ref="A1:P48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="A1:P48"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2304,7 +2307,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>87</v>
+        <v>151</v>
       </c>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>

</xml_diff>

<commit_message>
updated flanking genes for most
</commit_message>
<xml_diff>
--- a/tabular/eve/ehbv-refseqs-side-data.xlsx
+++ b/tabular/eve/ehbv-refseqs-side-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/eve/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anna/Projects/virus/Hepadnaviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAC3FB6-F1E6-AD41-9EFE-6B2909781BE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F2EE41-A75A-0541-B4E7-13D713EA0B89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="460" windowWidth="32720" windowHeight="17000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="460" windowWidth="25060" windowHeight="16420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,16 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$14</definedName>
   </definedNames>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -28,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="231">
   <si>
     <t>host_sci_name</t>
   </si>
@@ -321,18 +329,12 @@
     <t>Endogenous metahepadnavirus 5</t>
   </si>
   <si>
-    <t>ehbv-meta.6-neoavis</t>
-  </si>
-  <si>
     <t>Endogenous metahepadnavirus 6</t>
   </si>
   <si>
     <t>E2F7</t>
   </si>
   <si>
-    <t>neuron navigator 3</t>
-  </si>
-  <si>
     <t>TIMM21/FBXO15</t>
   </si>
   <si>
@@ -484,6 +486,249 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>WSCD2 (intronic)</t>
+  </si>
+  <si>
+    <t>NAV3</t>
+  </si>
+  <si>
+    <t>PCDH18</t>
+  </si>
+  <si>
+    <t>PCDH10</t>
+  </si>
+  <si>
+    <t>TAS1R3</t>
+  </si>
+  <si>
+    <t>DVL1</t>
+  </si>
+  <si>
+    <t>THBS1</t>
+  </si>
+  <si>
+    <t>KATNBL1</t>
+  </si>
+  <si>
+    <t>GRM7</t>
+  </si>
+  <si>
+    <t>ENSDNVG00000004794/LMCD1</t>
+  </si>
+  <si>
+    <t>BCKDHB</t>
+  </si>
+  <si>
+    <t>ENSDNVG00000017897</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.1-Neoaves</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.2-Estrildidae</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.3-Passeriformes</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.4-Passeriformes</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.5-Unranked</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.6-Passeriformes</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.7-Passeriformes</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.8-Australiaves</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.9-Melopsittacus</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.10-Melopsittacus</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.11-Tyto</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.12-Anatidas</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.13-Paleognathea</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.14-Gaviiformes</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.15-Gaviiformes</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.16-Accipter</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.17-Passeriformes</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.18-Calypte</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.19-Buceros</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.20-Cariama</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.21-Paleognathea</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.22-Tyto</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.23-Nothoprocta</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.24-Apaloderma</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.25-Sphenisciformes</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.26-Psittaciformes</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.27-Suliformes</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.28-Amazona</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.29-Psittacula</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.30-Anser</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.31-Passeriformes</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.32-Tinamiformes</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.33-Psittaciformes</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.34-Gallirallus</t>
+  </si>
+  <si>
+    <t>eHBV-Avi.35-Chaetura</t>
+  </si>
+  <si>
+    <t>FRY (intronic)</t>
+  </si>
+  <si>
+    <t>DHX32 (intronic)</t>
+  </si>
+  <si>
+    <t>SCN3B (intronic)</t>
+  </si>
+  <si>
+    <t>CDH23 (intronic)</t>
+  </si>
+  <si>
+    <t>LMO3</t>
+  </si>
+  <si>
+    <t>nk</t>
+  </si>
+  <si>
+    <t>FOXD3</t>
+  </si>
+  <si>
+    <t>ATG4C</t>
+  </si>
+  <si>
+    <t>SNORA13</t>
+  </si>
+  <si>
+    <t>MAST3 (intronic)</t>
+  </si>
+  <si>
+    <t>Get from paper</t>
+  </si>
+  <si>
+    <t>OLFM4</t>
+  </si>
+  <si>
+    <t>ENSTGUG00000000478</t>
+  </si>
+  <si>
+    <t>LRRC2</t>
+  </si>
+  <si>
+    <t>SUPT7L</t>
+  </si>
+  <si>
+    <t>ENSZALG00000002917</t>
+  </si>
+  <si>
+    <t>ENSACOG00000002175</t>
+  </si>
+  <si>
+    <t>ENSACOG00000002296</t>
+  </si>
+  <si>
+    <t>ENSANIG00000016593</t>
+  </si>
+  <si>
+    <t>ENSACDG00005009727</t>
+  </si>
+  <si>
+    <t>CCDC58</t>
+  </si>
+  <si>
+    <t>MYBL2</t>
+  </si>
+  <si>
+    <t>PTPRT</t>
+  </si>
+  <si>
+    <t>TMEM182 (intronic)</t>
+  </si>
+  <si>
+    <t>ENSABRG00000002559</t>
+  </si>
+  <si>
+    <t>ENSMUNG00000011927/CHSY3</t>
+  </si>
+  <si>
+    <t>ENSMUNG00000011929/HINT1</t>
+  </si>
+  <si>
+    <t>ARMC1</t>
+  </si>
+  <si>
+    <t>CYP7B1</t>
+  </si>
+  <si>
+    <t>ENSSCUG00000017518 (intronic)/TSKU</t>
+  </si>
+  <si>
+    <t>ENSSCUG00000017518 (intronic)/EMSY</t>
+  </si>
+  <si>
+    <t>Turaco</t>
+  </si>
+  <si>
+    <t>TMEM8B</t>
+  </si>
+  <si>
+    <t>ENSACUG00000013925</t>
   </si>
 </sst>
 </file>
@@ -1889,22 +2134,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P48"/>
+  <dimension ref="A1:P49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="47.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="32.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="21.5" style="7" customWidth="1"/>
-    <col min="7" max="7" width="24.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="25.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="29.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="7" customWidth="1"/>
+    <col min="6" max="6" width="11.5" style="7" customWidth="1"/>
+    <col min="7" max="7" width="40" style="2" customWidth="1"/>
+    <col min="8" max="8" width="22.83203125" style="2" customWidth="1"/>
     <col min="9" max="9" width="27.6640625" style="2" customWidth="1"/>
     <col min="10" max="10" width="25" style="2" customWidth="1"/>
     <col min="11" max="11" width="23.5" style="2" customWidth="1"/>
@@ -1979,16 +2225,16 @@
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
       <c r="F2" s="20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G2" s="16"/>
       <c r="H2" s="16"/>
       <c r="I2" s="16"/>
       <c r="J2" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
@@ -2136,10 +2382,14 @@
       <c r="F6" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="G6" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>150</v>
+      </c>
       <c r="I6" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>21</v>
@@ -2151,7 +2401,7 @@
         <v>32</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="2" t="s">
@@ -2183,7 +2433,7 @@
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
       <c r="I7" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>21</v>
@@ -2195,7 +2445,7 @@
         <v>32</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="N7" s="3"/>
       <c r="O7" s="2" t="s">
@@ -2227,7 +2477,7 @@
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
       <c r="I8" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>21</v>
@@ -2239,7 +2489,7 @@
         <v>32</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="N8" s="3"/>
       <c r="O8" s="2" t="s">
@@ -2268,7 +2518,7 @@
       <c r="G9" s="16"/>
       <c r="H9" s="16"/>
       <c r="I9" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>21</v>
@@ -2280,7 +2530,7 @@
         <v>32</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="2" t="s">
@@ -2307,12 +2557,12 @@
         <v>1</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
       <c r="I10" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>21</v>
@@ -2324,7 +2574,7 @@
         <v>32</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="N10" s="3"/>
       <c r="O10" s="2" t="s">
@@ -2356,7 +2606,7 @@
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
       <c r="I11" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>21</v>
@@ -2368,7 +2618,7 @@
         <v>32</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="2" t="s">
@@ -2380,10 +2630,10 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>89</v>
@@ -2421,7 +2671,7 @@
         <v>88</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>88</v>
@@ -2440,7 +2690,7 @@
         <v>21</v>
       </c>
       <c r="K13" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L13" s="11"/>
       <c r="M13" s="11"/>
@@ -2454,13 +2704,13 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D14" s="25">
         <v>1</v>
@@ -2469,8 +2719,12 @@
       <c r="F14" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
+      <c r="G14" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>197</v>
+      </c>
       <c r="I14" s="5"/>
       <c r="J14" s="6" t="s">
         <v>21</v>
@@ -2490,13 +2744,13 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>47</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D15" s="25">
         <v>2</v>
@@ -2505,8 +2759,12 @@
       <c r="F15" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
+      <c r="G15" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>198</v>
+      </c>
       <c r="I15" s="5"/>
       <c r="J15" s="6" t="s">
         <v>21</v>
@@ -2526,7 +2784,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>68</v>
+        <v>164</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>48</v>
@@ -2541,8 +2799,12 @@
       <c r="F16" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
+      <c r="G16" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>199</v>
+      </c>
       <c r="I16" s="5"/>
       <c r="J16" s="6" t="s">
         <v>21</v>
@@ -2562,13 +2824,13 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>49</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D17" s="25">
         <v>4</v>
@@ -2577,8 +2839,12 @@
       <c r="F17" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
+      <c r="G17" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>200</v>
+      </c>
       <c r="I17" s="5"/>
       <c r="J17" s="6" t="s">
         <v>21</v>
@@ -2598,13 +2864,13 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D18" s="25">
         <v>5</v>
@@ -2613,8 +2879,12 @@
       <c r="F18" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
+      <c r="G18" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="I18" s="5"/>
       <c r="J18" s="6" t="s">
         <v>21</v>
@@ -2634,7 +2904,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>69</v>
+        <v>167</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>50</v>
@@ -2649,8 +2919,12 @@
       <c r="F19" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
+      <c r="G19" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>204</v>
+      </c>
       <c r="I19" s="5"/>
       <c r="J19" s="6" t="s">
         <v>21</v>
@@ -2670,7 +2944,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>70</v>
+        <v>168</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>51</v>
@@ -2685,8 +2959,12 @@
       <c r="F20" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
+      <c r="G20" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="I20" s="5"/>
       <c r="J20" s="6" t="s">
         <v>21</v>
@@ -2706,13 +2984,13 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>52</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D21" s="25">
         <v>8</v>
@@ -2721,8 +2999,12 @@
       <c r="F21" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
+      <c r="G21" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>206</v>
+      </c>
       <c r="I21" s="5"/>
       <c r="J21" s="6" t="s">
         <v>21</v>
@@ -2742,7 +3024,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>71</v>
+        <v>170</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>53</v>
@@ -2757,8 +3039,12 @@
       <c r="F22" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
+      <c r="G22" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>207</v>
+      </c>
       <c r="I22" s="5"/>
       <c r="J22" s="6" t="s">
         <v>21</v>
@@ -2778,7 +3064,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>72</v>
+        <v>171</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>54</v>
@@ -2794,10 +3080,10 @@
         <v>87</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>99</v>
+        <v>207</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>100</v>
+        <v>207</v>
       </c>
       <c r="I23" s="5"/>
       <c r="J23" s="6" t="s">
@@ -2818,7 +3104,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>73</v>
+        <v>172</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>55</v>
@@ -2833,8 +3119,12 @@
       <c r="F24" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
+      <c r="G24" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="I24" s="5"/>
       <c r="J24" s="6" t="s">
         <v>21</v>
@@ -2854,13 +3144,13 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D25" s="25">
         <v>12</v>
@@ -2869,8 +3159,12 @@
       <c r="F25" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
+      <c r="G25" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>217</v>
+      </c>
       <c r="I25" s="5"/>
       <c r="J25" s="6" t="s">
         <v>21</v>
@@ -2890,13 +3184,13 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>57</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D26" s="25">
         <v>13</v>
@@ -2905,8 +3199,12 @@
       <c r="F26" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
+      <c r="G26" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>160</v>
+      </c>
       <c r="I26" s="5"/>
       <c r="J26" s="6" t="s">
         <v>21</v>
@@ -2926,7 +3224,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>74</v>
+        <v>175</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>58</v>
@@ -2941,8 +3239,12 @@
       <c r="F27" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
+      <c r="G27" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>155</v>
+      </c>
       <c r="I27" s="5"/>
       <c r="J27" s="6" t="s">
         <v>21</v>
@@ -2962,7 +3264,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>84</v>
+        <v>176</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>93</v>
@@ -2977,8 +3279,12 @@
       <c r="F28" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
+      <c r="G28" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>220</v>
+      </c>
       <c r="I28" s="5"/>
       <c r="J28" s="6" t="s">
         <v>21</v>
@@ -2998,7 +3304,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>75</v>
+        <v>177</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>59</v>
@@ -3014,10 +3320,10 @@
         <v>87</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I29" s="5"/>
       <c r="J29" s="6" t="s">
@@ -3038,13 +3344,13 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>123</v>
+        <v>178</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>60</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D30" s="25">
         <v>17</v>
@@ -3053,8 +3359,12 @@
       <c r="F30" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
+      <c r="G30" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>100</v>
+      </c>
       <c r="I30" s="5"/>
       <c r="J30" s="6" t="s">
         <v>21</v>
@@ -3074,23 +3384,27 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>124</v>
+        <v>179</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>61</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D31" s="25">
         <v>18</v>
       </c>
       <c r="E31" s="25"/>
       <c r="F31" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>227</v>
+      </c>
       <c r="I31" s="5"/>
       <c r="J31" s="6" t="s">
         <v>21</v>
@@ -3110,13 +3424,13 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>125</v>
+        <v>180</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>62</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D32" s="25">
         <v>19</v>
@@ -3125,8 +3439,12 @@
       <c r="F32" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
+      <c r="G32" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>153</v>
+      </c>
       <c r="I32" s="5"/>
       <c r="J32" s="6" t="s">
         <v>21</v>
@@ -3146,23 +3464,27 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>126</v>
+        <v>181</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>63</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D33" s="25">
         <v>20</v>
       </c>
       <c r="E33" s="25"/>
       <c r="F33" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>157</v>
+      </c>
       <c r="I33" s="5"/>
       <c r="J33" s="6" t="s">
         <v>21</v>
@@ -3176,13 +3498,13 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>127</v>
+        <v>182</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D34" s="25">
         <v>21</v>
@@ -3191,8 +3513,12 @@
       <c r="F34" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
+      <c r="G34" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>158</v>
+      </c>
       <c r="I34" s="5"/>
       <c r="J34" s="6" t="s">
         <v>21</v>
@@ -3206,23 +3532,27 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>128</v>
+        <v>183</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D35" s="25">
         <v>22</v>
       </c>
       <c r="E35" s="25"/>
       <c r="F35" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>219</v>
+      </c>
       <c r="I35" s="5"/>
       <c r="J35" s="6" t="s">
         <v>21</v>
@@ -3236,23 +3566,27 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>129</v>
+        <v>184</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D36" s="25">
         <v>23</v>
       </c>
       <c r="E36" s="25"/>
       <c r="F36" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="I36" s="5"/>
       <c r="J36" s="6" t="s">
         <v>21</v>
@@ -3266,23 +3600,27 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>130</v>
+        <v>185</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D37" s="25">
         <v>24</v>
       </c>
       <c r="E37" s="25"/>
       <c r="F37" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>200</v>
+      </c>
       <c r="I37" s="5"/>
       <c r="J37" s="6" t="s">
         <v>21</v>
@@ -3296,23 +3634,27 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>131</v>
+        <v>186</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D38" s="25">
         <v>25</v>
       </c>
       <c r="E38" s="25"/>
       <c r="F38" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="I38" s="5"/>
       <c r="J38" s="6" t="s">
         <v>21</v>
@@ -3326,23 +3668,27 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>132</v>
+        <v>187</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D39" s="25">
         <v>26</v>
       </c>
       <c r="E39" s="25"/>
       <c r="F39" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>214</v>
+      </c>
       <c r="I39" s="5"/>
       <c r="J39" s="6" t="s">
         <v>21</v>
@@ -3356,23 +3702,27 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>133</v>
+        <v>188</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D40" s="25">
         <v>27</v>
       </c>
       <c r="E40" s="25"/>
       <c r="F40" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>212</v>
+      </c>
       <c r="I40" s="5"/>
       <c r="J40" s="6" t="s">
         <v>21</v>
@@ -3386,20 +3736,20 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>134</v>
+        <v>189</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D41" s="25">
         <v>28</v>
       </c>
       <c r="E41" s="25"/>
       <c r="F41" s="20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
@@ -3416,23 +3766,27 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>135</v>
+        <v>190</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D42" s="25">
         <v>29</v>
       </c>
       <c r="E42" s="25"/>
       <c r="F42" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>223</v>
+      </c>
       <c r="I42" s="5"/>
       <c r="J42" s="6" t="s">
         <v>21</v>
@@ -3446,23 +3800,27 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>136</v>
+        <v>191</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D43" s="25">
         <v>30</v>
       </c>
       <c r="E43" s="25"/>
       <c r="F43" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>217</v>
+      </c>
       <c r="I43" s="5"/>
       <c r="J43" s="6" t="s">
         <v>21</v>
@@ -3476,23 +3834,27 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>137</v>
+        <v>192</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D44" s="25">
         <v>31</v>
       </c>
       <c r="E44" s="25"/>
       <c r="F44" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>210</v>
+      </c>
       <c r="I44" s="5"/>
       <c r="J44" s="6" t="s">
         <v>21</v>
@@ -3506,23 +3868,27 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>138</v>
+        <v>193</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D45" s="25">
         <v>32</v>
       </c>
       <c r="E45" s="25"/>
       <c r="F45" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="I45" s="5"/>
       <c r="J45" s="6" t="s">
         <v>21</v>
@@ -3536,23 +3902,27 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>139</v>
+        <v>194</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D46" s="25">
         <v>33</v>
       </c>
       <c r="E46" s="25"/>
       <c r="F46" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>214</v>
+      </c>
       <c r="I46" s="5"/>
       <c r="J46" s="6" t="s">
         <v>21</v>
@@ -3566,23 +3936,27 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>140</v>
+        <v>195</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D47" s="25">
         <v>34</v>
       </c>
       <c r="E47" s="25"/>
       <c r="F47" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>197</v>
+      </c>
       <c r="I47" s="5"/>
       <c r="J47" s="6" t="s">
         <v>21</v>
@@ -3596,23 +3970,27 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>141</v>
+        <v>196</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D48" s="25">
         <v>35</v>
       </c>
       <c r="E48" s="25"/>
       <c r="F48" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="I48" s="5"/>
       <c r="J48" s="6" t="s">
         <v>21</v>
@@ -3623,6 +4001,19 @@
       <c r="L48" s="6"/>
       <c r="M48" s="6"/>
       <c r="N48" s="6"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="G49" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>230</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:P1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Updated side data - flanks
</commit_message>
<xml_diff>
--- a/tabular/eve/ehbv-refseqs-side-data.xlsx
+++ b/tabular/eve/ehbv-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anna/Projects/virus/Hepadnaviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F2EE41-A75A-0541-B4E7-13D713EA0B89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA88E20E-F7B2-9340-94C9-A7E7768240B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="460" windowWidth="25060" windowHeight="16420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="235">
   <si>
     <t>host_sci_name</t>
   </si>
@@ -729,6 +729,18 @@
   </si>
   <si>
     <t>ENSACUG00000013925</t>
+  </si>
+  <si>
+    <t>LCP1</t>
+  </si>
+  <si>
+    <t>RUBCNL</t>
+  </si>
+  <si>
+    <t>NTF3</t>
+  </si>
+  <si>
+    <t>KCNA5</t>
   </si>
 </sst>
 </file>
@@ -2138,7 +2150,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G51" sqref="G51"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2559,8 +2571,12 @@
       <c r="F10" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
+      <c r="G10" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>232</v>
+      </c>
       <c r="I10" s="5" t="s">
         <v>148</v>
       </c>
@@ -2603,8 +2619,12 @@
       <c r="F11" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
+      <c r="G11" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>234</v>
+      </c>
       <c r="I11" s="5" t="s">
         <v>148</v>
       </c>

</xml_diff>

<commit_message>
Merging refseq table from ag_1 into master
</commit_message>
<xml_diff>
--- a/tabular/eve/ehbv-refseqs-side-data.xlsx
+++ b/tabular/eve/ehbv-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anna/Projects/virus/Hepadnaviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F2EE41-A75A-0541-B4E7-13D713EA0B89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA88E20E-F7B2-9340-94C9-A7E7768240B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="460" windowWidth="25060" windowHeight="16420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="235">
   <si>
     <t>host_sci_name</t>
   </si>
@@ -729,6 +729,18 @@
   </si>
   <si>
     <t>ENSACUG00000013925</t>
+  </si>
+  <si>
+    <t>LCP1</t>
+  </si>
+  <si>
+    <t>RUBCNL</t>
+  </si>
+  <si>
+    <t>NTF3</t>
+  </si>
+  <si>
+    <t>KCNA5</t>
   </si>
 </sst>
 </file>
@@ -2138,7 +2150,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G51" sqref="G51"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2559,8 +2571,12 @@
       <c r="F10" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
+      <c r="G10" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>232</v>
+      </c>
       <c r="I10" s="5" t="s">
         <v>148</v>
       </c>
@@ -2603,8 +2619,12 @@
       <c r="F11" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
+      <c r="G11" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>234</v>
+      </c>
       <c r="I11" s="5" t="s">
         <v>148</v>
       </c>

</xml_diff>

<commit_message>
updated flanking genes for some eveseseses
</commit_message>
<xml_diff>
--- a/tabular/eve/ehbv-refseqs-side-data.xlsx
+++ b/tabular/eve/ehbv-refseqs-side-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10510"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anna/Projects/virus/Hepadnaviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA88E20E-F7B2-9340-94C9-A7E7768240B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533AD928-AAD3-0F41-84EB-30055194B462}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="460" windowWidth="25060" windowHeight="16420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="560" yWindow="460" windowWidth="24160" windowHeight="16420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="237">
   <si>
     <t>host_sci_name</t>
   </si>
@@ -632,9 +632,6 @@
     <t>FRY (intronic)</t>
   </si>
   <si>
-    <t>DHX32 (intronic)</t>
-  </si>
-  <si>
     <t>SCN3B (intronic)</t>
   </si>
   <si>
@@ -656,9 +653,6 @@
     <t>SNORA13</t>
   </si>
   <si>
-    <t>MAST3 (intronic)</t>
-  </si>
-  <si>
     <t>Get from paper</t>
   </si>
   <si>
@@ -741,6 +735,18 @@
   </si>
   <si>
     <t>KCNA5</t>
+  </si>
+  <si>
+    <t>ENSTGUG00000004184 (intronic)</t>
+  </si>
+  <si>
+    <t>MGST1</t>
+  </si>
+  <si>
+    <t>LIG3</t>
+  </si>
+  <si>
+    <t>ATP2B2 (intronic)</t>
   </si>
 </sst>
 </file>
@@ -2149,19 +2155,19 @@
   <dimension ref="A1:P49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.5" style="2" customWidth="1"/>
+    <col min="1" max="1" width="28.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="16.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="29.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" style="7" customWidth="1"/>
     <col min="5" max="5" width="10.5" style="7" customWidth="1"/>
-    <col min="6" max="6" width="11.5" style="7" customWidth="1"/>
-    <col min="7" max="7" width="40" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9" style="7" customWidth="1"/>
+    <col min="7" max="7" width="27.6640625" style="2" customWidth="1"/>
     <col min="8" max="8" width="22.83203125" style="2" customWidth="1"/>
     <col min="9" max="9" width="27.6640625" style="2" customWidth="1"/>
     <col min="10" max="10" width="25" style="2" customWidth="1"/>
@@ -2572,10 +2578,10 @@
         <v>149</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>148</v>
@@ -2620,10 +2626,10 @@
         <v>87</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>148</v>
@@ -2780,10 +2786,10 @@
         <v>87</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="6" t="s">
@@ -2820,10 +2826,10 @@
         <v>87</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="6" t="s">
@@ -2860,10 +2866,10 @@
         <v>87</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>200</v>
+        <v>233</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>200</v>
+        <v>233</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="6" t="s">
@@ -2900,10 +2906,10 @@
         <v>87</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>202</v>
+        <v>234</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="6" t="s">
@@ -2940,10 +2946,10 @@
         <v>87</v>
       </c>
       <c r="G19" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="H19" s="5" t="s">
         <v>203</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>204</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="6" t="s">
@@ -2980,10 +2986,10 @@
         <v>87</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>202</v>
+        <v>235</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="6" t="s">
@@ -3020,10 +3026,10 @@
         <v>87</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>206</v>
+        <v>236</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>206</v>
+        <v>236</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="6" t="s">
@@ -3060,10 +3066,10 @@
         <v>87</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="6" t="s">
@@ -3100,10 +3106,10 @@
         <v>87</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I23" s="5"/>
       <c r="J23" s="6" t="s">
@@ -3180,10 +3186,10 @@
         <v>87</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="6" t="s">
@@ -3300,10 +3306,10 @@
         <v>87</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="I28" s="5"/>
       <c r="J28" s="6" t="s">
@@ -3420,10 +3426,10 @@
         <v>105</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I31" s="5"/>
       <c r="J31" s="6" t="s">
@@ -3568,10 +3574,10 @@
         <v>105</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="I35" s="5"/>
       <c r="J35" s="6" t="s">
@@ -3602,10 +3608,10 @@
         <v>105</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I36" s="5"/>
       <c r="J36" s="6" t="s">
@@ -3636,10 +3642,10 @@
         <v>105</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I37" s="5"/>
       <c r="J37" s="6" t="s">
@@ -3670,10 +3676,10 @@
         <v>105</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I38" s="5"/>
       <c r="J38" s="6" t="s">
@@ -3704,10 +3710,10 @@
         <v>105</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I39" s="5"/>
       <c r="J39" s="6" t="s">
@@ -3738,10 +3744,10 @@
         <v>105</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I40" s="5"/>
       <c r="J40" s="6" t="s">
@@ -3802,10 +3808,10 @@
         <v>105</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I42" s="5"/>
       <c r="J42" s="6" t="s">
@@ -3836,10 +3842,10 @@
         <v>105</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I43" s="5"/>
       <c r="J43" s="6" t="s">
@@ -3870,10 +3876,10 @@
         <v>105</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="I44" s="5"/>
       <c r="J44" s="6" t="s">
@@ -3904,10 +3910,10 @@
         <v>105</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I45" s="5"/>
       <c r="J45" s="6" t="s">
@@ -3938,10 +3944,10 @@
         <v>105</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I46" s="5"/>
       <c r="J46" s="6" t="s">
@@ -4006,10 +4012,10 @@
         <v>105</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I48" s="5"/>
       <c r="J48" s="6" t="s">
@@ -4024,15 +4030,15 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
       <c r="G49" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reviewed data for reference/consensus sequences
</commit_message>
<xml_diff>
--- a/tabular/eve/ehbv-refseqs-side-data.xlsx
+++ b/tabular/eve/ehbv-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D82A44-BE8C-9D40-9EF9-7E8516FF898D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E7D3AF-4BAB-FA4B-B001-15DAEAB5A847}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17340" yWindow="760" windowWidth="30800" windowHeight="26680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="200">
   <si>
     <t>Herpetohepadnavirus</t>
   </si>
@@ -627,6 +627,15 @@
   </si>
   <si>
     <t>ehbv-herpeto.4-crocodilia</t>
+  </si>
+  <si>
+    <t>NK</t>
+  </si>
+  <si>
+    <t>KLF8</t>
+  </si>
+  <si>
+    <t>ENSACUG00000005807</t>
   </si>
 </sst>
 </file>
@@ -2064,8 +2073,12 @@
       <c r="D3" s="11">
         <v>3</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
+      <c r="E3" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>197</v>
+      </c>
       <c r="G3" s="4" t="s">
         <v>11</v>
       </c>
@@ -2089,8 +2102,12 @@
       <c r="D4" s="11">
         <v>4</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
+      <c r="E4" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>197</v>
+      </c>
       <c r="G4" s="4" t="s">
         <v>11</v>
       </c>
@@ -2114,8 +2131,12 @@
       <c r="D5" s="11">
         <v>5</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
+      <c r="E5" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>197</v>
+      </c>
       <c r="G5" s="4" t="s">
         <v>11</v>
       </c>
@@ -2168,8 +2189,12 @@
       <c r="D7" s="12">
         <v>1</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
+      <c r="E7" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>199</v>
+      </c>
       <c r="G7" s="3" t="s">
         <v>11</v>
       </c>
@@ -2193,8 +2218,12 @@
       <c r="D8" s="12">
         <v>2</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
+      <c r="E8" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>197</v>
+      </c>
       <c r="G8" s="3" t="s">
         <v>11</v>
       </c>
@@ -2218,8 +2247,12 @@
       <c r="D9" s="12">
         <v>3</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
+      <c r="E9" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>197</v>
+      </c>
       <c r="G9" s="3" t="s">
         <v>11</v>
       </c>
@@ -3084,8 +3117,12 @@
       <c r="D39" s="13">
         <v>28</v>
       </c>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
+      <c r="E39" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>197</v>
+      </c>
       <c r="G39" s="5" t="s">
         <v>11</v>
       </c>
@@ -3254,8 +3291,12 @@
       <c r="D45" s="11">
         <v>2</v>
       </c>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
+      <c r="E45" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>197</v>
+      </c>
       <c r="G45" s="4" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Refactoring for paper-final build of EVE trees
</commit_message>
<xml_diff>
--- a/tabular/eve/ehbv-refseqs-side-data.xlsx
+++ b/tabular/eve/ehbv-refseqs-side-data.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D5D417-A7AD-CE4A-A66F-A8F74CDA9783}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDABF616-8241-7342-BB95-135527234AB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14280" yWindow="1220" windowWidth="27920" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10860" yWindow="3680" windowWidth="27920" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="224">
   <si>
     <t>Herpetohepadnavirus</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Tyto</t>
   </si>
   <si>
-    <t>Anser</t>
-  </si>
-  <si>
     <t>Paleognathae</t>
   </si>
   <si>
@@ -552,9 +549,6 @@
     <t>ehbv-avi.29-psittacula</t>
   </si>
   <si>
-    <t>ehbv-avi.30-anser-con</t>
-  </si>
-  <si>
     <t>ehbv-avi.31-passeriformes-con</t>
   </si>
   <si>
@@ -700,6 +694,21 @@
   </si>
   <si>
     <t>CYB5A</t>
+  </si>
+  <si>
+    <t>ehbv-avi.30-anseridae-con</t>
+  </si>
+  <si>
+    <t>Anseridae</t>
+  </si>
+  <si>
+    <t>ehbv-herpeto.8-serpentes-con</t>
+  </si>
+  <si>
+    <t>Endogenous herpetohepadnavirus 7</t>
+  </si>
+  <si>
+    <t>Endogenous herpetohepadnavirus 8</t>
   </si>
 </sst>
 </file>
@@ -2054,23 +2063,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E43" sqref="A1:I47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37" style="2" customWidth="1"/>
-    <col min="2" max="2" width="45.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="42.83203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="27.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="22.83203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="25" style="2" customWidth="1"/>
-    <col min="8" max="8" width="23.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="42.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="22.83203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="25" style="2" customWidth="1"/>
     <col min="9" max="9" width="32.5" style="2" customWidth="1"/>
     <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
@@ -2080,54 +2089,54 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>177</v>
+      <c r="B2" s="7" t="s">
+        <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="11">
-        <v>1</v>
-      </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="11">
+        <v>1</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>0</v>
+      <c r="H2" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>6</v>
@@ -2135,28 +2144,28 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="E3" s="11">
         <v>2</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>192</v>
-      </c>
       <c r="F3" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>0</v>
+        <v>190</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>6</v>
@@ -2164,405 +2173,405 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="11">
+        <v>3</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="11">
-        <v>3</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>0</v>
+      <c r="G4" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>175</v>
+        <v>189</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="D5" s="11">
+        <v>173</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E5" s="11">
         <v>4</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>192</v>
-      </c>
       <c r="F5" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>0</v>
+        <v>190</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>25</v>
+      <c r="B6" s="7" t="s">
+        <v>0</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="11">
+      <c r="E6" s="11">
         <v>5</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>192</v>
-      </c>
       <c r="F6" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>0</v>
+        <v>190</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>26</v>
+      <c r="B7" s="7" t="s">
+        <v>0</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="11">
+      <c r="E7" s="11">
         <v>6</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>102</v>
-      </c>
       <c r="F7" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D8" s="12">
-        <v>1</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="8" t="s">
+      <c r="C8" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="E8" s="11">
         <v>7</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>153</v>
+      <c r="F8" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="12">
-        <v>2</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>23</v>
+      <c r="A9" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="E9" s="11">
+        <v>8</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>66</v>
+        <v>156</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="12">
-        <v>3</v>
-      </c>
-      <c r="E10" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E10" s="12">
+        <v>1</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="G10" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="F10" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>7</v>
+      <c r="H10" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>9</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="12">
-        <v>4</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>145</v>
+        <v>27</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="12">
+        <v>2</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>7</v>
+        <v>190</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>188</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" s="12">
+        <v>65</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="12">
+        <v>3</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="12">
+        <v>4</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="12">
         <v>5</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="F14" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="G14" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="F12" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D13" s="13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D14" s="13">
-        <v>2</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>180</v>
+      <c r="H14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>31</v>
+        <v>155</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="13">
-        <v>3</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>115</v>
+        <v>28</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="13">
+        <v>1</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>1</v>
+        <v>113</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>16</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>32</v>
+        <v>95</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D16" s="13">
-        <v>4</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>149</v>
+        <v>29</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" s="13">
+        <v>2</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>1</v>
+        <v>123</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>16</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>72</v>
+        <v>47</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D17" s="13">
-        <v>5</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>117</v>
+        <v>30</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="13">
+        <v>3</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>1</v>
+        <v>114</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>16</v>
@@ -2570,28 +2579,28 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>33</v>
+        <v>96</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="13">
-        <v>6</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>119</v>
+        <v>31</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" s="13">
+        <v>4</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>1</v>
+        <v>148</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>16</v>
@@ -2599,28 +2608,28 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>34</v>
+        <v>193</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="13">
-        <v>7</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>121</v>
+        <v>71</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" s="13">
+        <v>5</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>1</v>
+        <v>116</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>16</v>
@@ -2628,579 +2637,579 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>35</v>
+        <v>48</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D20" s="13">
-        <v>8</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>152</v>
+        <v>32</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="13">
+        <v>6</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>1</v>
+        <v>118</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>181</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>36</v>
+        <v>49</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="13">
-        <v>9</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>1</v>
+        <v>33</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="13">
+        <v>7</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>37</v>
+        <v>97</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="13">
-        <v>10</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>1</v>
+        <v>34</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E22" s="13">
+        <v>8</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>8</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>38</v>
+        <v>50</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="13">
-        <v>11</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>1</v>
+        <v>35</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="13">
+        <v>9</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>39</v>
+        <v>51</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D24" s="13">
-        <v>12</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>1</v>
+        <v>36</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" s="13">
+        <v>10</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>182</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>40</v>
+        <v>52</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D25" s="13">
-        <v>13</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>113</v>
+        <v>37</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="13">
+        <v>11</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>1</v>
+        <v>102</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>41</v>
+        <v>157</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="13">
-        <v>14</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>106</v>
+        <v>38</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26" s="13">
+        <v>12</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>1</v>
+        <v>134</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>20</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>65</v>
+        <v>158</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="13">
-        <v>15</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>134</v>
+        <v>39</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E27" s="13">
+        <v>13</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>1</v>
+        <v>112</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>42</v>
+        <v>53</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="D28" s="13">
-        <v>16</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>143</v>
+        <v>40</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="13">
+        <v>14</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>1</v>
+        <v>105</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>142</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>43</v>
+        <v>58</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D29" s="13">
-        <v>17</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>70</v>
+        <v>64</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E29" s="13">
+        <v>15</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>1</v>
+        <v>133</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>44</v>
+        <v>154</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D30" s="13">
-        <v>18</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>140</v>
+        <v>41</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E30" s="13">
+        <v>16</v>
       </c>
       <c r="F30" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" s="5" t="s">
         <v>141</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>45</v>
+        <v>159</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D31" s="13">
-        <v>19</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>104</v>
+        <v>42</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E31" s="13">
+        <v>17</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>1</v>
+        <v>69</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>218</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>46</v>
+        <v>160</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D32" s="13">
-        <v>20</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>108</v>
+        <v>43</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E32" s="13">
+        <v>18</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>1</v>
+        <v>139</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>73</v>
+        <v>161</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D33" s="13">
-        <v>21</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>111</v>
+        <v>44</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E33" s="13">
+        <v>19</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>1</v>
+        <v>103</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>19</v>
+        <v>216</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>74</v>
+        <v>162</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D34" s="13">
-        <v>22</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>132</v>
+        <v>45</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E34" s="13">
+        <v>20</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>1</v>
+        <v>107</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>17</v>
+        <v>217</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>75</v>
+        <v>163</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="D35" s="13">
-        <v>23</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>123</v>
+        <v>72</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E35" s="13">
+        <v>21</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>1</v>
+        <v>110</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>184</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>76</v>
+        <v>164</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D36" s="13">
-        <v>24</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>116</v>
+        <v>73</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E36" s="13">
+        <v>22</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>1</v>
+        <v>131</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>183</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>77</v>
+        <v>209</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D37" s="13">
-        <v>25</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>138</v>
+        <v>74</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E37" s="13">
+        <v>23</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>1</v>
+        <v>122</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>78</v>
+        <v>165</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="D38" s="13">
-        <v>26</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>128</v>
+        <v>75</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E38" s="13">
+        <v>24</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>1</v>
+        <v>115</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>79</v>
+        <v>166</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="D39" s="13">
-        <v>27</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>126</v>
+        <v>76</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E39" s="13">
+        <v>25</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H39" s="9" t="s">
-        <v>1</v>
+        <v>137</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>185</v>
@@ -3208,241 +3217,298 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>80</v>
+        <v>167</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="D40" s="13">
-        <v>28</v>
-      </c>
-      <c r="E40" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="F40" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H40" s="9" t="s">
-        <v>1</v>
+        <v>77</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E40" s="13">
+        <v>26</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>210</v>
+        <v>182</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>81</v>
+        <v>168</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="D41" s="13">
-        <v>29</v>
-      </c>
-      <c r="E41" s="13" t="s">
-        <v>136</v>
+        <v>78</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E41" s="13">
+        <v>27</v>
       </c>
       <c r="F41" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H41" s="9" t="s">
-        <v>1</v>
+        <v>125</v>
+      </c>
+      <c r="G41" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>82</v>
+        <v>207</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="D42" s="13">
-        <v>30</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="F42" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H42" s="9" t="s">
-        <v>1</v>
+        <v>79</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="E42" s="13">
+        <v>28</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="G42" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>18</v>
+        <v>208</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>83</v>
+        <v>169</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="D43" s="13">
-        <v>31</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>124</v>
+        <v>80</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E43" s="13">
+        <v>29</v>
       </c>
       <c r="F43" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H43" s="9" t="s">
-        <v>1</v>
+        <v>135</v>
+      </c>
+      <c r="G43" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>16</v>
+        <v>184</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>84</v>
+        <v>219</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="D44" s="13">
-        <v>32</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>123</v>
+        <v>81</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="E44" s="13">
+        <v>30</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H44" s="9" t="s">
-        <v>1</v>
+        <v>129</v>
+      </c>
+      <c r="G44" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>214</v>
+        <v>170</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="D45" s="13">
-        <v>34</v>
-      </c>
-      <c r="E45" s="13" t="s">
-        <v>70</v>
+        <v>82</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E45" s="13">
+        <v>31</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H45" s="9" t="s">
-        <v>1</v>
+        <v>123</v>
+      </c>
+      <c r="G45" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>215</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>200</v>
+        <v>171</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>1</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="D46" s="13">
-        <v>36</v>
-      </c>
-      <c r="E46" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="F46" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H46" s="9" t="s">
-        <v>1</v>
+        <v>83</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E46" s="13">
+        <v>32</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G46" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E47" s="13">
+        <v>34</v>
+      </c>
+      <c r="F47" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G47" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="E48" s="13">
+        <v>36</v>
+      </c>
+      <c r="F48" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="G48" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="D49" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="E49" s="13">
+        <v>37</v>
+      </c>
+      <c r="F49" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="G49" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I49" s="5" t="s">
         <v>201</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="D47" s="13">
-        <v>37</v>
-      </c>
-      <c r="E47" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="F47" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H47" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I47" s="5" t="s">
-        <v>203</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I12">
-    <sortCondition ref="H2:H12"/>
-    <sortCondition ref="D2:D12"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I14">
+    <sortCondition ref="E2:E14"/>
   </sortState>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3476,13 +3542,13 @@
         <v>4</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>10</v>
@@ -3491,27 +3557,27 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D2" s="13">
         <v>33</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>11</v>
@@ -3520,28 +3586,28 @@
         <v>1</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D3" s="13">
         <v>33</v>
       </c>
       <c r="E3" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="F3" s="13" t="s">
-        <v>129</v>
-      </c>
       <c r="G3" s="5" t="s">
         <v>11</v>
       </c>
@@ -3549,7 +3615,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added final Avihepadna EVE set
</commit_message>
<xml_diff>
--- a/tabular/eve/ehbv-refseqs-side-data.xlsx
+++ b/tabular/eve/ehbv-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F034FD3B-73DF-674B-8957-44AB13A31628}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EDE6E9-9DED-EA49-BA61-3535DEAAEB5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="460" windowWidth="22960" windowHeight="16680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="283">
   <si>
     <t>Herpetohepadnavirus</t>
   </si>
@@ -760,6 +760,132 @@
   </si>
   <si>
     <t>avi-1-rhinobird</t>
+  </si>
+  <si>
+    <t>ehbv-avi.38-passeriformes</t>
+  </si>
+  <si>
+    <t>ehbv-avi.39-ara</t>
+  </si>
+  <si>
+    <t>ehbv-avi.40-oxyura</t>
+  </si>
+  <si>
+    <t>ehbv-avi.41-psittaciformes</t>
+  </si>
+  <si>
+    <t>ehbv-avi.42-passeriformes-con</t>
+  </si>
+  <si>
+    <t>ehbv-avi.43-gallirallus</t>
+  </si>
+  <si>
+    <t>ehbv-avi.44-antrostomus</t>
+  </si>
+  <si>
+    <t>ehbv-avi.45-ara</t>
+  </si>
+  <si>
+    <t>ehbv-avi.46-psittaciformes</t>
+  </si>
+  <si>
+    <t>ehbv-avi.47-passer</t>
+  </si>
+  <si>
+    <t>FXN</t>
+  </si>
+  <si>
+    <t>ENSACOG00000002782</t>
+  </si>
+  <si>
+    <t>ENSACOG00000002891</t>
+  </si>
+  <si>
+    <t>RAD23B</t>
+  </si>
+  <si>
+    <t>PHAX/MARCHF3</t>
+  </si>
+  <si>
+    <t>ABRACL/REPS1</t>
+  </si>
+  <si>
+    <t>TXLNB</t>
+  </si>
+  <si>
+    <t>ENSMUNG00000008889</t>
+  </si>
+  <si>
+    <t>KCNV1</t>
+  </si>
+  <si>
+    <t>ENSTGUG00000027711</t>
+  </si>
+  <si>
+    <t>LNPEP</t>
+  </si>
+  <si>
+    <t>ENSACOG00000006853</t>
+  </si>
+  <si>
+    <t>RYR3</t>
+  </si>
+  <si>
+    <t>FMN1</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 35</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 38</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 39</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 41</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 42</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 43</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 44</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 45</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 46</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 47</t>
+  </si>
+  <si>
+    <t>ehbv-avi.35-calypte</t>
+  </si>
+  <si>
+    <t>passeriformes</t>
+  </si>
+  <si>
+    <t>ara</t>
+  </si>
+  <si>
+    <t>oxyura</t>
+  </si>
+  <si>
+    <t>psittaciformes</t>
+  </si>
+  <si>
+    <t>gallirallus</t>
+  </si>
+  <si>
+    <t>antrostomus</t>
+  </si>
+  <si>
+    <t>passer</t>
   </si>
 </sst>
 </file>
@@ -2141,11 +2267,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="83" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K37" sqref="K37"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="83" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -3791,10 +3917,10 @@
         <v>34</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>69</v>
+        <v>124</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>217</v>
+        <v>117</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>11</v>
@@ -3810,73 +3936,458 @@
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>196</v>
+      <c r="A48" s="2" t="s">
+        <v>275</v>
       </c>
       <c r="B48" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>198</v>
+        <v>265</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>196</v>
+        <v>275</v>
       </c>
       <c r="E48" s="13">
-        <v>36</v>
-      </c>
-      <c r="F48" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="G48" s="15" t="s">
-        <v>210</v>
+        <v>35</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G48" s="13" t="s">
+        <v>217</v>
       </c>
       <c r="H48" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
       <c r="J48" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="K48" s="15" t="s">
-        <v>238</v>
+      <c r="K48" s="6" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="E49" s="13">
+        <v>36</v>
+      </c>
+      <c r="F49" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="G49" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="J49" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="K49" s="15" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="B49" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C49" s="5" t="s">
+      <c r="B50" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D50" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="E49" s="13">
+      <c r="E50" s="13">
         <v>37</v>
       </c>
-      <c r="F49" s="13" t="s">
+      <c r="F50" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="G49" s="13" t="s">
+      <c r="G50" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="H49" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I49" s="5" t="s">
+      <c r="H50" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I50" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="J49" s="16" t="s">
-        <v>226</v>
-      </c>
-      <c r="K49" s="18" t="s">
+      <c r="J50" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="K50" s="18" t="s">
         <v>236</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="E51" s="13">
+        <v>38</v>
+      </c>
+      <c r="F51" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="G51" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="J51" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="K51" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="E52" s="13">
+        <v>39</v>
+      </c>
+      <c r="F52" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="G52" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="J52" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="K52" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="E53" s="13">
+        <v>40</v>
+      </c>
+      <c r="F53" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="G53" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I53" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="J53" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="K53" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="E54" s="13">
+        <v>41</v>
+      </c>
+      <c r="F54" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="G54" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="J54" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="K54" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E55" s="13">
+        <v>42</v>
+      </c>
+      <c r="F55" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="G55" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="J55" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="K55" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="E56" s="13">
+        <v>43</v>
+      </c>
+      <c r="F56" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="G56" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I56" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="J56" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="K56" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="E57" s="13">
+        <v>44</v>
+      </c>
+      <c r="F57" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="G57" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I57" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="J57" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="K57" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="E58" s="13">
+        <v>45</v>
+      </c>
+      <c r="F58" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="G58" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I58" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="J58" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="K58" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="E59" s="13">
+        <v>46</v>
+      </c>
+      <c r="F59" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="G59" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I59" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="J59" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="K59" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="E60" s="13">
+        <v>47</v>
+      </c>
+      <c r="F60" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="G60" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I60" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="J60" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="K60" s="6" t="s">
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final avian eHBVs added
</commit_message>
<xml_diff>
--- a/tabular/eve/ehbv-refseqs-side-data.xlsx
+++ b/tabular/eve/ehbv-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EDE6E9-9DED-EA49-BA61-3535DEAAEB5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A274E5D-891B-1440-92F7-78AAB6F50EEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="460" windowWidth="22960" windowHeight="16680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="292">
   <si>
     <t>Herpetohepadnavirus</t>
   </si>
@@ -660,12 +660,6 @@
     <t>ENSTGUG00000027480</t>
   </si>
   <si>
-    <t>ehbv-avi.28-falco</t>
-  </si>
-  <si>
-    <t>Falco</t>
-  </si>
-  <si>
     <t>ehbv-avi.23-psittaciformes</t>
   </si>
   <si>
@@ -886,6 +880,39 @@
   </si>
   <si>
     <t>passer</t>
+  </si>
+  <si>
+    <t>ehbv-avi.48-podiceps</t>
+  </si>
+  <si>
+    <t>ehbv-avi.50-anas_zonorhyncha</t>
+  </si>
+  <si>
+    <t>ehbv-avi.52-melopsittacus</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 48</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 49</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 50</t>
+  </si>
+  <si>
+    <t>ehbv-avi.28-alauda</t>
+  </si>
+  <si>
+    <t>Aauda</t>
+  </si>
+  <si>
+    <t>podiceps</t>
+  </si>
+  <si>
+    <t>anas</t>
+  </si>
+  <si>
+    <t>melopsittacus</t>
   </si>
 </sst>
 </file>
@@ -960,7 +987,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1021,6 +1048,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAB82FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1458,7 +1491,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1496,6 +1529,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1930,8 +1966,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <mruColors>
+      <color rgb="FFAB82FF"/>
       <color rgb="FFFFAFFF"/>
-      <color rgb="FFAB82FF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2267,11 +2303,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K60"/>
+  <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="83" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="83" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I19" sqref="A1:K63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2319,10 +2355,10 @@
         <v>57</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2354,10 +2390,10 @@
         <v>6</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2389,10 +2425,10 @@
         <v>6</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2424,10 +2460,10 @@
         <v>20</v>
       </c>
       <c r="J4" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="K4" s="11" t="s">
         <v>226</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2459,10 +2495,10 @@
         <v>20</v>
       </c>
       <c r="J5" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="K5" s="11" t="s">
         <v>226</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2494,10 +2530,10 @@
         <v>21</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -2529,24 +2565,24 @@
         <v>22</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E8" s="11">
         <v>8</v>
@@ -2564,24 +2600,24 @@
         <v>6</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E9" s="11">
         <v>9</v>
@@ -2599,10 +2635,10 @@
         <v>6</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2634,10 +2670,10 @@
         <v>152</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -2669,10 +2705,10 @@
         <v>22</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -2704,10 +2740,10 @@
         <v>9</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2739,10 +2775,10 @@
         <v>186</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -2774,10 +2810,10 @@
         <v>186</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -2809,10 +2845,10 @@
         <v>177</v>
       </c>
       <c r="J15" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -2844,10 +2880,10 @@
         <v>178</v>
       </c>
       <c r="J16" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2879,10 +2915,10 @@
         <v>16</v>
       </c>
       <c r="J17" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -2914,10 +2950,10 @@
         <v>16</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -2949,10 +2985,10 @@
         <v>16</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -2984,10 +3020,10 @@
         <v>16</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -3019,10 +3055,10 @@
         <v>16</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K21" s="12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -3054,10 +3090,10 @@
         <v>179</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K22" s="12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -3089,10 +3125,10 @@
         <v>8</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K23" s="13" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -3124,10 +3160,10 @@
         <v>8</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K24" s="13" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -3159,10 +3195,10 @@
         <v>17</v>
       </c>
       <c r="J25" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K25" s="13" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -3194,10 +3230,10 @@
         <v>180</v>
       </c>
       <c r="J26" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K26" s="16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -3229,10 +3265,10 @@
         <v>18</v>
       </c>
       <c r="J27" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K27" s="16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -3264,10 +3300,10 @@
         <v>19</v>
       </c>
       <c r="J28" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K28" s="13" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -3299,10 +3335,10 @@
         <v>19</v>
       </c>
       <c r="J29" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K29" s="13" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -3334,10 +3370,10 @@
         <v>141</v>
       </c>
       <c r="J30" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K30" s="16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -3369,10 +3405,10 @@
         <v>16</v>
       </c>
       <c r="J31" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K31" s="16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -3401,13 +3437,13 @@
         <v>11</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J32" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K32" s="16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -3436,13 +3472,13 @@
         <v>11</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="J33" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K33" s="13" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -3471,13 +3507,13 @@
         <v>11</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J34" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K34" s="17" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -3509,10 +3545,10 @@
         <v>18</v>
       </c>
       <c r="J35" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K35" s="16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -3544,15 +3580,15 @@
         <v>17</v>
       </c>
       <c r="J36" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K36" s="14" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>1</v>
@@ -3561,7 +3597,7 @@
         <v>74</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E37" s="13">
         <v>23</v>
@@ -3579,10 +3615,10 @@
         <v>182</v>
       </c>
       <c r="J37" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K37" s="14" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -3614,10 +3650,10 @@
         <v>181</v>
       </c>
       <c r="J38" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K38" s="17" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -3649,10 +3685,10 @@
         <v>185</v>
       </c>
       <c r="J39" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K39" s="17" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -3684,7 +3720,7 @@
         <v>182</v>
       </c>
       <c r="J40" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K40" s="6" t="s">
         <v>190</v>
@@ -3719,15 +3755,15 @@
         <v>183</v>
       </c>
       <c r="J41" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K41" s="16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>207</v>
+        <v>287</v>
       </c>
       <c r="B42" s="9" t="s">
         <v>1</v>
@@ -3736,7 +3772,7 @@
         <v>79</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>207</v>
+        <v>287</v>
       </c>
       <c r="E42" s="13">
         <v>28</v>
@@ -3751,13 +3787,13 @@
         <v>11</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>208</v>
+        <v>288</v>
       </c>
       <c r="J42" s="16" t="s">
-        <v>226</v>
-      </c>
-      <c r="K42" s="16" t="s">
-        <v>227</v>
+        <v>224</v>
+      </c>
+      <c r="K42" s="6" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -3789,15 +3825,15 @@
         <v>184</v>
       </c>
       <c r="J43" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K43" s="15" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>1</v>
@@ -3806,7 +3842,7 @@
         <v>81</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E44" s="13">
         <v>30</v>
@@ -3821,13 +3857,13 @@
         <v>11</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J44" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K44" s="16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -3859,10 +3895,10 @@
         <v>16</v>
       </c>
       <c r="J45" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K45" s="18" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -3891,27 +3927,27 @@
         <v>11</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J46" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K46" s="16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B47" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E47" s="13">
         <v>34</v>
@@ -3926,27 +3962,27 @@
         <v>11</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J47" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K47" s="16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>275</v>
+      <c r="A48" s="5" t="s">
+        <v>273</v>
       </c>
       <c r="B48" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E48" s="13">
         <v>35</v>
@@ -3955,16 +3991,16 @@
         <v>69</v>
       </c>
       <c r="G48" s="13" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H48" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J48" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K48" s="6" t="s">
         <v>190</v>
@@ -3987,10 +4023,10 @@
         <v>36</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G49" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H49" s="5" t="s">
         <v>11</v>
@@ -3999,10 +4035,10 @@
         <v>200</v>
       </c>
       <c r="J49" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K49" s="15" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -4034,24 +4070,24 @@
         <v>201</v>
       </c>
       <c r="J50" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K50" s="18" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>241</v>
+      <c r="A51" s="5" t="s">
+        <v>239</v>
       </c>
       <c r="B51" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E51" s="13">
         <v>38</v>
@@ -4066,53 +4102,53 @@
         <v>11</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="J51" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K51" s="6" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>242</v>
+      <c r="A52" s="5" t="s">
+        <v>240</v>
       </c>
       <c r="B52" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E52" s="13">
         <v>39</v>
       </c>
       <c r="F52" s="13" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G52" s="13" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H52" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="J52" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K52" s="6" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>243</v>
+      <c r="A53" s="5" t="s">
+        <v>241</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>1</v>
@@ -4121,77 +4157,77 @@
         <v>194</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E53" s="13">
         <v>40</v>
       </c>
-      <c r="F53" s="13" t="s">
-        <v>252</v>
-      </c>
-      <c r="G53" s="13" t="s">
-        <v>253</v>
+      <c r="F53" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="G53" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="J53" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K53" s="6" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>244</v>
+      <c r="A54" s="5" t="s">
+        <v>242</v>
       </c>
       <c r="B54" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E54" s="13">
         <v>41</v>
       </c>
       <c r="F54" s="13" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G54" s="13" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H54" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="J54" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K54" s="6" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>245</v>
+      <c r="A55" s="5" t="s">
+        <v>243</v>
       </c>
       <c r="B55" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E55" s="13">
         <v>42</v>
@@ -4206,27 +4242,27 @@
         <v>11</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="J55" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K55" s="6" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>246</v>
+      <c r="A56" s="5" t="s">
+        <v>244</v>
       </c>
       <c r="B56" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E56" s="13">
         <v>43</v>
@@ -4235,39 +4271,39 @@
         <v>256</v>
       </c>
       <c r="G56" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H56" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J56" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K56" s="6" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>247</v>
+      <c r="A57" s="5" t="s">
+        <v>245</v>
       </c>
       <c r="B57" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E57" s="13">
         <v>44</v>
       </c>
       <c r="F57" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G57" s="13" t="s">
         <v>258</v>
@@ -4276,27 +4312,27 @@
         <v>11</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="J57" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K57" s="6" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>248</v>
+      <c r="A58" s="5" t="s">
+        <v>246</v>
       </c>
       <c r="B58" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E58" s="13">
         <v>45</v>
@@ -4311,27 +4347,27 @@
         <v>11</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="J58" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K58" s="6" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>249</v>
+      <c r="A59" s="5" t="s">
+        <v>247</v>
       </c>
       <c r="B59" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E59" s="13">
         <v>46</v>
@@ -4346,47 +4382,152 @@
         <v>11</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="J59" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K59" s="6" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>250</v>
+      <c r="A60" s="5" t="s">
+        <v>248</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E60" s="13">
         <v>47</v>
       </c>
-      <c r="F60" s="13" t="s">
-        <v>263</v>
-      </c>
-      <c r="G60" s="13" t="s">
-        <v>264</v>
+      <c r="F60" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="G60" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="H60" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I60" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="J60" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="K60" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="E61" s="13">
+        <v>48</v>
+      </c>
+      <c r="F61" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="G61" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I61" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="J61" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="K61" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="J60" s="16" t="s">
-        <v>226</v>
-      </c>
-      <c r="K60" s="6" t="s">
+      <c r="B62" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="E62" s="13">
+        <v>50</v>
+      </c>
+      <c r="F62" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="G62" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I62" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="J62" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="K62" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="E63" s="13">
+        <v>52</v>
+      </c>
+      <c r="F63" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="G63" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="J63" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="K63" s="6" t="s">
         <v>190</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactoring - adding last sequences
</commit_message>
<xml_diff>
--- a/tabular/eve/ehbv-refseqs-side-data.xlsx
+++ b/tabular/eve/ehbv-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A274E5D-891B-1440-92F7-78AAB6F50EEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690ADCDE-78A4-8D41-968B-C6DA75F59821}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="460" windowWidth="22960" windowHeight="16680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="300">
   <si>
     <t>Herpetohepadnavirus</t>
   </si>
@@ -84,9 +84,6 @@
     <t>ehbv-herpeto.5-testudines-con</t>
   </si>
   <si>
-    <t>ehbv-herpeto.6-varanus-con</t>
-  </si>
-  <si>
     <t>Passeriformes</t>
   </si>
   <si>
@@ -913,6 +910,33 @@
   </si>
   <si>
     <t>melopsittacus</t>
+  </si>
+  <si>
+    <t>ehbv-avi.49-leptosomus</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 52</t>
+  </si>
+  <si>
+    <t>leptosomus</t>
+  </si>
+  <si>
+    <t>ehbv-herpeto.7-emydocephalus</t>
+  </si>
+  <si>
+    <t>Endogenous herpetohepadnavirus 7</t>
+  </si>
+  <si>
+    <t>emydocephalus</t>
+  </si>
+  <si>
+    <t>ehbv-avi.51-psittaciformes-con</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 51</t>
+  </si>
+  <si>
+    <t>ehbv-herpeto.6-varanus</t>
   </si>
 </sst>
 </file>
@@ -2303,11 +2327,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K63"/>
+  <dimension ref="A1:K66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="83" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I19" sqref="A1:K63"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="A1:K66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2340,25 +2364,25 @@
         <v>4</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J1" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2369,7 +2393,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>12</v>
@@ -2378,10 +2402,10 @@
         <v>1</v>
       </c>
       <c r="F2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>59</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>60</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>11</v>
@@ -2390,33 +2414,33 @@
         <v>6</v>
       </c>
       <c r="J2" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K2" s="11" t="s">
         <v>224</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E3" s="11">
         <v>2</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>11</v>
@@ -2425,21 +2449,21 @@
         <v>6</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>13</v>
@@ -2448,57 +2472,57 @@
         <v>3</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E5" s="11">
         <v>4</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2509,7 +2533,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>14</v>
@@ -2518,115 +2542,115 @@
         <v>5</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J6" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K6" s="11" t="s">
         <v>224</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>15</v>
+        <v>299</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>15</v>
+        <v>299</v>
       </c>
       <c r="E7" s="11">
         <v>6</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>218</v>
+        <v>294</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>219</v>
+        <v>295</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>218</v>
+        <v>294</v>
       </c>
       <c r="E8" s="11">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>6</v>
+        <v>296</v>
       </c>
       <c r="J8" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K8" s="11" t="s">
         <v>224</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E9" s="11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>11</v>
@@ -2635,523 +2659,523 @@
         <v>6</v>
       </c>
       <c r="J9" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K9" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="K9" s="11" t="s">
-        <v>228</v>
-      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="E10" s="12">
-        <v>1</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>152</v>
+      <c r="A10" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="E10" s="11">
+        <v>9</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>229</v>
+        <v>223</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>63</v>
+        <v>155</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>63</v>
+        <v>152</v>
       </c>
       <c r="E11" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>190</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>22</v>
+        <v>151</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E12" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="E13" s="12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>144</v>
+        <v>189</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>145</v>
+        <v>189</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>186</v>
+        <v>9</v>
       </c>
       <c r="J13" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K13" s="12" t="s">
         <v>224</v>
-      </c>
-      <c r="K13" s="12" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="E14" s="12">
+        <v>4</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="12">
         <v>5</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F15" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="G15" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="G14" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="J14" s="16" t="s">
+      <c r="H15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="J15" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K15" s="12" t="s">
         <v>224</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E15" s="13">
-        <v>1</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="J15" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="K15" s="13" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>95</v>
+        <v>154</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E16" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J16" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="K16" s="12" t="s">
-        <v>225</v>
+        <v>223</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>47</v>
+        <v>94</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>47</v>
+        <v>94</v>
       </c>
       <c r="E17" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>16</v>
+        <v>177</v>
       </c>
       <c r="J17" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K17" s="12" t="s">
         <v>224</v>
-      </c>
-      <c r="K17" s="12" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>96</v>
+        <v>46</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>96</v>
+        <v>46</v>
       </c>
       <c r="E18" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>148</v>
+        <v>113</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>148</v>
+        <v>113</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J18" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K18" s="12" t="s">
         <v>224</v>
-      </c>
-      <c r="K18" s="12" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>193</v>
+        <v>95</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E19" s="13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J19" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K19" s="12" t="s">
         <v>224</v>
-      </c>
-      <c r="K19" s="12" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>48</v>
+        <v>192</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>48</v>
+        <v>99</v>
       </c>
       <c r="E20" s="13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>119</v>
+        <v>148</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J20" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K20" s="12" t="s">
         <v>224</v>
-      </c>
-      <c r="K20" s="12" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E21" s="13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>150</v>
+        <v>118</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J21" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K21" s="12" t="s">
         <v>224</v>
-      </c>
-      <c r="K21" s="12" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>97</v>
+        <v>48</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>97</v>
+        <v>48</v>
       </c>
       <c r="E22" s="13">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>179</v>
+        <v>15</v>
       </c>
       <c r="J22" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K22" s="12" t="s">
         <v>224</v>
-      </c>
-      <c r="K22" s="12" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>50</v>
+        <v>96</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>50</v>
+        <v>96</v>
       </c>
       <c r="E23" s="13">
-        <v>9</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>121</v>
+        <v>8</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>8</v>
+        <v>178</v>
       </c>
       <c r="J23" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K23" s="12" t="s">
         <v>224</v>
-      </c>
-      <c r="K23" s="13" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E24" s="13">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>11</v>
@@ -3160,418 +3184,418 @@
         <v>8</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K24" s="13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E25" s="13">
-        <v>11</v>
-      </c>
-      <c r="F25" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>68</v>
+        <v>10</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>120</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="J25" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K25" s="13" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>157</v>
+        <v>51</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>98</v>
+        <v>51</v>
       </c>
       <c r="E26" s="13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>134</v>
+        <v>101</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>130</v>
+        <v>67</v>
       </c>
       <c r="H26" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>180</v>
+        <v>16</v>
       </c>
       <c r="J26" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="K26" s="16" t="s">
-        <v>225</v>
+        <v>223</v>
+      </c>
+      <c r="K26" s="13" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E27" s="13">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>18</v>
+        <v>179</v>
       </c>
       <c r="J27" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K27" s="16" t="s">
         <v>224</v>
-      </c>
-      <c r="K27" s="16" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>53</v>
+        <v>157</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>53</v>
+        <v>98</v>
       </c>
       <c r="E28" s="13">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="H28" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J28" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K28" s="16" t="s">
         <v>224</v>
-      </c>
-      <c r="K28" s="13" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E29" s="13">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
       <c r="G29" s="13" t="s">
-        <v>133</v>
+        <v>105</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J29" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K29" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>154</v>
+        <v>57</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>154</v>
+        <v>57</v>
       </c>
       <c r="E30" s="13">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>141</v>
+        <v>18</v>
       </c>
       <c r="J30" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="K30" s="16" t="s">
-        <v>225</v>
+        <v>223</v>
+      </c>
+      <c r="K30" s="13" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>85</v>
+        <v>153</v>
       </c>
       <c r="E31" s="13">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>70</v>
+        <v>142</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>16</v>
+        <v>140</v>
       </c>
       <c r="J31" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K31" s="16" t="s">
         <v>224</v>
-      </c>
-      <c r="K31" s="16" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E32" s="13">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>139</v>
+        <v>68</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>140</v>
+        <v>69</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>212</v>
+        <v>15</v>
       </c>
       <c r="J32" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K32" s="16" t="s">
         <v>224</v>
-      </c>
-      <c r="K32" s="16" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E33" s="13">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>103</v>
+        <v>138</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>104</v>
+        <v>139</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J33" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K33" s="16" t="s">
         <v>224</v>
-      </c>
-      <c r="K33" s="13" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E34" s="13">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="H34" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J34" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="K34" s="17" t="s">
-        <v>233</v>
+        <v>223</v>
+      </c>
+      <c r="K34" s="13" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E35" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>18</v>
+        <v>213</v>
       </c>
       <c r="J35" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="K35" s="16" t="s">
-        <v>225</v>
+        <v>223</v>
+      </c>
+      <c r="K35" s="17" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E36" s="13">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="H36" s="5" t="s">
         <v>11</v>
@@ -3580,68 +3604,68 @@
         <v>17</v>
       </c>
       <c r="J36" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K36" s="16" t="s">
         <v>224</v>
-      </c>
-      <c r="K36" s="14" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>207</v>
+        <v>163</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>207</v>
+        <v>89</v>
       </c>
       <c r="E37" s="13">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>182</v>
+        <v>16</v>
       </c>
       <c r="J37" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K37" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>165</v>
+        <v>206</v>
       </c>
       <c r="B38" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>91</v>
+        <v>206</v>
       </c>
       <c r="E38" s="13">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>11</v>
@@ -3650,891 +3674,996 @@
         <v>181</v>
       </c>
       <c r="J38" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="K38" s="17" t="s">
-        <v>233</v>
+        <v>223</v>
+      </c>
+      <c r="K38" s="14" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B39" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E39" s="13">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="J39" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K39" s="17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>167</v>
+        <v>92</v>
       </c>
       <c r="E40" s="13">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F40" s="13" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="H40" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="J40" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="K40" s="6" t="s">
-        <v>190</v>
+        <v>223</v>
+      </c>
+      <c r="K40" s="17" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B41" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E41" s="13">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F41" s="13" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="J41" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="K41" s="16" t="s">
-        <v>225</v>
+        <v>223</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>287</v>
+        <v>167</v>
       </c>
       <c r="B42" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>287</v>
+        <v>167</v>
       </c>
       <c r="E42" s="13">
-        <v>28</v>
-      </c>
-      <c r="F42" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="G42" s="14" t="s">
-        <v>190</v>
+        <v>27</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>125</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>288</v>
+        <v>182</v>
       </c>
       <c r="J42" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K42" s="16" t="s">
         <v>224</v>
-      </c>
-      <c r="K42" s="6" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>169</v>
+        <v>286</v>
       </c>
       <c r="B43" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>169</v>
+        <v>286</v>
       </c>
       <c r="E43" s="13">
-        <v>29</v>
-      </c>
-      <c r="F43" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="G43" s="13" t="s">
-        <v>136</v>
+        <v>28</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="G43" s="14" t="s">
+        <v>189</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>184</v>
+        <v>287</v>
       </c>
       <c r="J43" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="K43" s="15" t="s">
-        <v>236</v>
+        <v>223</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
       <c r="E44" s="13">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="G44" s="13" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="H44" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>217</v>
+        <v>183</v>
       </c>
       <c r="J44" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="K44" s="16" t="s">
-        <v>225</v>
+        <v>223</v>
+      </c>
+      <c r="K44" s="15" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>170</v>
+        <v>215</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>170</v>
+        <v>215</v>
       </c>
       <c r="E45" s="13">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>16</v>
+        <v>216</v>
       </c>
       <c r="J45" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K45" s="16" t="s">
         <v>224</v>
-      </c>
-      <c r="K45" s="18" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B46" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E46" s="13">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F46" s="13" t="s">
         <v>122</v>
       </c>
       <c r="G46" s="13" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="H46" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>235</v>
+        <v>15</v>
       </c>
       <c r="J46" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="K46" s="16" t="s">
-        <v>225</v>
+        <v>223</v>
+      </c>
+      <c r="K46" s="18" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>209</v>
+        <v>170</v>
       </c>
       <c r="B47" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>210</v>
+        <v>82</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>209</v>
+        <v>170</v>
       </c>
       <c r="E47" s="13">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="J47" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K47" s="16" t="s">
         <v>224</v>
-      </c>
-      <c r="K47" s="16" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>273</v>
+        <v>208</v>
       </c>
       <c r="B48" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>263</v>
+        <v>209</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>273</v>
+        <v>208</v>
       </c>
       <c r="E48" s="13">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F48" s="13" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
       <c r="G48" s="13" t="s">
-        <v>215</v>
+        <v>116</v>
       </c>
       <c r="H48" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J48" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K48" s="16" t="s">
         <v>224</v>
-      </c>
-      <c r="K48" s="6" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>196</v>
+        <v>272</v>
       </c>
       <c r="B49" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>198</v>
+        <v>262</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>196</v>
+        <v>272</v>
       </c>
       <c r="E49" s="13">
-        <v>36</v>
-      </c>
-      <c r="F49" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="G49" s="15" t="s">
-        <v>208</v>
+        <v>35</v>
+      </c>
+      <c r="F49" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G49" s="13" t="s">
+        <v>214</v>
       </c>
       <c r="H49" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="J49" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="K49" s="15" t="s">
-        <v>236</v>
+        <v>223</v>
+      </c>
+      <c r="K49" s="6" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="B50" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C50" s="5" t="s">
+      <c r="D50" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E50" s="13">
+        <v>36</v>
+      </c>
+      <c r="F50" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="G50" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I50" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="D50" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="E50" s="13">
-        <v>37</v>
-      </c>
-      <c r="F50" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="G50" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="H50" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I50" s="5" t="s">
-        <v>201</v>
-      </c>
       <c r="J50" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="K50" s="18" t="s">
-        <v>234</v>
+        <v>223</v>
+      </c>
+      <c r="K50" s="15" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>239</v>
+        <v>196</v>
       </c>
       <c r="B51" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>264</v>
+        <v>198</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>239</v>
+        <v>196</v>
       </c>
       <c r="E51" s="13">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F51" s="13" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="G51" s="13" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="H51" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>274</v>
+        <v>200</v>
       </c>
       <c r="J51" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="K51" s="6" t="s">
-        <v>190</v>
+        <v>223</v>
+      </c>
+      <c r="K51" s="18" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B52" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E52" s="13">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F52" s="13" t="s">
-        <v>249</v>
+        <v>204</v>
       </c>
       <c r="G52" s="13" t="s">
-        <v>249</v>
+        <v>205</v>
       </c>
       <c r="H52" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J52" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K52" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>194</v>
+        <v>264</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E53" s="13">
-        <v>40</v>
-      </c>
-      <c r="F53" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="G53" s="14" t="s">
-        <v>190</v>
+        <v>39</v>
+      </c>
+      <c r="F53" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="G53" s="13" t="s">
+        <v>248</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="J53" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K53" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B54" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>266</v>
+        <v>193</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E54" s="13">
-        <v>41</v>
-      </c>
-      <c r="F54" s="13" t="s">
-        <v>252</v>
-      </c>
-      <c r="G54" s="13" t="s">
-        <v>253</v>
+        <v>40</v>
+      </c>
+      <c r="F54" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="G54" s="14" t="s">
+        <v>189</v>
       </c>
       <c r="H54" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="J54" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K54" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B55" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E55" s="13">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F55" s="13" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G55" s="13" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="J55" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K55" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B56" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E56" s="13">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F56" s="13" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G56" s="13" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="H56" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="J56" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K56" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B57" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E57" s="13">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F57" s="13" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G57" s="13" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="H57" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="J57" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K57" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B58" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E58" s="13">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F58" s="13" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="G58" s="13" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="H58" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="J58" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K58" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B59" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E59" s="13">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F59" s="13" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G59" s="13" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="H59" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="J59" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K59" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E60" s="13">
-        <v>47</v>
-      </c>
-      <c r="F60" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="G60" s="14" t="s">
-        <v>190</v>
+        <v>46</v>
+      </c>
+      <c r="F60" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="G60" s="13" t="s">
+        <v>261</v>
       </c>
       <c r="H60" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="J60" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K60" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>281</v>
+        <v>247</v>
       </c>
       <c r="B61" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>281</v>
+        <v>247</v>
       </c>
       <c r="E61" s="13">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F61" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G61" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H61" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="J61" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K61" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B62" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E62" s="13">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F62" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G62" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H62" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="J62" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K62" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="B63" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="E63" s="13">
+        <v>49</v>
+      </c>
+      <c r="F63" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="G63" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="J63" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K63" s="6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="E64" s="13">
+        <v>50</v>
+      </c>
+      <c r="F64" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="G64" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I64" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="J64" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K64" s="6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="E65" s="13">
+        <v>51</v>
+      </c>
+      <c r="F65" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="G65" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I65" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="J65" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K65" s="6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="E66" s="13">
         <v>52</v>
       </c>
-      <c r="F63" s="19" t="s">
+      <c r="F66" s="19" t="s">
+        <v>249</v>
+      </c>
+      <c r="G66" s="19" t="s">
         <v>250</v>
       </c>
-      <c r="G63" s="19" t="s">
-        <v>251</v>
-      </c>
-      <c r="H63" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I63" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="J63" s="16" t="s">
-        <v>224</v>
-      </c>
-      <c r="K63" s="6" t="s">
-        <v>190</v>
+      <c r="H66" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I66" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="J66" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K66" s="6" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I14">
-    <sortCondition ref="E2:E14"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I15">
+    <sortCondition ref="E2:E15"/>
   </sortState>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4568,13 +4697,13 @@
         <v>4</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>10</v>
@@ -4583,28 +4712,28 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>194</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>195</v>
       </c>
       <c r="D2" s="13">
         <v>33</v>
       </c>
       <c r="E2" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>206</v>
-      </c>
       <c r="G2" s="5" t="s">
         <v>11</v>
       </c>
@@ -4612,28 +4741,28 @@
         <v>1</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D3" s="13">
         <v>33</v>
       </c>
       <c r="E3" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="F3" s="13" t="s">
-        <v>128</v>
-      </c>
       <c r="G3" s="5" t="s">
         <v>11</v>
       </c>
@@ -4641,7 +4770,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactoring eHBV avihepadnavirus build
</commit_message>
<xml_diff>
--- a/tabular/eve/ehbv-refseqs-side-data.xlsx
+++ b/tabular/eve/ehbv-refseqs-side-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B0A1E0-7F14-FE4A-8163-CB92B8B7CBF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815BAFB2-FF4C-A145-B095-600576A8049D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="460" windowWidth="49380" windowHeight="27380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="880" yWindow="460" windowWidth="27920" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="293">
   <si>
     <t>Herpetohepadnavirus</t>
   </si>
@@ -294,9 +294,6 @@
     <t>ehbv-avi.17-Passeriformes</t>
   </si>
   <si>
-    <t>ehbv-avi.18-Calypte</t>
-  </si>
-  <si>
     <t>ehbv-avi.19-Buceros</t>
   </si>
   <si>
@@ -330,9 +327,6 @@
     <t>ehbv-avi.8-australiaves</t>
   </si>
   <si>
-    <t>ehbv-avi.12-anatidae</t>
-  </si>
-  <si>
     <t>ehbv-avi.13-paleognathea</t>
   </si>
   <si>
@@ -387,9 +381,6 @@
     <t>LMO3</t>
   </si>
   <si>
-    <t>nk</t>
-  </si>
-  <si>
     <t>FOXD3</t>
   </si>
   <si>
@@ -438,9 +429,6 @@
     <t>TMEM182 (intronic)</t>
   </si>
   <si>
-    <t>ENSABRG00000002559</t>
-  </si>
-  <si>
     <t>ENSMUNG00000011927/CHSY3</t>
   </si>
   <si>
@@ -507,9 +495,6 @@
     <t>ehbv-meta.1-sauria-con</t>
   </si>
   <si>
-    <t>ehbv-avi.12-anatidae-con</t>
-  </si>
-  <si>
     <t>ehbv-avi.13-paleognathae-con</t>
   </si>
   <si>
@@ -576,9 +561,6 @@
     <t>Australiaves</t>
   </si>
   <si>
-    <t>Anatidae</t>
-  </si>
-  <si>
     <t>Apaloderma</t>
   </si>
   <si>
@@ -756,9 +738,6 @@
     <t>ehbv-avi.39-ara</t>
   </si>
   <si>
-    <t>ehbv-avi.40-oxyura</t>
-  </si>
-  <si>
     <t>ehbv-avi.41-psittaciformes</t>
   </si>
   <si>
@@ -777,12 +756,6 @@
     <t>ehbv-avi.46-psittaciformes</t>
   </si>
   <si>
-    <t>ehbv-avi.47-passer</t>
-  </si>
-  <si>
-    <t>FXN</t>
-  </si>
-  <si>
     <t>ENSACOG00000002782</t>
   </si>
   <si>
@@ -849,9 +822,6 @@
     <t>Endogenous avihepadnavirus 46</t>
   </si>
   <si>
-    <t>Endogenous avihepadnavirus 47</t>
-  </si>
-  <si>
     <t>ehbv-avi.35-calypte</t>
   </si>
   <si>
@@ -861,9 +831,6 @@
     <t>ara</t>
   </si>
   <si>
-    <t>oxyura</t>
-  </si>
-  <si>
     <t>psittaciformes</t>
   </si>
   <si>
@@ -873,9 +840,6 @@
     <t>antrostomus</t>
   </si>
   <si>
-    <t>passer</t>
-  </si>
-  <si>
     <t>ehbv-avi.48-podiceps</t>
   </si>
   <si>
@@ -928,6 +892,30 @@
   </si>
   <si>
     <t>ehbv-herpeto.7-serpentes-con</t>
+  </si>
+  <si>
+    <t>ehbv-avi.12-anseriformes-con</t>
+  </si>
+  <si>
+    <t>Anseriformes</t>
+  </si>
+  <si>
+    <t>EPHA6</t>
+  </si>
+  <si>
+    <t>NSUN3/ARL13B</t>
+  </si>
+  <si>
+    <t>CCDC58 (intronic)</t>
+  </si>
+  <si>
+    <t>FXN (intronic)</t>
+  </si>
+  <si>
+    <t>ehbv-avi.35-passer</t>
+  </si>
+  <si>
+    <t>Passer</t>
   </si>
 </sst>
 </file>
@@ -2318,11 +2306,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K65"/>
+  <dimension ref="A1:K64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="A1:K65"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D31" sqref="A1:K64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2370,10 +2358,10 @@
         <v>56</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2384,7 +2372,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>12</v>
@@ -2405,33 +2393,33 @@
         <v>6</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E3" s="11">
         <v>2</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>11</v>
@@ -2440,15 +2428,15 @@
         <v>6</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>0</v>
@@ -2463,10 +2451,10 @@
         <v>3</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>11</v>
@@ -2475,33 +2463,33 @@
         <v>19</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E5" s="11">
         <v>4</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>11</v>
@@ -2510,10 +2498,10 @@
         <v>19</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2533,10 +2521,10 @@
         <v>5</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>11</v>
@@ -2545,15 +2533,15 @@
         <v>20</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>0</v>
@@ -2562,16 +2550,16 @@
         <v>24</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="E7" s="11">
         <v>6</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>11</v>
@@ -2580,33 +2568,33 @@
         <v>21</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="E8" s="11">
         <v>9</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>11</v>
@@ -2615,33 +2603,33 @@
         <v>6</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="E9" s="11">
         <v>8</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>11</v>
@@ -2650,15 +2638,15 @@
         <v>6</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>7</v>
@@ -2667,28 +2655,28 @@
         <v>25</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E10" s="12">
         <v>1</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -2708,10 +2696,10 @@
         <v>2</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>11</v>
@@ -2720,10 +2708,10 @@
         <v>21</v>
       </c>
       <c r="J11" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="K11" s="12" t="s">
         <v>222</v>
-      </c>
-      <c r="K11" s="12" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -2743,10 +2731,10 @@
         <v>3</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>11</v>
@@ -2755,10 +2743,10 @@
         <v>9</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2778,22 +2766,22 @@
         <v>4</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -2813,27 +2801,27 @@
         <v>5</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>1</v>
@@ -2842,33 +2830,33 @@
         <v>27</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E15" s="13">
         <v>1</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="J15" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>1</v>
@@ -2877,28 +2865,28 @@
         <v>28</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E16" s="13">
         <v>2</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="J16" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2918,10 +2906,10 @@
         <v>3</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>11</v>
@@ -2930,15 +2918,15 @@
         <v>15</v>
       </c>
       <c r="J17" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>1</v>
@@ -2947,16 +2935,16 @@
         <v>30</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E18" s="13">
         <v>4</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>11</v>
@@ -2965,15 +2953,15 @@
         <v>15</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>1</v>
@@ -2982,16 +2970,16 @@
         <v>70</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E19" s="13">
         <v>5</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>11</v>
@@ -3000,10 +2988,10 @@
         <v>15</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -3023,10 +3011,10 @@
         <v>6</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>11</v>
@@ -3035,10 +3023,10 @@
         <v>15</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -3058,10 +3046,10 @@
         <v>7</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>11</v>
@@ -3070,15 +3058,15 @@
         <v>15</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K21" s="12" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>1</v>
@@ -3087,28 +3075,28 @@
         <v>33</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E22" s="13">
         <v>8</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K22" s="12" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -3128,10 +3116,10 @@
         <v>9</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>11</v>
@@ -3140,10 +3128,10 @@
         <v>8</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K23" s="13" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -3163,10 +3151,10 @@
         <v>10</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>11</v>
@@ -3175,10 +3163,10 @@
         <v>8</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K24" s="13" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -3198,7 +3186,7 @@
         <v>11</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G25" s="13" t="s">
         <v>67</v>
@@ -3210,15 +3198,15 @@
         <v>16</v>
       </c>
       <c r="J25" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K25" s="13" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>156</v>
+        <v>285</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>1</v>
@@ -3227,33 +3215,33 @@
         <v>37</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>97</v>
+        <v>285</v>
       </c>
       <c r="E26" s="13">
         <v>12</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>133</v>
+        <v>289</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>129</v>
+        <v>289</v>
       </c>
       <c r="H26" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>179</v>
+        <v>286</v>
       </c>
       <c r="J26" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K26" s="16" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>1</v>
@@ -3262,16 +3250,16 @@
         <v>38</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E27" s="13">
         <v>13</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>11</v>
@@ -3280,10 +3268,10 @@
         <v>17</v>
       </c>
       <c r="J27" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K27" s="16" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -3303,10 +3291,10 @@
         <v>14</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H28" s="5" t="s">
         <v>11</v>
@@ -3315,10 +3303,10 @@
         <v>18</v>
       </c>
       <c r="J28" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K28" s="13" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -3338,10 +3326,10 @@
         <v>15</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="G29" s="13" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>11</v>
@@ -3350,15 +3338,15 @@
         <v>18</v>
       </c>
       <c r="J29" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K29" s="13" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>1</v>
@@ -3367,33 +3355,33 @@
         <v>40</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E30" s="13">
         <v>16</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J30" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K30" s="16" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>1</v>
@@ -3420,15 +3408,15 @@
         <v>15</v>
       </c>
       <c r="J31" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K31" s="16" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>1</v>
@@ -3437,978 +3425,978 @@
         <v>42</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>85</v>
+        <v>154</v>
       </c>
       <c r="E32" s="13">
         <v>18</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="J32" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K32" s="16" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>160</v>
+        <v>291</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>43</v>
+        <v>252</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>86</v>
+        <v>291</v>
       </c>
       <c r="E33" s="13">
-        <v>19</v>
-      </c>
-      <c r="F33" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="G33" s="13" t="s">
-        <v>103</v>
+        <v>35</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="G33" s="14" t="s">
+        <v>183</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>212</v>
+        <v>292</v>
       </c>
       <c r="J33" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="K33" s="13" t="s">
-        <v>236</v>
+        <v>216</v>
+      </c>
+      <c r="K33" s="18" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E34" s="13">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="H34" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="J34" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="K34" s="17" t="s">
-        <v>231</v>
+        <v>216</v>
+      </c>
+      <c r="K34" s="13" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E35" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>17</v>
+        <v>207</v>
       </c>
       <c r="J35" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="K35" s="16" t="s">
-        <v>223</v>
+        <v>216</v>
+      </c>
+      <c r="K35" s="17" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E36" s="13">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="H36" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J36" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="K36" s="14" t="s">
-        <v>235</v>
+        <v>216</v>
+      </c>
+      <c r="K36" s="16" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>206</v>
+        <v>158</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>206</v>
+        <v>88</v>
       </c>
       <c r="E37" s="13">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>181</v>
+        <v>16</v>
       </c>
       <c r="J37" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K37" s="14" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>164</v>
+        <v>200</v>
       </c>
       <c r="B38" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>90</v>
+        <v>200</v>
       </c>
       <c r="E38" s="13">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="G38" s="13" t="s">
-        <v>114</v>
+        <v>118</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>201</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="J38" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="K38" s="17" t="s">
-        <v>231</v>
+        <v>216</v>
+      </c>
+      <c r="K38" s="14" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B39" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E39" s="13">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="J39" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K39" s="17" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>166</v>
+        <v>91</v>
       </c>
       <c r="E40" s="13">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F40" s="13" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="H40" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="J40" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="K40" s="16" t="s">
-        <v>223</v>
+        <v>216</v>
+      </c>
+      <c r="K40" s="17" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B41" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="E41" s="13">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F41" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="G41" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="G41" s="13" t="s">
-        <v>125</v>
-      </c>
       <c r="H41" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="J41" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K41" s="16" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>285</v>
+        <v>162</v>
       </c>
       <c r="B42" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>285</v>
+        <v>162</v>
       </c>
       <c r="E42" s="13">
-        <v>28</v>
-      </c>
-      <c r="F42" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="G42" s="14" t="s">
-        <v>189</v>
+        <v>27</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>122</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>286</v>
+        <v>176</v>
       </c>
       <c r="J42" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="K42" s="13" t="s">
-        <v>229</v>
+        <v>216</v>
+      </c>
+      <c r="K42" s="16" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>168</v>
+        <v>273</v>
       </c>
       <c r="B43" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>168</v>
+        <v>273</v>
       </c>
       <c r="E43" s="13">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F43" s="13" t="s">
-        <v>134</v>
+        <v>287</v>
       </c>
       <c r="G43" s="13" t="s">
-        <v>135</v>
+        <v>288</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>183</v>
+        <v>274</v>
       </c>
       <c r="J43" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="K43" s="15" t="s">
-        <v>234</v>
+        <v>216</v>
+      </c>
+      <c r="K43" s="13" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>215</v>
+        <v>163</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>215</v>
+        <v>163</v>
       </c>
       <c r="E44" s="13">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G44" s="13" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H44" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>216</v>
+        <v>177</v>
       </c>
       <c r="J44" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="K44" s="16" t="s">
-        <v>223</v>
+        <v>216</v>
+      </c>
+      <c r="K44" s="15" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>169</v>
+        <v>209</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>169</v>
+        <v>209</v>
       </c>
       <c r="E45" s="13">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>15</v>
+        <v>210</v>
       </c>
       <c r="J45" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="K45" s="18" t="s">
-        <v>232</v>
+        <v>216</v>
+      </c>
+      <c r="K45" s="16" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B46" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E46" s="13">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F46" s="13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G46" s="13" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="H46" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>233</v>
+        <v>15</v>
       </c>
       <c r="J46" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="K46" s="16" t="s">
-        <v>223</v>
+        <v>216</v>
+      </c>
+      <c r="K46" s="18" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>208</v>
+        <v>165</v>
       </c>
       <c r="B47" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>209</v>
+        <v>82</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>208</v>
+        <v>165</v>
       </c>
       <c r="E47" s="13">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="G47" s="13" t="s">
-        <v>116</v>
+        <v>118</v>
+      </c>
+      <c r="G47" s="15" t="s">
+        <v>201</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>210</v>
+        <v>227</v>
       </c>
       <c r="J47" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K47" s="16" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>271</v>
+        <v>202</v>
       </c>
       <c r="B48" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>261</v>
+        <v>203</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>271</v>
+        <v>202</v>
       </c>
       <c r="E48" s="13">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F48" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="G48" s="13" t="s">
-        <v>214</v>
+        <v>120</v>
+      </c>
+      <c r="G48" s="15" t="s">
+        <v>201</v>
       </c>
       <c r="H48" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="J48" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K48" s="16" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>195</v>
+        <v>261</v>
       </c>
       <c r="B49" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>197</v>
+        <v>252</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>195</v>
+        <v>261</v>
       </c>
       <c r="E49" s="13">
-        <v>36</v>
-      </c>
-      <c r="F49" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="G49" s="15" t="s">
-        <v>207</v>
+        <v>35</v>
+      </c>
+      <c r="F49" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G49" s="13" t="s">
+        <v>208</v>
       </c>
       <c r="H49" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="J49" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="K49" s="15" t="s">
-        <v>234</v>
+        <v>216</v>
+      </c>
+      <c r="K49" s="16" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="B50" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="E50" s="13">
-        <v>37</v>
-      </c>
-      <c r="F50" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F50" s="15" t="s">
         <v>201</v>
       </c>
-      <c r="G50" s="13" t="s">
-        <v>202</v>
+      <c r="G50" s="15" t="s">
+        <v>201</v>
       </c>
       <c r="H50" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="J50" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="K50" s="18" t="s">
-        <v>232</v>
+        <v>216</v>
+      </c>
+      <c r="K50" s="15" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>237</v>
+        <v>190</v>
       </c>
       <c r="B51" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>262</v>
+        <v>192</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>237</v>
+        <v>190</v>
       </c>
       <c r="E51" s="13">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F51" s="13" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="G51" s="13" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="H51" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>272</v>
+        <v>194</v>
       </c>
       <c r="J51" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="K51" s="16" t="s">
-        <v>223</v>
+        <v>216</v>
+      </c>
+      <c r="K51" s="18" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="B52" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="E52" s="13">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F52" s="13" t="s">
-        <v>247</v>
+        <v>198</v>
       </c>
       <c r="G52" s="13" t="s">
-        <v>247</v>
+        <v>199</v>
       </c>
       <c r="H52" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="J52" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K52" s="16" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>193</v>
+        <v>254</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="E53" s="13">
-        <v>40</v>
-      </c>
-      <c r="F53" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="G53" s="14" t="s">
-        <v>189</v>
+        <v>39</v>
+      </c>
+      <c r="F53" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="G53" s="13" t="s">
+        <v>290</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="J53" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="K53" s="13" t="s">
-        <v>230</v>
+        <v>216</v>
+      </c>
+      <c r="K53" s="16" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="B54" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="E54" s="13">
         <v>41</v>
       </c>
       <c r="F54" s="13" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="G54" s="13" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="H54" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="J54" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K54" s="16" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="B55" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E55" s="13">
         <v>42</v>
       </c>
       <c r="F55" s="13" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="G55" s="13" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="J55" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K55" s="16" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="B56" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E56" s="13">
         <v>43</v>
       </c>
       <c r="F56" s="13" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="G56" s="13" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="H56" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="J56" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K56" s="16" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B57" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="E57" s="13">
         <v>44</v>
       </c>
       <c r="F57" s="13" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="G57" s="13" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="H57" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="J57" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K57" s="16" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B58" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E58" s="13">
         <v>45</v>
       </c>
       <c r="F58" s="13" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="G58" s="13" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="H58" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="J58" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K58" s="16" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="B59" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E59" s="13">
         <v>46</v>
       </c>
       <c r="F59" s="13" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="G59" s="13" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="H59" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="J59" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K59" s="16" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>246</v>
+        <v>267</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>1</v>
@@ -4417,203 +4405,168 @@
         <v>270</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>246</v>
+        <v>267</v>
       </c>
       <c r="E60" s="13">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F60" s="14" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="G60" s="14" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="H60" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="J60" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K60" s="18" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B61" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E61" s="13">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F61" s="14" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="G61" s="14" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="H61" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="J61" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="K61" s="18" t="s">
-        <v>232</v>
+        <v>216</v>
+      </c>
+      <c r="K61" s="15" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>290</v>
+        <v>268</v>
       </c>
       <c r="B62" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>290</v>
+        <v>268</v>
       </c>
       <c r="E62" s="13">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F62" s="14" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="G62" s="14" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="H62" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>292</v>
+        <v>276</v>
       </c>
       <c r="J62" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="K62" s="15" t="s">
-        <v>235</v>
+        <v>216</v>
+      </c>
+      <c r="K62" s="16" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B63" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E63" s="13">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F63" s="14" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="G63" s="14" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="H63" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I63" s="5" t="s">
-        <v>288</v>
+        <v>264</v>
       </c>
       <c r="J63" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K63" s="16" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>293</v>
+        <v>269</v>
       </c>
       <c r="B64" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>293</v>
+        <v>269</v>
       </c>
       <c r="E64" s="13">
-        <v>51</v>
-      </c>
-      <c r="F64" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="G64" s="14" t="s">
-        <v>189</v>
+        <v>52</v>
+      </c>
+      <c r="F64" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="G64" s="19" t="s">
+        <v>240</v>
       </c>
       <c r="H64" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="J64" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="K64" s="16" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="B65" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="E65" s="13">
-        <v>52</v>
-      </c>
-      <c r="F65" s="19" t="s">
-        <v>248</v>
-      </c>
-      <c r="G65" s="19" t="s">
-        <v>249</v>
-      </c>
-      <c r="H65" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I65" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="J65" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="K65" s="16" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -4673,22 +4626,22 @@
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D2" s="13">
         <v>33</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>11</v>
@@ -4697,27 +4650,27 @@
         <v>1</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>83</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D3" s="13">
         <v>33</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>11</v>
@@ -4726,7 +4679,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated DIGS side data
</commit_message>
<xml_diff>
--- a/tabular/eve/ehbv-refseqs-side-data.xlsx
+++ b/tabular/eve/ehbv-refseqs-side-data.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/eve/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2200F6-51E9-3B42-B006-3C2C22CCF056}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF60C7BF-F9BC-2A47-91C5-F3B873A91B09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="460" windowWidth="25080" windowHeight="16500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10500" yWindow="6440" windowWidth="38560" windowHeight="18740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="360">
   <si>
     <t>Herpetohepadnavirus</t>
   </si>
@@ -1089,13 +1089,40 @@
   </si>
   <si>
     <t>avi.5-passeriformes</t>
+  </si>
+  <si>
+    <t>start_codon</t>
+  </si>
+  <si>
+    <t>start gene</t>
+  </si>
+  <si>
+    <t>Core</t>
+  </si>
+  <si>
+    <t>structure</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>fragment</t>
+  </si>
+  <si>
+    <t>amp fragment</t>
+  </si>
+  <si>
+    <t>Pol</t>
+  </si>
+  <si>
+    <t>nd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1162,8 +1189,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1230,6 +1264,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1667,7 +1713,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1708,6 +1754,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2479,11 +2534,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L64"/>
+  <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C44" sqref="A1:L64"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="83" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H26" sqref="H26:I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2492,17 +2547,17 @@
     <col min="3" max="3" width="23.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="45.6640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="42.83203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.83203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="27.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="22.83203125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="25" style="2" customWidth="1"/>
-    <col min="10" max="10" width="32.5" style="2" customWidth="1"/>
-    <col min="11" max="11" width="21.1640625" style="6" customWidth="1"/>
-    <col min="12" max="12" width="33.5" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="2"/>
+    <col min="6" max="9" width="24.83203125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="27.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="22.83203125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="25" style="2" customWidth="1"/>
+    <col min="13" max="13" width="32.5" style="2" customWidth="1"/>
+    <col min="14" max="14" width="21.1640625" style="6" customWidth="1"/>
+    <col min="15" max="15" width="33.5" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>285</v>
       </c>
@@ -2521,26 +2576,35 @@
       <c r="F1" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="10" t="s">
+        <v>354</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>352</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -2559,26 +2623,29 @@
       <c r="F2" s="11">
         <v>1</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="4" t="s">
+      <c r="L2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L2" s="11" t="s">
+      <c r="N2" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O2" s="11" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>164</v>
       </c>
@@ -2597,26 +2664,29 @@
       <c r="F3" s="11">
         <v>2</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="K3" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="4" t="s">
+      <c r="L3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L3" s="11" t="s">
+      <c r="N3" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O3" s="11" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>176</v>
       </c>
@@ -2635,26 +2705,29 @@
       <c r="F4" s="11">
         <v>3</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="K4" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="4" t="s">
+      <c r="L4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L4" s="11" t="s">
+      <c r="N4" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O4" s="11" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>177</v>
       </c>
@@ -2673,26 +2746,29 @@
       <c r="F5" s="11">
         <v>4</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="K5" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="4" t="s">
+      <c r="L5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L5" s="11" t="s">
+      <c r="N5" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O5" s="11" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -2711,26 +2787,29 @@
       <c r="F6" s="11">
         <v>5</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="K6" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="4" t="s">
+      <c r="L6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L6" s="11" t="s">
+      <c r="N6" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O6" s="11" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>274</v>
       </c>
@@ -2749,26 +2828,29 @@
       <c r="F7" s="11">
         <v>6</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="K7" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="4" t="s">
+      <c r="L7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K7" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L7" s="11" t="s">
+      <c r="N7" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O7" s="11" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>275</v>
       </c>
@@ -2787,26 +2869,29 @@
       <c r="F8" s="11">
         <v>9</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="K8" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="4" t="s">
+      <c r="L8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L8" s="11" t="s">
+      <c r="N8" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O8" s="11" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>203</v>
       </c>
@@ -2825,26 +2910,29 @@
       <c r="F9" s="11">
         <v>8</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="K9" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9" s="4" t="s">
+      <c r="L9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K9" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L9" s="11" t="s">
+      <c r="N9" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O9" s="11" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>147</v>
       </c>
@@ -2863,26 +2951,29 @@
       <c r="F10" s="12">
         <v>1</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="K10" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="I10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J10" s="3" t="s">
+      <c r="L10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M10" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="K10" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L10" s="12" t="s">
+      <c r="N10" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O10" s="12" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>60</v>
       </c>
@@ -2901,26 +2992,29 @@
       <c r="F11" s="12">
         <v>2</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="K11" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="I11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J11" s="3" t="s">
+      <c r="L11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K11" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L11" s="12" t="s">
+      <c r="N11" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O11" s="12" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>58</v>
       </c>
@@ -2939,26 +3033,29 @@
       <c r="F12" s="12">
         <v>3</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="K12" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="I12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J12" s="3" t="s">
+      <c r="L12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K12" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L12" s="12" t="s">
+      <c r="N12" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O12" s="12" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>43</v>
       </c>
@@ -2977,26 +3074,29 @@
       <c r="F13" s="12">
         <v>4</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="K13" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="I13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13" s="3" t="s">
+      <c r="L13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M13" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="K13" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L13" s="12" t="s">
+      <c r="N13" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O13" s="12" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>59</v>
       </c>
@@ -3015,26 +3115,29 @@
       <c r="F14" s="12">
         <v>5</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="K14" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="I14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J14" s="3" t="s">
+      <c r="L14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M14" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="K14" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L14" s="12" t="s">
+      <c r="N14" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O14" s="12" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>146</v>
       </c>
@@ -3053,26 +3156,35 @@
       <c r="F15" s="13">
         <v>1</v>
       </c>
-      <c r="G15" s="13" t="s">
+      <c r="G15" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="I15" s="13">
+        <v>1</v>
+      </c>
+      <c r="J15" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="K15" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="I15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J15" s="5" t="s">
+      <c r="L15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M15" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="K15" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L15" s="13" t="s">
+      <c r="N15" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O15" s="13" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>89</v>
       </c>
@@ -3092,25 +3204,34 @@
         <v>2</v>
       </c>
       <c r="G16" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="I16" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="J16" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="K16" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="I16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J16" s="5" t="s">
+      <c r="L16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M16" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="K16" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L16" s="12" t="s">
+      <c r="N16" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O16" s="12" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>44</v>
       </c>
@@ -3130,25 +3251,34 @@
         <v>3</v>
       </c>
       <c r="G17" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="H17" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="I17" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="J17" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="K17" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J17" s="5" t="s">
+      <c r="L17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K17" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L17" s="12" t="s">
+      <c r="N17" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O17" s="12" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>90</v>
       </c>
@@ -3168,25 +3298,34 @@
         <v>4</v>
       </c>
       <c r="G18" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="H18" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="I18" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="J18" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="H18" s="13" t="s">
+      <c r="K18" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="I18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J18" s="5" t="s">
+      <c r="L18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M18" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K18" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L18" s="12" t="s">
+      <c r="N18" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O18" s="12" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>181</v>
       </c>
@@ -3206,25 +3345,34 @@
         <v>5</v>
       </c>
       <c r="G19" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="I19" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="J19" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="H19" s="13" t="s">
+      <c r="K19" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="I19" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J19" s="5" t="s">
+      <c r="L19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K19" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L19" s="12" t="s">
+      <c r="N19" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O19" s="12" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>45</v>
       </c>
@@ -3244,25 +3392,34 @@
         <v>6</v>
       </c>
       <c r="G20" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="I20" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="J20" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="K20" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="I20" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J20" s="5" t="s">
+      <c r="L20" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M20" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K20" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L20" s="12" t="s">
+      <c r="N20" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O20" s="12" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>46</v>
       </c>
@@ -3282,25 +3439,34 @@
         <v>7</v>
       </c>
       <c r="G21" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="H21" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="I21" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="J21" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="H21" s="13" t="s">
+      <c r="K21" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="I21" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J21" s="5" t="s">
+      <c r="L21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M21" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K21" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L21" s="12" t="s">
+      <c r="N21" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O21" s="12" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>91</v>
       </c>
@@ -3320,25 +3486,34 @@
         <v>8</v>
       </c>
       <c r="G22" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="H22" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="I22" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="J22" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="H22" s="13" t="s">
+      <c r="K22" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="I22" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J22" s="5" t="s">
+      <c r="L22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M22" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="K22" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L22" s="12" t="s">
+      <c r="N22" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O22" s="12" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>47</v>
       </c>
@@ -3357,26 +3532,31 @@
       <c r="F23" s="13">
         <v>9</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="G23" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="H23" s="14" t="s">
+      <c r="K23" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="I23" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J23" s="5" t="s">
+      <c r="L23" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M23" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K23" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L23" s="13" t="s">
+      <c r="N23" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O23" s="13" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>48</v>
       </c>
@@ -3395,26 +3575,31 @@
       <c r="F24" s="13">
         <v>10</v>
       </c>
-      <c r="G24" s="14" t="s">
+      <c r="G24" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="H24" s="14" t="s">
+      <c r="K24" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="I24" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J24" s="5" t="s">
+      <c r="L24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M24" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K24" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L24" s="13" t="s">
+      <c r="N24" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O24" s="13" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>49</v>
       </c>
@@ -3433,26 +3618,31 @@
       <c r="F25" s="13">
         <v>11</v>
       </c>
-      <c r="G25" s="13" t="s">
+      <c r="G25" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="H25" s="13" t="s">
+      <c r="K25" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="I25" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J25" s="5" t="s">
+      <c r="L25" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M25" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K25" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L25" s="13" t="s">
+      <c r="N25" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O25" s="13" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>276</v>
       </c>
@@ -3471,26 +3661,35 @@
       <c r="F26" s="13">
         <v>12</v>
       </c>
-      <c r="G26" s="13" t="s">
+      <c r="G26" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="I26" s="13">
+        <v>1</v>
+      </c>
+      <c r="J26" s="13" t="s">
         <v>280</v>
       </c>
-      <c r="H26" s="13" t="s">
+      <c r="K26" s="13" t="s">
         <v>280</v>
       </c>
-      <c r="I26" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J26" s="5" t="s">
+      <c r="L26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M26" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="K26" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L26" s="16" t="s">
+      <c r="N26" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O26" s="16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>148</v>
       </c>
@@ -3510,25 +3709,34 @@
         <v>13</v>
       </c>
       <c r="G27" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="J27" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="H27" s="13" t="s">
+      <c r="K27" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="I27" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J27" s="5" t="s">
+      <c r="L27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M27" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K27" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L27" s="16" t="s">
+      <c r="N27" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O27" s="16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>50</v>
       </c>
@@ -3547,26 +3755,35 @@
       <c r="F28" s="13">
         <v>14</v>
       </c>
-      <c r="G28" s="13" t="s">
+      <c r="G28" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="I28" s="13">
+        <v>1</v>
+      </c>
+      <c r="J28" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="H28" s="13" t="s">
+      <c r="K28" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I28" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J28" s="5" t="s">
+      <c r="L28" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M28" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K28" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L28" s="13" t="s">
+      <c r="N28" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O28" s="13" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>55</v>
       </c>
@@ -3585,26 +3802,35 @@
       <c r="F29" s="13">
         <v>15</v>
       </c>
-      <c r="G29" s="13" t="s">
+      <c r="G29" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="I29" s="13">
+        <v>1</v>
+      </c>
+      <c r="J29" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="H29" s="13" t="s">
+      <c r="K29" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="I29" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J29" s="5" t="s">
+      <c r="L29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M29" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K29" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L29" s="13" t="s">
+      <c r="N29" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O29" s="13" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>145</v>
       </c>
@@ -3624,25 +3850,34 @@
         <v>16</v>
       </c>
       <c r="G30" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="J30" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="H30" s="13" t="s">
+      <c r="K30" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="I30" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J30" s="5" t="s">
+      <c r="L30" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M30" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="K30" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L30" s="16" t="s">
+      <c r="N30" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O30" s="16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>149</v>
       </c>
@@ -3661,26 +3896,31 @@
       <c r="F31" s="13">
         <v>17</v>
       </c>
-      <c r="G31" s="13" t="s">
+      <c r="G31" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="H31" s="13" t="s">
+      <c r="K31" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="I31" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J31" s="5" t="s">
+      <c r="L31" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M31" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K31" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L31" s="16" t="s">
+      <c r="N31" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O31" s="16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>150</v>
       </c>
@@ -3699,26 +3939,31 @@
       <c r="F32" s="13">
         <v>18</v>
       </c>
-      <c r="G32" s="13" t="s">
+      <c r="G32" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="H32" s="13" t="s">
+      <c r="K32" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="I32" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J32" s="5" t="s">
+      <c r="L32" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M32" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="K32" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L32" s="16" t="s">
+      <c r="N32" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O32" s="16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>282</v>
       </c>
@@ -3737,26 +3982,31 @@
       <c r="F33" s="13">
         <v>35</v>
       </c>
-      <c r="G33" s="14" t="s">
+      <c r="G33" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="H33" s="14" t="s">
+      <c r="K33" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="I33" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J33" s="5" t="s">
+      <c r="L33" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M33" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="K33" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L33" s="18" t="s">
+      <c r="N33" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O33" s="18" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>151</v>
       </c>
@@ -3775,26 +4025,31 @@
       <c r="F34" s="13">
         <v>19</v>
       </c>
-      <c r="G34" s="13" t="s">
+      <c r="G34" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="H34" s="13" t="s">
+      <c r="K34" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="I34" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J34" s="5" t="s">
+      <c r="L34" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M34" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="K34" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L34" s="13" t="s">
+      <c r="N34" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O34" s="13" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>152</v>
       </c>
@@ -3813,26 +4068,29 @@
       <c r="F35" s="13">
         <v>20</v>
       </c>
-      <c r="G35" s="13" t="s">
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="H35" s="13" t="s">
+      <c r="K35" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="I35" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J35" s="5" t="s">
+      <c r="L35" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M35" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="K35" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L35" s="17" t="s">
+      <c r="N35" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O35" s="17" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>153</v>
       </c>
@@ -3852,25 +4110,30 @@
         <v>21</v>
       </c>
       <c r="G36" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="H36" s="13" t="s">
+      <c r="K36" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="I36" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J36" s="5" t="s">
+      <c r="L36" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M36" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K36" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L36" s="16" t="s">
+      <c r="N36" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O36" s="16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>154</v>
       </c>
@@ -3889,26 +4152,29 @@
       <c r="F37" s="13">
         <v>22</v>
       </c>
-      <c r="G37" s="13" t="s">
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="H37" s="13" t="s">
+      <c r="K37" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="I37" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J37" s="5" t="s">
+      <c r="L37" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M37" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K37" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L37" s="14" t="s">
+      <c r="N37" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O37" s="14" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>192</v>
       </c>
@@ -3927,26 +4193,29 @@
       <c r="F38" s="13">
         <v>23</v>
       </c>
-      <c r="G38" s="13" t="s">
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="H38" s="15" t="s">
+      <c r="K38" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="I38" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J38" s="5" t="s">
+      <c r="L38" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M38" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="K38" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L38" s="14" t="s">
+      <c r="N38" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O38" s="14" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>155</v>
       </c>
@@ -3965,26 +4234,29 @@
       <c r="F39" s="13">
         <v>24</v>
       </c>
-      <c r="G39" s="13" t="s">
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="H39" s="13" t="s">
+      <c r="K39" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="I39" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J39" s="5" t="s">
+      <c r="L39" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M39" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="K39" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L39" s="17" t="s">
+      <c r="N39" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O39" s="17" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>156</v>
       </c>
@@ -4003,26 +4275,35 @@
       <c r="F40" s="13">
         <v>25</v>
       </c>
-      <c r="G40" s="13" t="s">
+      <c r="G40" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="I40" s="13">
+        <v>523</v>
+      </c>
+      <c r="J40" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="H40" s="13" t="s">
+      <c r="K40" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="I40" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J40" s="5" t="s">
+      <c r="L40" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M40" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="K40" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L40" s="17" t="s">
+      <c r="N40" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O40" s="17" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>157</v>
       </c>
@@ -4041,26 +4322,29 @@
       <c r="F41" s="13">
         <v>26</v>
       </c>
-      <c r="G41" s="13" t="s">
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="H41" s="13" t="s">
+      <c r="K41" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="I41" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J41" s="5" t="s">
+      <c r="L41" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M41" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="K41" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L41" s="16" t="s">
+      <c r="N41" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O41" s="16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>158</v>
       </c>
@@ -4079,26 +4363,31 @@
       <c r="F42" s="13">
         <v>27</v>
       </c>
-      <c r="G42" s="13" t="s">
+      <c r="G42" s="21" t="s">
+        <v>357</v>
+      </c>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="H42" s="13" t="s">
+      <c r="K42" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="I42" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J42" s="5" t="s">
+      <c r="L42" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M42" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="K42" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L42" s="16" t="s">
+      <c r="N42" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O42" s="16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>264</v>
       </c>
@@ -4117,26 +4406,35 @@
       <c r="F43" s="13">
         <v>28</v>
       </c>
-      <c r="G43" s="13" t="s">
+      <c r="G43" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="H43" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="I43" s="13">
+        <v>745</v>
+      </c>
+      <c r="J43" s="13" t="s">
         <v>278</v>
       </c>
-      <c r="H43" s="13" t="s">
+      <c r="K43" s="13" t="s">
         <v>279</v>
       </c>
-      <c r="I43" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J43" s="5" t="s">
+      <c r="L43" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M43" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="K43" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L43" s="13" t="s">
+      <c r="N43" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O43" s="13" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>159</v>
       </c>
@@ -4155,26 +4453,29 @@
       <c r="F44" s="13">
         <v>29</v>
       </c>
-      <c r="G44" s="13" t="s">
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="H44" s="13" t="s">
+      <c r="K44" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="I44" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J44" s="5" t="s">
+      <c r="L44" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M44" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="K44" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L44" s="15" t="s">
+      <c r="N44" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O44" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>201</v>
       </c>
@@ -4193,26 +4494,29 @@
       <c r="F45" s="13">
         <v>30</v>
       </c>
-      <c r="G45" s="13" t="s">
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="H45" s="13" t="s">
+      <c r="K45" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="I45" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J45" s="5" t="s">
+      <c r="L45" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M45" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="K45" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L45" s="16" t="s">
+      <c r="N45" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O45" s="16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>160</v>
       </c>
@@ -4231,26 +4535,31 @@
       <c r="F46" s="13">
         <v>31</v>
       </c>
-      <c r="G46" s="13" t="s">
+      <c r="G46" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="H46" s="13" t="s">
+      <c r="K46" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="I46" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J46" s="5" t="s">
+      <c r="L46" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M46" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K46" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L46" s="18" t="s">
+      <c r="N46" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O46" s="18" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>161</v>
       </c>
@@ -4269,26 +4578,29 @@
       <c r="F47" s="13">
         <v>32</v>
       </c>
-      <c r="G47" s="13" t="s">
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="H47" s="15" t="s">
+      <c r="K47" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="I47" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J47" s="5" t="s">
+      <c r="L47" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M47" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="K47" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L47" s="16" t="s">
+      <c r="N47" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O47" s="16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>194</v>
       </c>
@@ -4308,25 +4620,30 @@
         <v>34</v>
       </c>
       <c r="G48" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="H48" s="15" t="s">
+      <c r="K48" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="I48" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J48" s="5" t="s">
+      <c r="L48" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M48" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="K48" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L48" s="16" t="s">
+      <c r="N48" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O48" s="16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>252</v>
       </c>
@@ -4345,26 +4662,29 @@
       <c r="F49" s="13">
         <v>35</v>
       </c>
-      <c r="G49" s="13" t="s">
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="H49" s="13" t="s">
+      <c r="K49" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="I49" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J49" s="5" t="s">
+      <c r="L49" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M49" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="K49" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L49" s="16" t="s">
+      <c r="N49" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O49" s="16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>182</v>
       </c>
@@ -4383,26 +4703,29 @@
       <c r="F50" s="13">
         <v>36</v>
       </c>
-      <c r="G50" s="15" t="s">
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="H50" s="15" t="s">
+      <c r="K50" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="I50" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J50" s="5" t="s">
+      <c r="L50" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M50" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="K50" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L50" s="15" t="s">
+      <c r="N50" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O50" s="15" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>183</v>
       </c>
@@ -4421,26 +4744,29 @@
       <c r="F51" s="13">
         <v>37</v>
       </c>
-      <c r="G51" s="13" t="s">
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="H51" s="13" t="s">
+      <c r="K51" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="I51" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J51" s="5" t="s">
+      <c r="L51" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M51" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="K51" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L51" s="18" t="s">
+      <c r="N51" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O51" s="18" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>222</v>
       </c>
@@ -4459,26 +4785,29 @@
       <c r="F52" s="13">
         <v>38</v>
       </c>
-      <c r="G52" s="13" t="s">
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="H52" s="13" t="s">
+      <c r="K52" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="I52" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J52" s="5" t="s">
+      <c r="L52" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M52" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="K52" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L52" s="16" t="s">
+      <c r="N52" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O52" s="16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>223</v>
       </c>
@@ -4497,26 +4826,29 @@
       <c r="F53" s="13">
         <v>39</v>
       </c>
-      <c r="G53" s="13" t="s">
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="13"/>
+      <c r="J53" s="13" t="s">
         <v>281</v>
       </c>
-      <c r="H53" s="13" t="s">
+      <c r="K53" s="13" t="s">
         <v>281</v>
       </c>
-      <c r="I53" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J53" s="5" t="s">
+      <c r="L53" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M53" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="K53" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L53" s="16" t="s">
+      <c r="N53" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O53" s="16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>224</v>
       </c>
@@ -4535,26 +4867,29 @@
       <c r="F54" s="13">
         <v>41</v>
       </c>
-      <c r="G54" s="13" t="s">
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="H54" s="13" t="s">
+      <c r="K54" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="I54" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J54" s="5" t="s">
+      <c r="L54" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M54" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="K54" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L54" s="16" t="s">
+      <c r="N54" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O54" s="16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>225</v>
       </c>
@@ -4573,26 +4908,29 @@
       <c r="F55" s="13">
         <v>42</v>
       </c>
-      <c r="G55" s="13" t="s">
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="13" t="s">
         <v>234</v>
       </c>
-      <c r="H55" s="13" t="s">
+      <c r="K55" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="I55" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J55" s="5" t="s">
+      <c r="L55" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M55" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="K55" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L55" s="16" t="s">
+      <c r="N55" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O55" s="16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>226</v>
       </c>
@@ -4611,26 +4949,29 @@
       <c r="F56" s="13">
         <v>43</v>
       </c>
-      <c r="G56" s="13" t="s">
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="H56" s="13" t="s">
+      <c r="K56" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="I56" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J56" s="5" t="s">
+      <c r="L56" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M56" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="K56" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L56" s="16" t="s">
+      <c r="N56" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O56" s="16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>227</v>
       </c>
@@ -4649,26 +4990,29 @@
       <c r="F57" s="13">
         <v>44</v>
       </c>
-      <c r="G57" s="13" t="s">
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="13"/>
+      <c r="J57" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="H57" s="13" t="s">
+      <c r="K57" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="I57" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J57" s="5" t="s">
+      <c r="L57" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M57" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="K57" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L57" s="16" t="s">
+      <c r="N57" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O57" s="16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>228</v>
       </c>
@@ -4688,25 +5032,30 @@
         <v>45</v>
       </c>
       <c r="G58" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="H58" s="13"/>
+      <c r="I58" s="13"/>
+      <c r="J58" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="H58" s="13" t="s">
+      <c r="K58" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="I58" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J58" s="5" t="s">
+      <c r="L58" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M58" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="K58" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L58" s="16" t="s">
+      <c r="N58" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O58" s="16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>229</v>
       </c>
@@ -4725,26 +5074,29 @@
       <c r="F59" s="13">
         <v>46</v>
       </c>
-      <c r="G59" s="13" t="s">
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="H59" s="13" t="s">
+      <c r="K59" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="I59" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J59" s="5" t="s">
+      <c r="L59" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M59" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="K59" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L59" s="16" t="s">
+      <c r="N59" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O59" s="16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>258</v>
       </c>
@@ -4763,26 +5115,31 @@
       <c r="F60" s="13">
         <v>48</v>
       </c>
-      <c r="G60" s="14" t="s">
+      <c r="G60" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="H60" s="13"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="H60" s="14" t="s">
+      <c r="K60" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="I60" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J60" s="5" t="s">
+      <c r="L60" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M60" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="K60" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L60" s="18" t="s">
+      <c r="N60" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O60" s="18" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>269</v>
       </c>
@@ -4801,26 +5158,31 @@
       <c r="F61" s="13">
         <v>49</v>
       </c>
-      <c r="G61" s="14" t="s">
+      <c r="G61" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="H61" s="13"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="H61" s="14" t="s">
+      <c r="K61" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="I61" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J61" s="5" t="s">
+      <c r="L61" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M61" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="K61" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L61" s="15" t="s">
+      <c r="N61" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O61" s="15" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>259</v>
       </c>
@@ -4839,26 +5201,31 @@
       <c r="F62" s="13">
         <v>50</v>
       </c>
-      <c r="G62" s="14" t="s">
+      <c r="G62" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="H62" s="13"/>
+      <c r="I62" s="13"/>
+      <c r="J62" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="H62" s="14" t="s">
+      <c r="K62" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="I62" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J62" s="5" t="s">
+      <c r="L62" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M62" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="K62" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L62" s="16" t="s">
+      <c r="N62" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O62" s="16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>272</v>
       </c>
@@ -4877,26 +5244,31 @@
       <c r="F63" s="13">
         <v>51</v>
       </c>
-      <c r="G63" s="14" t="s">
+      <c r="G63" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="H63" s="13"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="H63" s="14" t="s">
+      <c r="K63" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="I63" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J63" s="5" t="s">
+      <c r="L63" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M63" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="K63" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L63" s="16" t="s">
+      <c r="N63" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O63" s="16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>260</v>
       </c>
@@ -4915,28 +5287,33 @@
       <c r="F64" s="13">
         <v>52</v>
       </c>
-      <c r="G64" s="19" t="s">
+      <c r="G64" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="H64" s="13"/>
+      <c r="I64" s="13"/>
+      <c r="J64" s="19" t="s">
         <v>230</v>
       </c>
-      <c r="H64" s="19" t="s">
+      <c r="K64" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="I64" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J64" s="5" t="s">
+      <c r="L64" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M64" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="K64" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="L64" s="16" t="s">
+      <c r="N64" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="O64" s="16" t="s">
         <v>209</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J14">
+  <autoFilter ref="A1:M1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M14">
     <sortCondition ref="F2:F14"/>
   </sortState>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>

<commit_message>
Include locus references as well as ancestral hepadnavirus genome reconstructions
</commit_message>
<xml_diff>
--- a/tabular/eve/ehbv-refseqs-side-data.xlsx
+++ b/tabular/eve/ehbv-refseqs-side-data.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1429BD-97FE-D248-A399-1A04534AF8D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA56615-EBEA-C145-8C50-567F11801983}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15340" yWindow="460" windowWidth="34200" windowHeight="26840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5560" yWindow="460" windowWidth="34200" windowHeight="26840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="357">
   <si>
     <t>Herpetohepadnavirus</t>
   </si>
@@ -2546,8 +2546,8 @@
   <dimension ref="A1:O62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="A1:O62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2614,690 +2614,690 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="13">
+        <v>1</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="I2" s="13">
+        <v>1</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="13">
+        <v>9</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="I3" s="13">
+        <v>1</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="13">
         <v>10</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>322</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="11">
-        <v>1</v>
-      </c>
-      <c r="G2" s="24" t="s">
+      <c r="G4" s="20" t="s">
         <v>343</v>
       </c>
-      <c r="H2" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>350</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="N2" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="O2" s="11" t="s">
+      <c r="H4" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="I4" s="13">
+        <v>1</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="O4" s="13" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="13">
+        <v>11</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="I5" s="13">
+        <v>1</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="O5" s="13" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="F6" s="13">
+        <v>12</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="I6" s="13">
+        <v>1</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="N6" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="O6" s="16" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>323</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="F3" s="11">
-        <v>2</v>
-      </c>
-      <c r="G3" s="24" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="13">
+        <v>14</v>
+      </c>
+      <c r="G7" s="20" t="s">
         <v>343</v>
       </c>
-      <c r="H3" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>351</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>352</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="N3" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="H7" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="I7" s="13">
+        <v>11</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="O7" s="13" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="13">
+        <v>15</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="I8" s="13">
+        <v>1</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N8" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="O8" s="13" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="F9" s="13">
+        <v>17</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="I9" s="13">
+        <v>1</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N9" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="O9" s="16" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F10" s="13">
+        <v>18</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="I10" s="13">
+        <v>1</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="N10" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="O10" s="16" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" s="13">
+        <v>19</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="I11" s="13">
+        <v>1</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="N11" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="O11" s="13" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" s="13">
         <v>20</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="11">
-        <v>3</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="N4" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="O4" s="11" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="F5" s="11">
-        <v>4</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="O5" s="11" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="11">
-        <v>5</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N6" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="O6" s="11" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="F7" s="11">
-        <v>6</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N7" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="O7" s="11" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="F8" s="11">
-        <v>9</v>
-      </c>
-      <c r="G8" s="24" t="s">
+      <c r="G12" s="20" t="s">
         <v>343</v>
       </c>
-      <c r="H8" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>353</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>354</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="N8" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="O8" s="11" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="F9" s="11">
-        <v>8</v>
-      </c>
-      <c r="G9" s="24" t="s">
+      <c r="H12" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="I12" s="13">
+        <v>1</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="N12" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="O12" s="17" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="F13" s="13">
+        <v>25</v>
+      </c>
+      <c r="G13" s="20" t="s">
         <v>343</v>
       </c>
-      <c r="H9" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>355</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>356</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="N9" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="O9" s="11" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="F10" s="12">
-        <v>1</v>
-      </c>
-      <c r="G10" s="23" t="s">
+      <c r="H13" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="I13" s="13">
+        <v>523</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="N13" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="O13" s="17" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="F14" s="13">
+        <v>28</v>
+      </c>
+      <c r="G14" s="20" t="s">
         <v>343</v>
       </c>
-      <c r="H10" s="12" t="s">
-        <v>341</v>
-      </c>
-      <c r="I10" s="12">
-        <v>1</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="N10" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="O10" s="12" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F11" s="12">
-        <v>2</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>344</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>347</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>347</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="K11" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N11" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="O11" s="12" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="12">
-        <v>3</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>344</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>347</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>347</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="K12" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="N12" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="O12" s="12" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="12">
-        <v>4</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>344</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>347</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>347</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="K13" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="N13" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="O13" s="12" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="12">
-        <v>5</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>344</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>347</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>347</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>170</v>
+      <c r="H14" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="I14" s="13">
+        <v>745</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="N14" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="O14" s="12" t="s">
-        <v>204</v>
+      <c r="O14" s="13" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>328</v>
+        <v>306</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>83</v>
+        <v>154</v>
       </c>
       <c r="F15" s="13">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="G15" s="20" t="s">
         <v>343</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>341</v>
-      </c>
-      <c r="I15" s="13">
-        <v>1</v>
+        <v>347</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>347</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="L15" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="N15" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="O15" s="13" t="s">
-        <v>209</v>
+      <c r="O15" s="15" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>84</v>
+        <v>155</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>285</v>
+        <v>335</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>84</v>
+        <v>155</v>
       </c>
       <c r="F16" s="13">
-        <v>2</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="H16" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="I16" s="22" t="s">
-        <v>347</v>
+        <v>31</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="I16" s="13">
+        <v>1</v>
       </c>
       <c r="J16" s="13" t="s">
         <v>110</v>
@@ -3309,80 +3309,80 @@
         <v>9</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>163</v>
+        <v>13</v>
       </c>
       <c r="N16" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="O16" s="12" t="s">
-        <v>204</v>
+      <c r="O16" s="18" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>44</v>
+        <v>178</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>286</v>
+        <v>310</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>27</v>
+        <v>180</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>44</v>
+        <v>178</v>
       </c>
       <c r="F17" s="13">
-        <v>3</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="H17" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="I17" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="I17" s="13" t="s">
         <v>347</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>102</v>
+        <v>183</v>
       </c>
       <c r="K17" s="13" t="s">
-        <v>102</v>
+        <v>184</v>
       </c>
       <c r="L17" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>13</v>
+        <v>182</v>
       </c>
       <c r="N17" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="O17" s="12" t="s">
-        <v>204</v>
+      <c r="O17" s="18" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F18" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G18" s="13" t="s">
         <v>344</v>
@@ -3394,16 +3394,16 @@
         <v>347</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>134</v>
+        <v>110</v>
       </c>
       <c r="K18" s="13" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="L18" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M18" s="5" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="N18" s="16" t="s">
         <v>203</v>
@@ -3414,22 +3414,22 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>176</v>
+        <v>44</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>338</v>
+        <v>286</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="F19" s="13">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G19" s="13" t="s">
         <v>344</v>
@@ -3441,10 +3441,10 @@
         <v>347</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>135</v>
+        <v>102</v>
       </c>
       <c r="L19" s="5" t="s">
         <v>9</v>
@@ -3461,22 +3461,22 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="F20" s="13">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G20" s="13" t="s">
         <v>344</v>
@@ -3488,10 +3488,10 @@
         <v>347</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>105</v>
+        <v>134</v>
       </c>
       <c r="K20" s="13" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="L20" s="5" t="s">
         <v>9</v>
@@ -3508,22 +3508,22 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>46</v>
+        <v>176</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>289</v>
+        <v>338</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="F21" s="13">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G21" s="13" t="s">
         <v>344</v>
@@ -3535,10 +3535,10 @@
         <v>347</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L21" s="5" t="s">
         <v>9</v>
@@ -3555,22 +3555,22 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="F22" s="13">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G22" s="13" t="s">
         <v>344</v>
@@ -3582,16 +3582,16 @@
         <v>347</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="K22" s="13" t="s">
-        <v>137</v>
+        <v>106</v>
       </c>
       <c r="L22" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>164</v>
+        <v>13</v>
       </c>
       <c r="N22" s="16" t="s">
         <v>203</v>
@@ -3602,184 +3602,184 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F23" s="13">
-        <v>9</v>
-      </c>
-      <c r="G23" s="20" t="s">
-        <v>343</v>
-      </c>
-      <c r="H23" s="13" t="s">
-        <v>341</v>
-      </c>
-      <c r="I23" s="13">
-        <v>1</v>
-      </c>
-      <c r="J23" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="K23" s="14" t="s">
-        <v>108</v>
+        <v>7</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="H23" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="I23" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="J23" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>136</v>
       </c>
       <c r="L23" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="N23" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="O23" s="13" t="s">
-        <v>209</v>
+      <c r="O23" s="12" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="F24" s="13">
-        <v>10</v>
-      </c>
-      <c r="G24" s="20" t="s">
-        <v>343</v>
-      </c>
-      <c r="H24" s="13" t="s">
-        <v>341</v>
-      </c>
-      <c r="I24" s="13">
-        <v>1</v>
-      </c>
-      <c r="J24" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="K24" s="14" t="s">
-        <v>108</v>
+        <v>8</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="H24" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="I24" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="K24" s="13" t="s">
+        <v>137</v>
       </c>
       <c r="L24" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>6</v>
+        <v>164</v>
       </c>
       <c r="N24" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="O24" s="13" t="s">
-        <v>209</v>
+      <c r="O24" s="12" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>49</v>
+        <v>143</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>293</v>
+        <v>330</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>49</v>
+        <v>87</v>
       </c>
       <c r="F25" s="13">
-        <v>11</v>
-      </c>
-      <c r="G25" s="20" t="s">
-        <v>343</v>
-      </c>
-      <c r="H25" s="13" t="s">
-        <v>341</v>
-      </c>
-      <c r="I25" s="13">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="H25" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="I25" s="22" t="s">
+        <v>347</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="K25" s="13" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="L25" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N25" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="O25" s="13" t="s">
-        <v>210</v>
+      <c r="O25" s="16" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>268</v>
+        <v>140</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>329</v>
+        <v>296</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>268</v>
+        <v>140</v>
       </c>
       <c r="F26" s="13">
-        <v>12</v>
-      </c>
-      <c r="G26" s="20" t="s">
-        <v>343</v>
-      </c>
-      <c r="H26" s="13" t="s">
-        <v>341</v>
-      </c>
-      <c r="I26" s="13">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="H26" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="I26" s="22" t="s">
+        <v>347</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>272</v>
+        <v>128</v>
       </c>
       <c r="K26" s="13" t="s">
-        <v>272</v>
+        <v>129</v>
       </c>
       <c r="L26" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M26" s="5" t="s">
-        <v>269</v>
+        <v>127</v>
       </c>
       <c r="N26" s="16" t="s">
         <v>203</v>
@@ -3790,22 +3790,22 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F27" s="13">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G27" s="13" t="s">
         <v>344</v>
@@ -3817,10 +3817,10 @@
         <v>347</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K27" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="L27" s="5" t="s">
         <v>9</v>
@@ -3837,116 +3837,116 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>50</v>
+        <v>149</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>50</v>
+        <v>149</v>
       </c>
       <c r="F28" s="13">
+        <v>22</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="H28" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="I28" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="J28" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="K28" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M28" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G28" s="20" t="s">
-        <v>343</v>
-      </c>
-      <c r="H28" s="13" t="s">
-        <v>341</v>
-      </c>
-      <c r="I28" s="13">
-        <v>11</v>
-      </c>
-      <c r="J28" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="K28" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="L28" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M28" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="N28" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="O28" s="13" t="s">
-        <v>210</v>
+      <c r="O28" s="14" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>55</v>
+        <v>150</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>55</v>
+        <v>150</v>
       </c>
       <c r="F29" s="13">
-        <v>15</v>
-      </c>
-      <c r="G29" s="20" t="s">
-        <v>343</v>
-      </c>
-      <c r="H29" s="13" t="s">
-        <v>341</v>
-      </c>
-      <c r="I29" s="13">
-        <v>1</v>
+        <v>24</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="H29" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="I29" s="22" t="s">
+        <v>347</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="K29" s="13" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="L29" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M29" s="5" t="s">
-        <v>16</v>
+        <v>165</v>
       </c>
       <c r="N29" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="O29" s="13" t="s">
-        <v>210</v>
+      <c r="O29" s="17" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>140</v>
+        <v>196</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>296</v>
+        <v>334</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>140</v>
+        <v>196</v>
       </c>
       <c r="F30" s="13">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="G30" s="13" t="s">
         <v>344</v>
@@ -3958,16 +3958,16 @@
         <v>347</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="K30" s="13" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="L30" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>127</v>
+        <v>197</v>
       </c>
       <c r="N30" s="16" t="s">
         <v>203</v>
@@ -3978,43 +3978,43 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>348</v>
+        <v>156</v>
       </c>
       <c r="F31" s="13">
-        <v>17</v>
-      </c>
-      <c r="G31" s="20" t="s">
-        <v>343</v>
-      </c>
-      <c r="H31" s="13" t="s">
-        <v>341</v>
-      </c>
-      <c r="I31" s="13">
-        <v>1</v>
+        <v>32</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="H31" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="I31" s="22" t="s">
+        <v>347</v>
       </c>
       <c r="J31" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="K31" s="13" t="s">
-        <v>66</v>
+        <v>109</v>
+      </c>
+      <c r="K31" s="15" t="s">
+        <v>188</v>
       </c>
       <c r="L31" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>13</v>
+        <v>213</v>
       </c>
       <c r="N31" s="16" t="s">
         <v>203</v>
@@ -4025,43 +4025,43 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>145</v>
+        <v>189</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>297</v>
+        <v>307</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>40</v>
+        <v>190</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>145</v>
+        <v>189</v>
       </c>
       <c r="F32" s="13">
-        <v>18</v>
-      </c>
-      <c r="G32" s="20" t="s">
-        <v>343</v>
-      </c>
-      <c r="H32" s="13" t="s">
-        <v>341</v>
-      </c>
-      <c r="I32" s="13">
-        <v>1</v>
+        <v>34</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="H32" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="I32" s="22" t="s">
+        <v>347</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="K32" s="13" t="s">
-        <v>126</v>
+        <v>111</v>
+      </c>
+      <c r="K32" s="15" t="s">
+        <v>188</v>
       </c>
       <c r="L32" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N32" s="16" t="s">
         <v>203</v>
@@ -4072,116 +4072,116 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>146</v>
+        <v>247</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>41</v>
+        <v>238</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>80</v>
+        <v>247</v>
       </c>
       <c r="F33" s="13">
-        <v>19</v>
-      </c>
-      <c r="G33" s="20" t="s">
-        <v>343</v>
-      </c>
-      <c r="H33" s="13" t="s">
-        <v>341</v>
-      </c>
-      <c r="I33" s="13">
-        <v>1</v>
+        <v>35</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="H33" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="I33" s="22" t="s">
+        <v>347</v>
       </c>
       <c r="J33" s="13" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="K33" s="13" t="s">
-        <v>92</v>
+        <v>195</v>
       </c>
       <c r="L33" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M33" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N33" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="O33" s="13" t="s">
-        <v>216</v>
+      <c r="O33" s="16" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>147</v>
+        <v>177</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>299</v>
+        <v>309</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>42</v>
+        <v>179</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>81</v>
+        <v>177</v>
       </c>
       <c r="F34" s="13">
-        <v>20</v>
-      </c>
-      <c r="G34" s="20" t="s">
-        <v>343</v>
-      </c>
-      <c r="H34" s="13" t="s">
-        <v>341</v>
-      </c>
-      <c r="I34" s="13">
-        <v>1</v>
-      </c>
-      <c r="J34" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="K34" s="13" t="s">
-        <v>96</v>
+        <v>36</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="H34" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="I34" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="J34" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="K34" s="15" t="s">
+        <v>188</v>
       </c>
       <c r="L34" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M34" s="5" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="N34" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="O34" s="17" t="s">
-        <v>211</v>
+      <c r="O34" s="15" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>148</v>
+        <v>217</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>332</v>
+        <v>311</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>68</v>
+        <v>239</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>82</v>
+        <v>217</v>
       </c>
       <c r="F35" s="13">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="G35" s="13" t="s">
         <v>344</v>
@@ -4193,16 +4193,16 @@
         <v>347</v>
       </c>
       <c r="J35" s="13" t="s">
-        <v>98</v>
+        <v>185</v>
       </c>
       <c r="K35" s="13" t="s">
-        <v>97</v>
+        <v>186</v>
       </c>
       <c r="L35" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>15</v>
+        <v>248</v>
       </c>
       <c r="N35" s="16" t="s">
         <v>203</v>
@@ -4213,22 +4213,22 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>149</v>
+        <v>218</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>300</v>
+        <v>312</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>69</v>
+        <v>240</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>149</v>
+        <v>218</v>
       </c>
       <c r="F36" s="13">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="G36" s="13" t="s">
         <v>344</v>
@@ -4240,45 +4240,45 @@
         <v>347</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>118</v>
+        <v>273</v>
       </c>
       <c r="K36" s="13" t="s">
-        <v>119</v>
+        <v>273</v>
       </c>
       <c r="L36" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>14</v>
+        <v>249</v>
       </c>
       <c r="N36" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="O36" s="14" t="s">
-        <v>215</v>
+      <c r="O36" s="16" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>187</v>
+        <v>219</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>301</v>
+        <v>313</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>70</v>
+        <v>241</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>187</v>
+        <v>219</v>
       </c>
       <c r="F37" s="13">
-        <v>23</v>
-      </c>
-      <c r="G37" s="21" t="s">
-        <v>345</v>
+        <v>41</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>344</v>
       </c>
       <c r="H37" s="22" t="s">
         <v>347</v>
@@ -4287,42 +4287,42 @@
         <v>347</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="K37" s="15" t="s">
-        <v>188</v>
+        <v>227</v>
+      </c>
+      <c r="K37" s="13" t="s">
+        <v>228</v>
       </c>
       <c r="L37" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>166</v>
+        <v>250</v>
       </c>
       <c r="N37" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="O37" s="14" t="s">
-        <v>215</v>
+      <c r="O37" s="16" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>150</v>
+        <v>220</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>302</v>
+        <v>336</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>71</v>
+        <v>242</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>150</v>
+        <v>220</v>
       </c>
       <c r="F38" s="13">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="G38" s="13" t="s">
         <v>344</v>
@@ -4334,92 +4334,92 @@
         <v>347</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>103</v>
+        <v>229</v>
       </c>
       <c r="K38" s="13" t="s">
-        <v>103</v>
+        <v>230</v>
       </c>
       <c r="L38" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M38" s="5" t="s">
-        <v>165</v>
+        <v>248</v>
       </c>
       <c r="N38" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="O38" s="17" t="s">
-        <v>211</v>
+      <c r="O38" s="16" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>151</v>
+        <v>221</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>303</v>
+        <v>314</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>72</v>
+        <v>243</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>349</v>
+        <v>221</v>
       </c>
       <c r="F39" s="13">
-        <v>25</v>
-      </c>
-      <c r="G39" s="20" t="s">
-        <v>343</v>
-      </c>
-      <c r="H39" s="13" t="s">
-        <v>346</v>
-      </c>
-      <c r="I39" s="13">
-        <v>523</v>
+        <v>43</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="H39" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="I39" s="22" t="s">
+        <v>347</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>123</v>
+        <v>231</v>
       </c>
       <c r="K39" s="13" t="s">
-        <v>124</v>
+        <v>231</v>
       </c>
       <c r="L39" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M39" s="5" t="s">
-        <v>169</v>
+        <v>251</v>
       </c>
       <c r="N39" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="O39" s="17" t="s">
-        <v>211</v>
+      <c r="O39" s="16" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>152</v>
+        <v>222</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>304</v>
+        <v>315</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>73</v>
+        <v>244</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>152</v>
+        <v>222</v>
       </c>
       <c r="F40" s="13">
-        <v>26</v>
-      </c>
-      <c r="G40" s="21" t="s">
-        <v>345</v>
+        <v>44</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>344</v>
       </c>
       <c r="H40" s="22" t="s">
         <v>347</v>
@@ -4428,16 +4428,16 @@
         <v>347</v>
       </c>
       <c r="J40" s="13" t="s">
-        <v>114</v>
+        <v>232</v>
       </c>
       <c r="K40" s="13" t="s">
-        <v>115</v>
+        <v>233</v>
       </c>
       <c r="L40" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M40" s="5" t="s">
-        <v>166</v>
+        <v>252</v>
       </c>
       <c r="N40" s="16" t="s">
         <v>203</v>
@@ -4448,25 +4448,25 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>153</v>
+        <v>223</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>333</v>
+        <v>316</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>74</v>
+        <v>245</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>153</v>
+        <v>223</v>
       </c>
       <c r="F41" s="13">
-        <v>27</v>
-      </c>
-      <c r="G41" s="21" t="s">
-        <v>345</v>
+        <v>45</v>
+      </c>
+      <c r="G41" s="13" t="s">
+        <v>344</v>
       </c>
       <c r="H41" s="22" t="s">
         <v>347</v>
@@ -4475,16 +4475,16 @@
         <v>347</v>
       </c>
       <c r="J41" s="13" t="s">
-        <v>112</v>
+        <v>234</v>
       </c>
       <c r="K41" s="13" t="s">
-        <v>113</v>
+        <v>235</v>
       </c>
       <c r="L41" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M41" s="5" t="s">
-        <v>167</v>
+        <v>249</v>
       </c>
       <c r="N41" s="16" t="s">
         <v>203</v>
@@ -4495,72 +4495,72 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>75</v>
+        <v>246</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="F42" s="13">
-        <v>28</v>
-      </c>
-      <c r="G42" s="20" t="s">
-        <v>343</v>
-      </c>
-      <c r="H42" s="13" t="s">
-        <v>346</v>
-      </c>
-      <c r="I42" s="13">
-        <v>745</v>
+        <v>46</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="H42" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="I42" s="22" t="s">
+        <v>347</v>
       </c>
       <c r="J42" s="13" t="s">
-        <v>270</v>
+        <v>236</v>
       </c>
       <c r="K42" s="13" t="s">
-        <v>271</v>
+        <v>237</v>
       </c>
       <c r="L42" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M42" s="5" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="N42" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="O42" s="13" t="s">
-        <v>209</v>
+      <c r="O42" s="16" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>154</v>
+        <v>253</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>306</v>
+        <v>318</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>76</v>
+        <v>256</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>154</v>
+        <v>253</v>
       </c>
       <c r="F43" s="13">
-        <v>29</v>
-      </c>
-      <c r="G43" s="20" t="s">
-        <v>343</v>
+        <v>48</v>
+      </c>
+      <c r="G43" s="13" t="s">
+        <v>344</v>
       </c>
       <c r="H43" s="22" t="s">
         <v>347</v>
@@ -4568,43 +4568,43 @@
       <c r="I43" s="22" t="s">
         <v>347</v>
       </c>
-      <c r="J43" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="K43" s="13" t="s">
-        <v>122</v>
+      <c r="J43" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="K43" s="14" t="s">
+        <v>173</v>
       </c>
       <c r="L43" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M43" s="5" t="s">
-        <v>168</v>
+        <v>260</v>
       </c>
       <c r="N43" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="O43" s="15" t="s">
-        <v>214</v>
+      <c r="O43" s="18" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>196</v>
+        <v>254</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>77</v>
+        <v>257</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>196</v>
+        <v>254</v>
       </c>
       <c r="F44" s="13">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G44" s="13" t="s">
         <v>344</v>
@@ -4615,17 +4615,17 @@
       <c r="I44" s="22" t="s">
         <v>347</v>
       </c>
-      <c r="J44" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="K44" s="13" t="s">
-        <v>117</v>
+      <c r="J44" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="K44" s="14" t="s">
+        <v>173</v>
       </c>
       <c r="L44" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M44" s="5" t="s">
-        <v>197</v>
+        <v>261</v>
       </c>
       <c r="N44" s="16" t="s">
         <v>203</v>
@@ -4636,69 +4636,69 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>155</v>
+        <v>264</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>78</v>
+        <v>265</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>155</v>
+        <v>264</v>
       </c>
       <c r="F45" s="13">
-        <v>31</v>
-      </c>
-      <c r="G45" s="20" t="s">
-        <v>343</v>
-      </c>
-      <c r="H45" s="13" t="s">
-        <v>341</v>
-      </c>
-      <c r="I45" s="13">
-        <v>1</v>
-      </c>
-      <c r="J45" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="K45" s="13" t="s">
-        <v>111</v>
+        <v>51</v>
+      </c>
+      <c r="G45" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="H45" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="I45" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="J45" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="K45" s="14" t="s">
+        <v>173</v>
       </c>
       <c r="L45" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M45" s="5" t="s">
-        <v>13</v>
+        <v>250</v>
       </c>
       <c r="N45" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="O45" s="18" t="s">
-        <v>212</v>
+      <c r="O45" s="16" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>156</v>
+        <v>255</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>79</v>
+        <v>263</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>156</v>
+        <v>255</v>
       </c>
       <c r="F46" s="13">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="G46" s="13" t="s">
         <v>344</v>
@@ -4709,17 +4709,17 @@
       <c r="I46" s="22" t="s">
         <v>347</v>
       </c>
-      <c r="J46" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="K46" s="15" t="s">
-        <v>188</v>
+      <c r="J46" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="K46" s="19" t="s">
+        <v>226</v>
       </c>
       <c r="L46" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M46" s="5" t="s">
-        <v>213</v>
+        <v>262</v>
       </c>
       <c r="N46" s="16" t="s">
         <v>203</v>
@@ -4730,25 +4730,25 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>190</v>
+        <v>70</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F47" s="13">
-        <v>34</v>
-      </c>
-      <c r="G47" s="13" t="s">
-        <v>344</v>
+        <v>23</v>
+      </c>
+      <c r="G47" s="21" t="s">
+        <v>345</v>
       </c>
       <c r="H47" s="22" t="s">
         <v>347</v>
@@ -4757,7 +4757,7 @@
         <v>347</v>
       </c>
       <c r="J47" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K47" s="15" t="s">
         <v>188</v>
@@ -4766,36 +4766,36 @@
         <v>9</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
       <c r="N47" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="O47" s="16" t="s">
-        <v>204</v>
+      <c r="O47" s="14" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>247</v>
+        <v>152</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C48" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>238</v>
+        <v>73</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>247</v>
+        <v>152</v>
       </c>
       <c r="F48" s="13">
-        <v>35</v>
-      </c>
-      <c r="G48" s="13" t="s">
-        <v>344</v>
+        <v>26</v>
+      </c>
+      <c r="G48" s="21" t="s">
+        <v>345</v>
       </c>
       <c r="H48" s="22" t="s">
         <v>347</v>
@@ -4804,16 +4804,16 @@
         <v>347</v>
       </c>
       <c r="J48" s="13" t="s">
-        <v>65</v>
+        <v>114</v>
       </c>
       <c r="K48" s="13" t="s">
-        <v>195</v>
+        <v>115</v>
       </c>
       <c r="L48" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="N48" s="16" t="s">
         <v>203</v>
@@ -4824,662 +4824,667 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>177</v>
+        <v>153</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>309</v>
+        <v>333</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>179</v>
+        <v>74</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>177</v>
+        <v>153</v>
       </c>
       <c r="F49" s="13">
-        <v>36</v>
-      </c>
-      <c r="G49" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G49" s="21" t="s">
+        <v>345</v>
+      </c>
+      <c r="H49" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="I49" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="J49" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="K49" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="L49" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M49" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="N49" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="O49" s="16" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F50" s="11">
+        <v>1</v>
+      </c>
+      <c r="G50" s="24" t="s">
+        <v>343</v>
+      </c>
+      <c r="H50" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="I50" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="J50" s="11" t="s">
+        <v>350</v>
+      </c>
+      <c r="K50" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="L50" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M50" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="N50" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="O50" s="11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F51" s="11">
+        <v>2</v>
+      </c>
+      <c r="G51" s="24" t="s">
+        <v>343</v>
+      </c>
+      <c r="H51" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="I51" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="J51" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="K51" s="11" t="s">
+        <v>352</v>
+      </c>
+      <c r="L51" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M51" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="N51" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="O51" s="11" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="F52" s="11">
+        <v>9</v>
+      </c>
+      <c r="G52" s="24" t="s">
+        <v>343</v>
+      </c>
+      <c r="H52" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="I52" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="J52" s="11" t="s">
+        <v>353</v>
+      </c>
+      <c r="K52" s="11" t="s">
+        <v>354</v>
+      </c>
+      <c r="L52" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M52" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="N52" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="O52" s="11" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F53" s="11">
+        <v>8</v>
+      </c>
+      <c r="G53" s="24" t="s">
+        <v>343</v>
+      </c>
+      <c r="H53" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="I53" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="J53" s="11" t="s">
+        <v>355</v>
+      </c>
+      <c r="K53" s="11" t="s">
+        <v>356</v>
+      </c>
+      <c r="L53" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M53" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="N53" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="O53" s="11" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" s="11">
+        <v>3</v>
+      </c>
+      <c r="G54" s="11" t="s">
         <v>344</v>
       </c>
-      <c r="H49" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="I49" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="J49" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="K49" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="L49" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M49" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="N49" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="O49" s="15" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="F50" s="13">
-        <v>37</v>
-      </c>
-      <c r="G50" s="20" t="s">
+      <c r="H54" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="I54" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="J54" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="K54" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="L54" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M54" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N54" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="O54" s="11" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="F55" s="11">
+        <v>4</v>
+      </c>
+      <c r="G55" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="H55" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="I55" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="J55" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="K55" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="L55" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M55" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N55" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="O55" s="11" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56" s="11">
+        <v>5</v>
+      </c>
+      <c r="G56" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="H56" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="I56" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="J56" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="K56" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="L56" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M56" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N56" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="O56" s="11" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="F57" s="11">
+        <v>6</v>
+      </c>
+      <c r="G57" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="H57" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="I57" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="J57" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="K57" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="L57" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M57" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N57" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="O57" s="11" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F58" s="12">
+        <v>1</v>
+      </c>
+      <c r="G58" s="23" t="s">
         <v>343</v>
       </c>
-      <c r="H50" s="13"/>
-      <c r="I50" s="13"/>
-      <c r="J50" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="K50" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="L50" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M50" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="N50" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="O50" s="18" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>311</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="F51" s="13">
-        <v>38</v>
-      </c>
-      <c r="G51" s="13" t="s">
+      <c r="H58" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="I58" s="12">
+        <v>1</v>
+      </c>
+      <c r="J58" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="K58" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="L58" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M58" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="N58" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="O58" s="12" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F59" s="12">
+        <v>2</v>
+      </c>
+      <c r="G59" s="12" t="s">
         <v>344</v>
       </c>
-      <c r="H51" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="I51" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="J51" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="K51" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="L51" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M51" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="N51" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="O51" s="16" t="s">
+      <c r="H59" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="I59" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="J59" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="K59" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="L59" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M59" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N59" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="O59" s="12" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F60" s="12">
+        <v>3</v>
+      </c>
+      <c r="G60" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="H60" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="I60" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="J60" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="K60" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="L60" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M60" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N60" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="O60" s="12" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="F52" s="13">
-        <v>39</v>
-      </c>
-      <c r="G52" s="13" t="s">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F61" s="12">
+        <v>4</v>
+      </c>
+      <c r="G61" s="12" t="s">
         <v>344</v>
       </c>
-      <c r="H52" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="I52" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="J52" s="13" t="s">
-        <v>273</v>
-      </c>
-      <c r="K52" s="13" t="s">
-        <v>273</v>
-      </c>
-      <c r="L52" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M52" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="N52" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="O52" s="16" t="s">
+      <c r="H61" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="I61" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="J61" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="K61" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="L61" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M61" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="N61" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="O61" s="12" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="F53" s="13">
-        <v>41</v>
-      </c>
-      <c r="G53" s="13" t="s">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F62" s="12">
+        <v>5</v>
+      </c>
+      <c r="G62" s="12" t="s">
         <v>344</v>
       </c>
-      <c r="H53" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="I53" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="J53" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="K53" s="13" t="s">
-        <v>228</v>
-      </c>
-      <c r="L53" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M53" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="N53" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="O53" s="16" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>336</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="F54" s="13">
-        <v>42</v>
-      </c>
-      <c r="G54" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="H54" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="I54" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="J54" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="K54" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="L54" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M54" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="N54" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="O54" s="16" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="F55" s="13">
-        <v>43</v>
-      </c>
-      <c r="G55" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="H55" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="I55" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="J55" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="K55" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="L55" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M55" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="N55" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="O55" s="16" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="F56" s="13">
-        <v>44</v>
-      </c>
-      <c r="G56" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="H56" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="I56" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="J56" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="K56" s="13" t="s">
-        <v>233</v>
-      </c>
-      <c r="L56" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M56" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="N56" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="O56" s="16" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="F57" s="13">
-        <v>45</v>
-      </c>
-      <c r="G57" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="H57" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="I57" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="J57" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="K57" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="L57" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M57" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="N57" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="O57" s="16" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="F58" s="13">
-        <v>46</v>
-      </c>
-      <c r="G58" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="H58" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="I58" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="J58" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="K58" s="13" t="s">
-        <v>237</v>
-      </c>
-      <c r="L58" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M58" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="N58" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="O58" s="16" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="F59" s="13">
-        <v>48</v>
-      </c>
-      <c r="G59" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="H59" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="I59" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="J59" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="K59" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="L59" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M59" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="N59" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="O59" s="18" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="F60" s="13">
-        <v>50</v>
-      </c>
-      <c r="G60" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="H60" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="I60" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="J60" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="K60" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="L60" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M60" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="N60" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="O60" s="16" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>337</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="F61" s="13">
-        <v>51</v>
-      </c>
-      <c r="G61" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="H61" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="I61" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="J61" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="K61" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="L61" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M61" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="N61" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="O61" s="16" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="F62" s="13">
-        <v>52</v>
-      </c>
-      <c r="G62" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="H62" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="I62" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="J62" s="19" t="s">
-        <v>225</v>
-      </c>
-      <c r="K62" s="19" t="s">
-        <v>226</v>
-      </c>
-      <c r="L62" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M62" s="5" t="s">
-        <v>262</v>
+      <c r="H62" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="I62" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="J62" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="K62" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="L62" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M62" s="3" t="s">
+        <v>170</v>
       </c>
       <c r="N62" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="O62" s="16" t="s">
+      <c r="O62" s="12" t="s">
         <v>204</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:M1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M14">
-    <sortCondition ref="F2:F14"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O62">
+    <sortCondition ref="C2:C62"/>
+    <sortCondition ref="G2:G62"/>
   </sortState>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Refactoring for final DIGS data set
</commit_message>
<xml_diff>
--- a/tabular/eve/ehbv-refseqs-side-data.xlsx
+++ b/tabular/eve/ehbv-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791296DD-9BB0-E348-BA86-04A50473E068}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47DE488-D72F-C84F-95EA-A8FACF6D4E73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12680" yWindow="1820" windowWidth="36120" windowHeight="22320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="365">
   <si>
     <t>Herpetohepadnavirus</t>
   </si>
@@ -1122,6 +1122,15 @@
   </si>
   <si>
     <t>avi.39-psittaciformes</t>
+  </si>
+  <si>
+    <t>ehbv-meta.6-sphenodon</t>
+  </si>
+  <si>
+    <t>meta.6-sphenodon</t>
+  </si>
+  <si>
+    <t>Sphenodon</t>
   </si>
 </sst>
 </file>
@@ -2594,10 +2603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P60"/>
+  <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A32" sqref="A1:P60"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -5499,6 +5508,54 @@
         <v>185</v>
       </c>
     </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="F61" s="12">
+        <v>1</v>
+      </c>
+      <c r="G61" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="H61" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="I61" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="J61" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="K61" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="L61" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M61" s="3"/>
+      <c r="N61" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="O61" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="P61" s="12" t="s">
+        <v>185</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:N1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P60">

</xml_diff>

<commit_message>
Refactor element IDs - more accurate distribution component for avi 12,14,15,27,30
</commit_message>
<xml_diff>
--- a/tabular/eve/ehbv-refseqs-side-data.xlsx
+++ b/tabular/eve/ehbv-refseqs-side-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47DE488-D72F-C84F-95EA-A8FACF6D4E73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E57346F-C565-3C41-A00A-D5A8483FEAF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12680" yWindow="1820" windowWidth="36120" windowHeight="22320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -86,9 +86,6 @@
     <t>Paleognathae</t>
   </si>
   <si>
-    <t>Gaviiformes</t>
-  </si>
-  <si>
     <t>Crocodilia</t>
   </si>
   <si>
@@ -185,9 +182,6 @@
     <t>ehbv-avi.11-tyto</t>
   </si>
   <si>
-    <t>ehbv-avi.14-gaviiformes</t>
-  </si>
-  <si>
     <t>nearest_upstream_orf</t>
   </si>
   <si>
@@ -200,9 +194,6 @@
     <t>host_group_name</t>
   </si>
   <si>
-    <t>ehbv-avi.15-gaviiformes</t>
-  </si>
-  <si>
     <t>ZNF516</t>
   </si>
   <si>
@@ -458,9 +449,6 @@
     <t>ehbv-avi.26-psittaciformes</t>
   </si>
   <si>
-    <t>ehbv-avi.27-suliformes-con</t>
-  </si>
-  <si>
     <t>ehbv-avi.29-psittacula</t>
   </si>
   <si>
@@ -500,9 +488,6 @@
     <t>Psittaciformes</t>
   </si>
   <si>
-    <t>Suliformes</t>
-  </si>
-  <si>
     <t>Psittacula</t>
   </si>
   <si>
@@ -737,12 +722,6 @@
     <t>ehbv-herpeto.7-serpentes-con</t>
   </si>
   <si>
-    <t>ehbv-avi.12-anseriformes-con</t>
-  </si>
-  <si>
-    <t>Anseriformes</t>
-  </si>
-  <si>
     <t>EPHA6</t>
   </si>
   <si>
@@ -812,12 +791,6 @@
     <t>avi.11-tyto</t>
   </si>
   <si>
-    <t>avi.14-gaviiformes</t>
-  </si>
-  <si>
-    <t>avi.15-gaviiformes</t>
-  </si>
-  <si>
     <t>avi.16-turaco</t>
   </si>
   <si>
@@ -902,18 +875,12 @@
     <t>avi.1-neoaves</t>
   </si>
   <si>
-    <t>avi.12-anseriformes</t>
-  </si>
-  <si>
     <t>avi.13-paleognathae</t>
   </si>
   <si>
     <t>avi.21-paleognathae</t>
   </si>
   <si>
-    <t>avi.27-suliformes</t>
-  </si>
-  <si>
     <t>avi.31-passeriformes</t>
   </si>
   <si>
@@ -1109,12 +1076,6 @@
     <t>avi.45-psittaciformes</t>
   </si>
   <si>
-    <t>ehbv-avi.30-anseriformes-con</t>
-  </si>
-  <si>
-    <t>avi.30-anseriformes</t>
-  </si>
-  <si>
     <t>ehbv-avi.5-passeriformes</t>
   </si>
   <si>
@@ -1131,6 +1092,45 @@
   </si>
   <si>
     <t>Sphenodon</t>
+  </si>
+  <si>
+    <t>ehbv-avi.14-gavia</t>
+  </si>
+  <si>
+    <t>avi.14-gavia</t>
+  </si>
+  <si>
+    <t>gavia</t>
+  </si>
+  <si>
+    <t>ehbv-avi.15-gavia</t>
+  </si>
+  <si>
+    <t>avi.15-gavia</t>
+  </si>
+  <si>
+    <t>ehbv-avi.12-anseridae-con</t>
+  </si>
+  <si>
+    <t>ehbv-avi.30-anseridae-con</t>
+  </si>
+  <si>
+    <t>avi.12-anseridae</t>
+  </si>
+  <si>
+    <t>anseridae</t>
+  </si>
+  <si>
+    <t>avi.30-anseridae</t>
+  </si>
+  <si>
+    <t>ehbv-avi.27-sulidae-con</t>
+  </si>
+  <si>
+    <t>avi.27-sulidae</t>
+  </si>
+  <si>
+    <t>sulidae</t>
   </si>
 </sst>
 </file>
@@ -2605,8 +2605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D42" sqref="A1:P61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2628,13 +2628,13 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -2643,168 +2643,168 @@
         <v>3</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F2" s="13">
         <v>1</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="I2" s="13">
         <v>1</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M2" s="5"/>
       <c r="N2" s="5" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="O2" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F3" s="13">
         <v>2</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P3" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" s="13">
         <v>3</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>9</v>
@@ -2814,45 +2814,45 @@
         <v>13</v>
       </c>
       <c r="O4" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F5" s="13">
         <v>4</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J5" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="K5" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>9</v>
@@ -2862,45 +2862,45 @@
         <v>13</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>359</v>
+        <v>346</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F6" s="13">
         <v>5</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>9</v>
@@ -2910,45 +2910,45 @@
         <v>13</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P6" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F7" s="13">
         <v>6</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H7" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I7" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>9</v>
@@ -2958,45 +2958,45 @@
         <v>13</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P7" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F8" s="13">
         <v>7</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H8" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I8" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>9</v>
@@ -3006,93 +3006,93 @@
         <v>13</v>
       </c>
       <c r="O8" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P8" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F9" s="13">
         <v>8</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I9" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M9" s="5"/>
       <c r="N9" s="5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="O9" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P9" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F10" s="13">
         <v>9</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="I10" s="13">
         <v>1</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>9</v>
@@ -3102,45 +3102,45 @@
         <v>6</v>
       </c>
       <c r="O10" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P10" s="13" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F11" s="13">
         <v>10</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="I11" s="13">
         <v>1</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>9</v>
@@ -3150,45 +3150,45 @@
         <v>6</v>
       </c>
       <c r="O11" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P11" s="13" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F12" s="13">
         <v>11</v>
       </c>
       <c r="G12" s="19" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="I12" s="13">
         <v>1</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="K12" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="L12" s="5" t="s">
         <v>9</v>
@@ -3198,93 +3198,93 @@
         <v>14</v>
       </c>
       <c r="O12" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P12" s="24" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>233</v>
+        <v>357</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>288</v>
+        <v>359</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>233</v>
+        <v>357</v>
       </c>
       <c r="F13" s="13">
         <v>12</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="I13" s="13">
         <v>1</v>
       </c>
       <c r="J13" s="26" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="K13" s="26" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M13" s="5"/>
       <c r="N13" s="5" t="s">
-        <v>234</v>
+        <v>360</v>
       </c>
       <c r="O13" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P13" s="24" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F14" s="13">
         <v>13</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H14" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I14" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="L14" s="5" t="s">
         <v>9</v>
@@ -3294,333 +3294,333 @@
         <v>15</v>
       </c>
       <c r="O14" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P14" s="16" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>49</v>
+        <v>352</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>258</v>
+        <v>353</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>49</v>
+        <v>352</v>
       </c>
       <c r="F15" s="13">
         <v>14</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="I15" s="13">
         <v>11</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="L15" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M15" s="5"/>
       <c r="N15" s="5" t="s">
-        <v>16</v>
+        <v>354</v>
       </c>
       <c r="O15" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P15" s="24" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>54</v>
+        <v>355</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>259</v>
+        <v>356</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>54</v>
+        <v>355</v>
       </c>
       <c r="F16" s="13">
         <v>15</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="I16" s="13">
         <v>1</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="K16" s="13" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="L16" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M16" s="5"/>
       <c r="N16" s="5" t="s">
-        <v>16</v>
+        <v>354</v>
       </c>
       <c r="O16" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P16" s="24" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F17" s="13">
         <v>16</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H17" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I17" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="K17" s="13" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="L17" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M17" s="5"/>
       <c r="N17" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="O17" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P17" s="16" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F18" s="13">
         <v>18</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="I18" s="13">
         <v>1</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="K18" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="L18" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M18" s="5"/>
       <c r="N18" s="5" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="O18" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P18" s="16" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F19" s="13">
         <v>19</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="I19" s="13">
         <v>1</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="L19" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M19" s="5"/>
       <c r="N19" s="5" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="O19" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P19" s="13" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F20" s="13">
         <v>20</v>
       </c>
       <c r="G20" s="19" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="I20" s="13">
         <v>1</v>
       </c>
       <c r="J20" s="27" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K20" s="27" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="L20" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M20" s="5"/>
       <c r="N20" s="5" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="O20" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P20" s="17" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F21" s="13">
         <v>21</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H21" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I21" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="L21" s="5" t="s">
         <v>9</v>
@@ -3630,45 +3630,45 @@
         <v>15</v>
       </c>
       <c r="O21" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P21" s="16" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F22" s="13">
         <v>22</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H22" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I22" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K22" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="L22" s="5" t="s">
         <v>9</v>
@@ -3678,429 +3678,429 @@
         <v>14</v>
       </c>
       <c r="O22" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P22" s="24" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="F23" s="13">
         <v>23</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="H23" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I23" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J23" s="28" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="K23" s="28" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="L23" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M23" s="5"/>
       <c r="N23" s="5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="O23" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P23" s="14" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F24" s="13">
         <v>24</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H24" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I24" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J24" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="K24" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L24" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M24" s="5"/>
       <c r="N24" s="5" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="O24" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P24" s="17" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F25" s="13">
         <v>25</v>
       </c>
       <c r="G25" s="19" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="I25" s="13">
         <v>523</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K25" s="13" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="L25" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M25" s="5"/>
       <c r="N25" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="O25" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P25" s="17" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F26" s="13">
         <v>26</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="H26" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I26" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J26" s="18" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="K26" s="18" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="L26" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M26" s="5"/>
       <c r="N26" s="5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="O26" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P26" s="16" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>140</v>
+        <v>362</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>291</v>
+        <v>363</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>140</v>
+        <v>362</v>
       </c>
       <c r="F27" s="13">
         <v>27</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="H27" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I27" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K27" s="13" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="L27" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M27" s="5"/>
       <c r="N27" s="5" t="s">
-        <v>154</v>
+        <v>364</v>
       </c>
       <c r="O27" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P27" s="16" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="F28" s="13">
         <v>28</v>
       </c>
       <c r="G28" s="19" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="I28" s="13">
         <v>745</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="K28" s="13" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="L28" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M28" s="5"/>
       <c r="N28" s="5" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="O28" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P28" s="13" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F29" s="13">
         <v>29</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K29" s="13" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="L29" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M29" s="5"/>
       <c r="N29" s="5" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="O29" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P29" s="14" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" s="5" t="s">
         <v>358</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>357</v>
       </c>
       <c r="F30" s="13">
         <v>30</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H30" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I30" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J30" s="26" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="K30" s="26" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L30" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M30" s="5"/>
       <c r="N30" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="O30" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P30" s="16" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F31" s="13">
         <v>31</v>
       </c>
       <c r="G31" s="19" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="I31" s="13">
         <v>1</v>
       </c>
       <c r="J31" s="25" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="K31" s="25" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="L31" s="5" t="s">
         <v>9</v>
@@ -4110,778 +4110,778 @@
         <v>13</v>
       </c>
       <c r="O31" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P31" s="14" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F32" s="13">
         <v>32</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H32" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I32" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="K32" s="15" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="L32" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M32" s="5"/>
       <c r="N32" s="5" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="O32" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P32" s="16" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F33" s="13">
         <v>34</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H33" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I33" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J33" s="13" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="K33" s="13" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="L33" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M33" s="5"/>
       <c r="N33" s="5" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="O33" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P33" s="16" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="F34" s="13">
         <v>35</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H34" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I34" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J34" s="25" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="K34" s="25" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="L34" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M34" s="5"/>
       <c r="N34" s="5" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="O34" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P34" s="16" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="F35" s="13">
         <v>37</v>
       </c>
       <c r="G35" s="19" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I35" s="13" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J35" s="13" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="K35" s="13" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="L35" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M35" s="5"/>
       <c r="N35" s="5" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="O35" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P35" s="14" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="F36" s="13">
         <v>38</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H36" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I36" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="K36" s="13" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="L36" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M36" s="5"/>
       <c r="N36" s="5" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="O36" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P36" s="16" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>360</v>
+        <v>347</v>
       </c>
       <c r="F37" s="13">
         <v>39</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H37" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I37" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="K37" s="13" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="L37" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M37" s="5"/>
       <c r="N37" s="5" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="O37" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P37" s="16" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F38" s="13">
         <v>41</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H38" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I38" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="K38" s="13" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="L38" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M38" s="5"/>
       <c r="N38" s="5" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="O38" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P38" s="16" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F39" s="13">
         <v>42</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H39" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I39" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="K39" s="13" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="L39" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M39" s="5"/>
       <c r="N39" s="5" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="O39" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P39" s="16" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="F40" s="13">
         <v>43</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H40" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I40" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J40" s="13" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="K40" s="13" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="L40" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M40" s="5"/>
       <c r="N40" s="5" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
       <c r="O40" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P40" s="16" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="F41" s="13">
         <v>44</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H41" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I41" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J41" s="13" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="K41" s="13" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="L41" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M41" s="5"/>
       <c r="N41" s="5" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="O41" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P41" s="16" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
       <c r="F42" s="13">
         <v>45</v>
       </c>
       <c r="G42" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H42" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I42" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J42" s="13" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="K42" s="13" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L42" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M42" s="5"/>
       <c r="N42" s="5" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="O42" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P42" s="16" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="F43" s="13">
         <v>46</v>
       </c>
       <c r="G43" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H43" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I43" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J43" s="27" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="K43" s="27" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="L43" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M43" s="5"/>
       <c r="N43" s="5" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="O43" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P43" s="16" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="F44" s="13">
         <v>48</v>
       </c>
       <c r="G44" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H44" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I44" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J44" s="13" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="K44" s="13" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="L44" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M44" s="5"/>
       <c r="N44" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="O44" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P44" s="16" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="F45" s="13">
         <v>49</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H45" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I45" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J45" s="13" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="K45" s="13" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="L45" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M45" s="5"/>
       <c r="N45" s="5" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="O45" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P45" s="16" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F46" s="13">
         <v>52</v>
       </c>
       <c r="G46" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H46" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I46" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J46" s="18" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="K46" s="18" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="L46" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M46" s="5"/>
       <c r="N46" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="O46" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P46" s="16" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="F47" s="13">
         <v>53</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H47" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I47" s="21" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J47" s="13" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="K47" s="13" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="L47" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M47" s="5"/>
       <c r="N47" s="5" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="O47" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P47" s="16" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -4889,13 +4889,13 @@
         <v>10</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>10</v>
@@ -4904,19 +4904,19 @@
         <v>1</v>
       </c>
       <c r="G48" s="23" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="H48" s="11" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I48" s="11" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J48" s="11" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="K48" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L48" s="4" t="s">
         <v>9</v>
@@ -4926,45 +4926,45 @@
         <v>4</v>
       </c>
       <c r="O48" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P48" s="11" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F49" s="11">
         <v>2</v>
       </c>
       <c r="G49" s="23" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="H49" s="11" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I49" s="11" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J49" s="11" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="K49" s="11" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="L49" s="4" t="s">
         <v>9</v>
@@ -4974,24 +4974,24 @@
         <v>4</v>
       </c>
       <c r="O49" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P49" s="11" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>11</v>
@@ -5000,80 +5000,80 @@
         <v>3</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H50" s="11" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J50" s="11" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="K50" s="11" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="L50" s="4" t="s">
         <v>9</v>
       </c>
       <c r="M50" s="4"/>
       <c r="N50" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O50" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P50" s="11" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F51" s="11">
         <v>4</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H51" s="11" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I51" s="11" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J51" s="11" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="K51" s="11" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="L51" s="4" t="s">
         <v>9</v>
       </c>
       <c r="M51" s="4"/>
       <c r="N51" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O51" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P51" s="11" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
@@ -5081,13 +5081,13 @@
         <v>12</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>12</v>
@@ -5096,115 +5096,115 @@
         <v>5</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H52" s="11" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I52" s="11" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J52" s="11" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="K52" s="11" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="L52" s="4" t="s">
         <v>9</v>
       </c>
       <c r="M52" s="4"/>
       <c r="N52" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O52" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P52" s="11" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="F53" s="11">
         <v>6</v>
       </c>
       <c r="G53" s="11" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H53" s="11" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I53" s="11" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J53" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="K53" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L53" s="4" t="s">
         <v>9</v>
       </c>
       <c r="M53" s="4"/>
       <c r="N53" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O53" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P53" s="11" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F54" s="11">
         <v>9</v>
       </c>
       <c r="G54" s="23" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="H54" s="11" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I54" s="11" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J54" s="28" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="K54" s="28" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="L54" s="4" t="s">
         <v>9</v>
@@ -5214,45 +5214,45 @@
         <v>4</v>
       </c>
       <c r="O54" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P54" s="11" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="F55" s="11">
         <v>8</v>
       </c>
       <c r="G55" s="23" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="H55" s="11" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I55" s="11" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J55" s="11" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="K55" s="11" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
       <c r="L55" s="4" t="s">
         <v>9</v>
@@ -5262,141 +5262,141 @@
         <v>4</v>
       </c>
       <c r="O55" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P55" s="11" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F56" s="12">
         <v>1</v>
       </c>
       <c r="G56" s="22" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="H56" s="12" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="I56" s="12">
         <v>1</v>
       </c>
       <c r="J56" s="12" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K56" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="L56" s="3" t="s">
         <v>9</v>
       </c>
       <c r="M56" s="3"/>
       <c r="N56" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="O56" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P56" s="12" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F57" s="12">
         <v>2</v>
       </c>
       <c r="G57" s="12" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H57" s="12" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I57" s="12" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J57" s="12" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="K57" s="12" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="L57" s="3" t="s">
         <v>9</v>
       </c>
       <c r="M57" s="3"/>
       <c r="N57" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O57" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="P57" s="12" t="s">
         <v>184</v>
-      </c>
-      <c r="P57" s="12" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F58" s="12">
         <v>3</v>
       </c>
       <c r="G58" s="12" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H58" s="12" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I58" s="12" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J58" s="12" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K58" s="12" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="L58" s="3" t="s">
         <v>9</v>
@@ -5406,154 +5406,154 @@
         <v>7</v>
       </c>
       <c r="O58" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P58" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F59" s="12">
         <v>4</v>
       </c>
       <c r="G59" s="12" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H59" s="12" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I59" s="12" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J59" s="12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="K59" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="L59" s="3" t="s">
         <v>9</v>
       </c>
       <c r="M59" s="3"/>
       <c r="N59" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="O59" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P59" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F60" s="12">
         <v>5</v>
       </c>
       <c r="G60" s="12" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H60" s="12" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I60" s="12" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J60" s="12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="K60" s="12" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="L60" s="3" t="s">
         <v>9</v>
       </c>
       <c r="M60" s="3"/>
       <c r="N60" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="O60" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P60" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>362</v>
+        <v>349</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>363</v>
+        <v>350</v>
       </c>
       <c r="C61" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>362</v>
+        <v>349</v>
       </c>
       <c r="F61" s="12">
         <v>1</v>
       </c>
       <c r="G61" s="12" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="H61" s="12" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="I61" s="12" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="J61" s="12" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="K61" s="12" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="L61" s="3" t="s">
         <v>9</v>
       </c>
       <c r="M61" s="3"/>
       <c r="N61" s="3" t="s">
-        <v>364</v>
+        <v>351</v>
       </c>
       <c r="O61" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P61" s="12" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactoring for updated IDs
</commit_message>
<xml_diff>
--- a/tabular/eve/ehbv-refseqs-side-data.xlsx
+++ b/tabular/eve/ehbv-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E57346F-C565-3C41-A00A-D5A8483FEAF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC438172-2C86-0E4B-89FA-DA2020EA916A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12680" yWindow="1820" windowWidth="36120" windowHeight="22320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="364">
   <si>
     <t>Herpetohepadnavirus</t>
   </si>
@@ -557,9 +557,6 @@
     <t>CYB5A</t>
   </si>
   <si>
-    <t>Anseridae</t>
-  </si>
-  <si>
     <t>ehbv-herpeto.8-serpentes-con</t>
   </si>
   <si>
@@ -1109,21 +1106,6 @@
     <t>avi.15-gavia</t>
   </si>
   <si>
-    <t>ehbv-avi.12-anseridae-con</t>
-  </si>
-  <si>
-    <t>ehbv-avi.30-anseridae-con</t>
-  </si>
-  <si>
-    <t>avi.12-anseridae</t>
-  </si>
-  <si>
-    <t>anseridae</t>
-  </si>
-  <si>
-    <t>avi.30-anseridae</t>
-  </si>
-  <si>
     <t>ehbv-avi.27-sulidae-con</t>
   </si>
   <si>
@@ -1131,6 +1113,21 @@
   </si>
   <si>
     <t>sulidae</t>
+  </si>
+  <si>
+    <t>ehbv-avi.12-anatidae-con</t>
+  </si>
+  <si>
+    <t>avi.12-anatidae</t>
+  </si>
+  <si>
+    <t>anatidae</t>
+  </si>
+  <si>
+    <t>ehbv-avi.30-anatidae-con</t>
+  </si>
+  <si>
+    <t>avi.30-anatidae</t>
   </si>
 </sst>
 </file>
@@ -2605,8 +2602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D42" sqref="A1:P61"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D27" sqref="A1:P61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2628,13 +2625,13 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>233</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -2646,13 +2643,13 @@
         <v>50</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>48</v>
@@ -2664,16 +2661,16 @@
         <v>8</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="O1" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -2681,7 +2678,7 @@
         <v>126</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>1</v>
@@ -2696,10 +2693,10 @@
         <v>1</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I2" s="13">
         <v>1</v>
@@ -2718,10 +2715,10 @@
         <v>145</v>
       </c>
       <c r="O2" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -2729,7 +2726,7 @@
         <v>78</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>1</v>
@@ -2744,19 +2741,19 @@
         <v>2</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>9</v>
@@ -2766,10 +2763,10 @@
         <v>146</v>
       </c>
       <c r="O3" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P3" s="12" t="s">
         <v>179</v>
-      </c>
-      <c r="P3" s="12" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -2777,7 +2774,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>1</v>
@@ -2792,13 +2789,13 @@
         <v>3</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J4" s="13" t="s">
         <v>95</v>
@@ -2814,10 +2811,10 @@
         <v>13</v>
       </c>
       <c r="O4" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P4" s="12" t="s">
         <v>179</v>
-      </c>
-      <c r="P4" s="12" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -2825,7 +2822,7 @@
         <v>79</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>1</v>
@@ -2840,13 +2837,13 @@
         <v>4</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J5" s="27" t="s">
         <v>96</v>
@@ -2862,18 +2859,18 @@
         <v>13</v>
       </c>
       <c r="O5" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P5" s="12" t="s">
         <v>179</v>
-      </c>
-      <c r="P5" s="12" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>1</v>
@@ -2888,13 +2885,13 @@
         <v>5</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J6" s="13" t="s">
         <v>97</v>
@@ -2910,10 +2907,10 @@
         <v>13</v>
       </c>
       <c r="O6" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P6" s="12" t="s">
         <v>179</v>
-      </c>
-      <c r="P6" s="12" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -2921,7 +2918,7 @@
         <v>43</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>1</v>
@@ -2936,13 +2933,13 @@
         <v>6</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H7" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I7" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J7" s="13" t="s">
         <v>98</v>
@@ -2958,10 +2955,10 @@
         <v>13</v>
       </c>
       <c r="O7" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P7" s="12" t="s">
         <v>179</v>
-      </c>
-      <c r="P7" s="12" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -2969,7 +2966,7 @@
         <v>44</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>1</v>
@@ -2984,16 +2981,16 @@
         <v>7</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H8" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I8" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K8" s="13" t="s">
         <v>121</v>
@@ -3006,10 +3003,10 @@
         <v>13</v>
       </c>
       <c r="O8" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P8" s="12" t="s">
         <v>179</v>
-      </c>
-      <c r="P8" s="12" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -3017,7 +3014,7 @@
         <v>80</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>1</v>
@@ -3032,13 +3029,13 @@
         <v>8</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I9" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J9" s="13" t="s">
         <v>122</v>
@@ -3054,10 +3051,10 @@
         <v>147</v>
       </c>
       <c r="O9" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P9" s="12" t="s">
         <v>179</v>
-      </c>
-      <c r="P9" s="12" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -3065,7 +3062,7 @@
         <v>45</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>1</v>
@@ -3080,19 +3077,19 @@
         <v>9</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I10" s="13">
         <v>1</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>9</v>
@@ -3102,10 +3099,10 @@
         <v>6</v>
       </c>
       <c r="O10" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P10" s="13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -3113,7 +3110,7 @@
         <v>46</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>1</v>
@@ -3128,19 +3125,19 @@
         <v>10</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I11" s="13">
         <v>1</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>9</v>
@@ -3150,10 +3147,10 @@
         <v>6</v>
       </c>
       <c r="O11" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P11" s="13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -3161,7 +3158,7 @@
         <v>47</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>1</v>
@@ -3176,10 +3173,10 @@
         <v>11</v>
       </c>
       <c r="G12" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I12" s="13">
         <v>1</v>
@@ -3198,18 +3195,18 @@
         <v>14</v>
       </c>
       <c r="O12" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P12" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>1</v>
@@ -3218,38 +3215,38 @@
         <v>34</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="F13" s="13">
         <v>12</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I13" s="13">
         <v>1</v>
       </c>
       <c r="J13" s="26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K13" s="26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M13" s="5"/>
       <c r="N13" s="5" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="O13" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P13" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -3257,7 +3254,7 @@
         <v>128</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>1</v>
@@ -3272,13 +3269,13 @@
         <v>13</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H14" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I14" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J14" s="13" t="s">
         <v>93</v>
@@ -3294,18 +3291,18 @@
         <v>15</v>
       </c>
       <c r="O14" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P14" s="16" t="s">
         <v>179</v>
-      </c>
-      <c r="P14" s="16" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>352</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>353</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>1</v>
@@ -3314,16 +3311,16 @@
         <v>36</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F15" s="13">
         <v>14</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I15" s="13">
         <v>11</v>
@@ -3339,21 +3336,21 @@
       </c>
       <c r="M15" s="5"/>
       <c r="N15" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="O15" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P15" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>355</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>356</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>1</v>
@@ -3362,16 +3359,16 @@
         <v>56</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F16" s="13">
         <v>15</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I16" s="13">
         <v>1</v>
@@ -3387,13 +3384,13 @@
       </c>
       <c r="M16" s="5"/>
       <c r="N16" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="O16" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P16" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -3401,7 +3398,7 @@
         <v>125</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>1</v>
@@ -3416,13 +3413,13 @@
         <v>16</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H17" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I17" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J17" s="13" t="s">
         <v>114</v>
@@ -3438,10 +3435,10 @@
         <v>113</v>
       </c>
       <c r="O17" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P17" s="16" t="s">
         <v>179</v>
-      </c>
-      <c r="P17" s="16" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -3449,7 +3446,7 @@
         <v>129</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>1</v>
@@ -3464,10 +3461,10 @@
         <v>18</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I18" s="13">
         <v>1</v>
@@ -3486,10 +3483,10 @@
         <v>169</v>
       </c>
       <c r="O18" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P18" s="16" t="s">
         <v>179</v>
-      </c>
-      <c r="P18" s="16" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -3497,7 +3494,7 @@
         <v>130</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>1</v>
@@ -3512,10 +3509,10 @@
         <v>19</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I19" s="13">
         <v>1</v>
@@ -3534,10 +3531,10 @@
         <v>170</v>
       </c>
       <c r="O19" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P19" s="13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -3545,7 +3542,7 @@
         <v>131</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>1</v>
@@ -3560,10 +3557,10 @@
         <v>20</v>
       </c>
       <c r="G20" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I20" s="13">
         <v>1</v>
@@ -3582,10 +3579,10 @@
         <v>171</v>
       </c>
       <c r="O20" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P20" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -3593,7 +3590,7 @@
         <v>132</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>1</v>
@@ -3608,16 +3605,16 @@
         <v>21</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H21" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I21" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="K21" s="13" t="s">
         <v>91</v>
@@ -3630,10 +3627,10 @@
         <v>15</v>
       </c>
       <c r="O21" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P21" s="16" t="s">
         <v>179</v>
-      </c>
-      <c r="P21" s="16" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -3641,7 +3638,7 @@
         <v>133</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>1</v>
@@ -3656,13 +3653,13 @@
         <v>22</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H22" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I22" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J22" s="13" t="s">
         <v>104</v>
@@ -3678,10 +3675,10 @@
         <v>14</v>
       </c>
       <c r="O22" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P22" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -3689,7 +3686,7 @@
         <v>164</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>1</v>
@@ -3698,25 +3695,25 @@
         <v>64</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F23" s="13">
         <v>23</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H23" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I23" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J23" s="28" t="s">
+        <v>323</v>
+      </c>
+      <c r="K23" s="28" t="s">
         <v>324</v>
-      </c>
-      <c r="K23" s="28" t="s">
-        <v>325</v>
       </c>
       <c r="L23" s="5" t="s">
         <v>9</v>
@@ -3726,10 +3723,10 @@
         <v>149</v>
       </c>
       <c r="O23" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P23" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -3737,7 +3734,7 @@
         <v>134</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>1</v>
@@ -3752,13 +3749,13 @@
         <v>24</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H24" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I24" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J24" s="27" t="s">
         <v>96</v>
@@ -3774,10 +3771,10 @@
         <v>148</v>
       </c>
       <c r="O24" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P24" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -3785,7 +3782,7 @@
         <v>135</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>1</v>
@@ -3800,10 +3797,10 @@
         <v>25</v>
       </c>
       <c r="G25" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I25" s="13">
         <v>523</v>
@@ -3822,10 +3819,10 @@
         <v>151</v>
       </c>
       <c r="O25" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P25" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -3833,7 +3830,7 @@
         <v>136</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>1</v>
@@ -3848,19 +3845,19 @@
         <v>26</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H26" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I26" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J26" s="18" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="K26" s="18" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L26" s="5" t="s">
         <v>9</v>
@@ -3870,18 +3867,18 @@
         <v>149</v>
       </c>
       <c r="O26" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P26" s="16" t="s">
         <v>179</v>
-      </c>
-      <c r="P26" s="16" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>1</v>
@@ -3890,46 +3887,46 @@
         <v>68</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="F27" s="13">
         <v>27</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H27" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I27" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J27" s="13" t="s">
         <v>101</v>
       </c>
       <c r="K27" s="13" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L27" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M27" s="5"/>
       <c r="N27" s="5" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="O27" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P27" s="16" t="s">
         <v>179</v>
-      </c>
-      <c r="P27" s="16" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>1</v>
@@ -3938,38 +3935,38 @@
         <v>69</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F28" s="13">
         <v>28</v>
       </c>
       <c r="G28" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I28" s="13">
         <v>745</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K28" s="13" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="L28" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M28" s="5"/>
       <c r="N28" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O28" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P28" s="13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -3977,7 +3974,7 @@
         <v>137</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>1</v>
@@ -3992,13 +3989,13 @@
         <v>29</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J29" s="13" t="s">
         <v>107</v>
@@ -4014,18 +4011,18 @@
         <v>150</v>
       </c>
       <c r="O29" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P29" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>1</v>
@@ -4034,19 +4031,19 @@
         <v>71</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="F30" s="13">
         <v>30</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H30" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I30" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J30" s="26" t="s">
         <v>102</v>
@@ -4059,21 +4056,21 @@
       </c>
       <c r="M30" s="5"/>
       <c r="N30" s="5" t="s">
-        <v>173</v>
+        <v>361</v>
       </c>
       <c r="O30" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P30" s="16" t="s">
         <v>179</v>
-      </c>
-      <c r="P30" s="16" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>1</v>
@@ -4088,19 +4085,19 @@
         <v>31</v>
       </c>
       <c r="G31" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I31" s="13">
         <v>1</v>
       </c>
       <c r="J31" s="25" t="s">
+        <v>313</v>
+      </c>
+      <c r="K31" s="25" t="s">
         <v>314</v>
-      </c>
-      <c r="K31" s="25" t="s">
-        <v>315</v>
       </c>
       <c r="L31" s="5" t="s">
         <v>9</v>
@@ -4110,10 +4107,10 @@
         <v>13</v>
       </c>
       <c r="O31" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P31" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -4121,7 +4118,7 @@
         <v>139</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>1</v>
@@ -4136,13 +4133,13 @@
         <v>32</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H32" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I32" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J32" s="13" t="s">
         <v>100</v>
@@ -4155,13 +4152,13 @@
       </c>
       <c r="M32" s="5"/>
       <c r="N32" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O32" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P32" s="16" t="s">
         <v>179</v>
-      </c>
-      <c r="P32" s="16" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -4169,7 +4166,7 @@
         <v>166</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>1</v>
@@ -4184,19 +4181,19 @@
         <v>34</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H33" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I33" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J33" s="13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="K33" s="13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="L33" s="5" t="s">
         <v>9</v>
@@ -4206,42 +4203,42 @@
         <v>168</v>
       </c>
       <c r="O33" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P33" s="16" t="s">
         <v>179</v>
-      </c>
-      <c r="P33" s="16" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F34" s="13">
         <v>35</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H34" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I34" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J34" s="25" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="K34" s="25" t="s">
         <v>172</v>
@@ -4254,10 +4251,10 @@
         <v>169</v>
       </c>
       <c r="O34" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P34" s="16" t="s">
         <v>179</v>
-      </c>
-      <c r="P34" s="16" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -4265,7 +4262,7 @@
         <v>158</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>1</v>
@@ -4280,19 +4277,19 @@
         <v>37</v>
       </c>
       <c r="G35" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I35" s="13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J35" s="13" t="s">
         <v>161</v>
       </c>
       <c r="K35" s="13" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L35" s="5" t="s">
         <v>9</v>
@@ -4302,39 +4299,39 @@
         <v>160</v>
       </c>
       <c r="O35" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P35" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F36" s="13">
         <v>38</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H36" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I36" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J36" s="13" t="s">
         <v>162</v>
@@ -4347,541 +4344,541 @@
       </c>
       <c r="M36" s="5"/>
       <c r="N36" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="O36" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P36" s="16" t="s">
         <v>179</v>
-      </c>
-      <c r="P36" s="16" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>347</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>348</v>
-      </c>
       <c r="C37" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F37" s="13">
         <v>39</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H37" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I37" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K37" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L37" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M37" s="5"/>
       <c r="N37" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O37" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P37" s="16" t="s">
         <v>179</v>
-      </c>
-      <c r="P37" s="16" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F38" s="13">
         <v>41</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H38" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I38" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J38" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="K38" s="13" t="s">
         <v>195</v>
-      </c>
-      <c r="K38" s="13" t="s">
-        <v>196</v>
       </c>
       <c r="L38" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M38" s="5"/>
       <c r="N38" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="O38" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P38" s="16" t="s">
         <v>179</v>
-      </c>
-      <c r="P38" s="16" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F39" s="13">
         <v>42</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H39" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I39" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J39" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="K39" s="13" t="s">
         <v>197</v>
-      </c>
-      <c r="K39" s="13" t="s">
-        <v>198</v>
       </c>
       <c r="L39" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M39" s="5"/>
       <c r="N39" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="O39" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P39" s="16" t="s">
         <v>179</v>
-      </c>
-      <c r="P39" s="16" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>337</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="C40" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="C40" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>339</v>
-      </c>
       <c r="E40" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F40" s="13">
         <v>43</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H40" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I40" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J40" s="13" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K40" s="13" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="L40" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M40" s="5"/>
       <c r="N40" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="O40" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P40" s="16" t="s">
         <v>179</v>
-      </c>
-      <c r="P40" s="16" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F41" s="13">
         <v>44</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H41" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I41" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J41" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="K41" s="13" t="s">
         <v>199</v>
-      </c>
-      <c r="K41" s="13" t="s">
-        <v>200</v>
       </c>
       <c r="L41" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M41" s="5"/>
       <c r="N41" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O41" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P41" s="16" t="s">
         <v>179</v>
-      </c>
-      <c r="P41" s="16" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>344</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>345</v>
-      </c>
       <c r="C42" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F42" s="13">
         <v>45</v>
       </c>
       <c r="G42" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H42" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I42" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J42" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="K42" s="13" t="s">
         <v>201</v>
-      </c>
-      <c r="K42" s="13" t="s">
-        <v>202</v>
       </c>
       <c r="L42" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M42" s="5"/>
       <c r="N42" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="O42" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P42" s="16" t="s">
         <v>179</v>
-      </c>
-      <c r="P42" s="16" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F43" s="13">
         <v>46</v>
       </c>
       <c r="G43" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H43" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I43" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J43" s="27" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K43" s="27" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L43" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M43" s="5"/>
       <c r="N43" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="O43" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P43" s="16" t="s">
         <v>179</v>
-      </c>
-      <c r="P43" s="16" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F44" s="13">
         <v>48</v>
       </c>
       <c r="G44" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H44" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I44" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J44" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="K44" s="13" t="s">
         <v>310</v>
-      </c>
-      <c r="K44" s="13" t="s">
-        <v>311</v>
       </c>
       <c r="L44" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M44" s="5"/>
       <c r="N44" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O44" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P44" s="16" t="s">
         <v>179</v>
-      </c>
-      <c r="P44" s="16" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F45" s="13">
         <v>49</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H45" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I45" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J45" s="13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K45" s="13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L45" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M45" s="5"/>
       <c r="N45" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="O45" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P45" s="16" t="s">
         <v>179</v>
-      </c>
-      <c r="P45" s="16" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F46" s="13">
         <v>52</v>
       </c>
       <c r="G46" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H46" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I46" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J46" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="K46" s="18" t="s">
         <v>316</v>
-      </c>
-      <c r="K46" s="18" t="s">
-        <v>317</v>
       </c>
       <c r="L46" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M46" s="5"/>
       <c r="N46" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O46" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P46" s="16" t="s">
         <v>179</v>
-      </c>
-      <c r="P46" s="16" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F47" s="13">
         <v>53</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H47" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I47" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J47" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="K47" s="13" t="s">
         <v>308</v>
-      </c>
-      <c r="K47" s="13" t="s">
-        <v>309</v>
       </c>
       <c r="L47" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M47" s="5"/>
       <c r="N47" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="O47" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P47" s="16" t="s">
         <v>179</v>
-      </c>
-      <c r="P47" s="16" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -4889,7 +4886,7 @@
         <v>10</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>0</v>
@@ -4904,16 +4901,16 @@
         <v>1</v>
       </c>
       <c r="G48" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H48" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="I48" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="J48" s="11" t="s">
         <v>292</v>
-      </c>
-      <c r="I48" s="11" t="s">
-        <v>292</v>
-      </c>
-      <c r="J48" s="11" t="s">
-        <v>293</v>
       </c>
       <c r="K48" s="11" t="s">
         <v>52</v>
@@ -4926,10 +4923,10 @@
         <v>4</v>
       </c>
       <c r="O48" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P48" s="11" t="s">
         <v>179</v>
-      </c>
-      <c r="P48" s="11" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -4937,7 +4934,7 @@
         <v>142</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>0</v>
@@ -4952,19 +4949,19 @@
         <v>2</v>
       </c>
       <c r="G49" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H49" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I49" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J49" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="K49" s="11" t="s">
         <v>327</v>
-      </c>
-      <c r="K49" s="11" t="s">
-        <v>328</v>
       </c>
       <c r="L49" s="4" t="s">
         <v>9</v>
@@ -4974,10 +4971,10 @@
         <v>4</v>
       </c>
       <c r="O49" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P49" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -4985,7 +4982,7 @@
         <v>153</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>0</v>
@@ -5000,19 +4997,19 @@
         <v>3</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H50" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J50" s="11" t="s">
+        <v>328</v>
+      </c>
+      <c r="K50" s="11" t="s">
         <v>329</v>
-      </c>
-      <c r="K50" s="11" t="s">
-        <v>330</v>
       </c>
       <c r="L50" s="4" t="s">
         <v>9</v>
@@ -5022,10 +5019,10 @@
         <v>16</v>
       </c>
       <c r="O50" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P50" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -5033,7 +5030,7 @@
         <v>154</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>0</v>
@@ -5048,19 +5045,19 @@
         <v>4</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H51" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I51" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J51" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="K51" s="11" t="s">
         <v>331</v>
-      </c>
-      <c r="K51" s="11" t="s">
-        <v>332</v>
       </c>
       <c r="L51" s="4" t="s">
         <v>9</v>
@@ -5070,10 +5067,10 @@
         <v>16</v>
       </c>
       <c r="O51" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P51" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
@@ -5081,7 +5078,7 @@
         <v>12</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>0</v>
@@ -5096,19 +5093,19 @@
         <v>5</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H52" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I52" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J52" s="11" t="s">
+        <v>332</v>
+      </c>
+      <c r="K52" s="11" t="s">
         <v>333</v>
-      </c>
-      <c r="K52" s="11" t="s">
-        <v>334</v>
       </c>
       <c r="L52" s="4" t="s">
         <v>9</v>
@@ -5118,18 +5115,18 @@
         <v>17</v>
       </c>
       <c r="O52" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P52" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>0</v>
@@ -5138,19 +5135,19 @@
         <v>21</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F53" s="11">
         <v>6</v>
       </c>
       <c r="G53" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H53" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I53" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J53" s="11" t="s">
         <v>83</v>
@@ -5166,45 +5163,45 @@
         <v>18</v>
       </c>
       <c r="O53" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P53" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F54" s="11">
         <v>9</v>
       </c>
       <c r="G54" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H54" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I54" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J54" s="28" t="s">
+        <v>293</v>
+      </c>
+      <c r="K54" s="28" t="s">
         <v>294</v>
-      </c>
-      <c r="K54" s="28" t="s">
-        <v>295</v>
       </c>
       <c r="L54" s="4" t="s">
         <v>9</v>
@@ -5214,45 +5211,45 @@
         <v>4</v>
       </c>
       <c r="O54" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P54" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F55" s="11">
         <v>8</v>
       </c>
       <c r="G55" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H55" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I55" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J55" s="11" t="s">
+        <v>340</v>
+      </c>
+      <c r="K55" s="11" t="s">
         <v>341</v>
-      </c>
-      <c r="K55" s="11" t="s">
-        <v>342</v>
       </c>
       <c r="L55" s="4" t="s">
         <v>9</v>
@@ -5262,10 +5259,10 @@
         <v>4</v>
       </c>
       <c r="O55" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P55" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
@@ -5273,7 +5270,7 @@
         <v>127</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>5</v>
@@ -5288,10 +5285,10 @@
         <v>1</v>
       </c>
       <c r="G56" s="22" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H56" s="12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I56" s="12">
         <v>1</v>
@@ -5310,10 +5307,10 @@
         <v>123</v>
       </c>
       <c r="O56" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P56" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
@@ -5321,7 +5318,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>5</v>
@@ -5336,19 +5333,19 @@
         <v>2</v>
       </c>
       <c r="G57" s="12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H57" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I57" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J57" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="K57" s="12" t="s">
         <v>335</v>
-      </c>
-      <c r="K57" s="12" t="s">
-        <v>336</v>
       </c>
       <c r="L57" s="3" t="s">
         <v>9</v>
@@ -5358,10 +5355,10 @@
         <v>18</v>
       </c>
       <c r="O57" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P57" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
@@ -5369,7 +5366,7 @@
         <v>53</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>5</v>
@@ -5384,13 +5381,13 @@
         <v>3</v>
       </c>
       <c r="G58" s="12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H58" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I58" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J58" s="12" t="s">
         <v>155</v>
@@ -5406,10 +5403,10 @@
         <v>7</v>
       </c>
       <c r="O58" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P58" s="12" t="s">
         <v>179</v>
-      </c>
-      <c r="P58" s="12" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
@@ -5417,7 +5414,7 @@
         <v>41</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>5</v>
@@ -5432,13 +5429,13 @@
         <v>4</v>
       </c>
       <c r="G59" s="12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H59" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I59" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J59" s="12" t="s">
         <v>116</v>
@@ -5454,10 +5451,10 @@
         <v>152</v>
       </c>
       <c r="O59" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P59" s="12" t="s">
         <v>179</v>
-      </c>
-      <c r="P59" s="12" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
@@ -5465,7 +5462,7 @@
         <v>54</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>5</v>
@@ -5480,13 +5477,13 @@
         <v>5</v>
       </c>
       <c r="G60" s="12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H60" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I60" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J60" s="12" t="s">
         <v>118</v>
@@ -5502,18 +5499,18 @@
         <v>152</v>
       </c>
       <c r="O60" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P60" s="12" t="s">
         <v>179</v>
-      </c>
-      <c r="P60" s="12" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>349</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>350</v>
       </c>
       <c r="C61" s="8" t="s">
         <v>5</v>
@@ -5522,38 +5519,38 @@
         <v>22</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F61" s="12">
         <v>1</v>
       </c>
       <c r="G61" s="12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H61" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I61" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J61" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K61" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L61" s="3" t="s">
         <v>9</v>
       </c>
       <c r="M61" s="3"/>
       <c r="N61" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="O61" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P61" s="12" t="s">
         <v>179</v>
-      </c>
-      <c r="P61" s="12" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed a couple of duplicate sequences from DIGS set
</commit_message>
<xml_diff>
--- a/tabular/eve/ehbv-refseqs-side-data.xlsx
+++ b/tabular/eve/ehbv-refseqs-side-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC438172-2C86-0E4B-89FA-DA2020EA916A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C87AAF-4151-9048-A82E-1C14862F8FCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12680" yWindow="1820" windowWidth="36120" windowHeight="22320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2602,8 +2602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D27" sqref="A1:P61"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Filled out taxonomic clade level information for reference loci
</commit_message>
<xml_diff>
--- a/tabular/eve/ehbv-refseqs-side-data.xlsx
+++ b/tabular/eve/ehbv-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891E4AF2-C097-7E43-8DC3-DD6CBF8BA015}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0941A9-8E03-FB46-B53D-772F0EAD2F9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12720" yWindow="1800" windowWidth="36120" windowHeight="22320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="366">
   <si>
     <t>Herpetohepadnavirus</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Passeriformes</t>
   </si>
   <si>
-    <t>Tyto</t>
-  </si>
-  <si>
     <t>Paleognathae</t>
   </si>
   <si>
@@ -407,9 +404,6 @@
     <t>ATP2B2 (intronic)</t>
   </si>
   <si>
-    <t>Sauropsids</t>
-  </si>
-  <si>
     <t>ehbv-meta.1-sauria</t>
   </si>
   <si>
@@ -542,9 +536,6 @@
     <t>Endogenous avihepadnavirus 34</t>
   </si>
   <si>
-    <t>Leptosomidae</t>
-  </si>
-  <si>
     <t>Calypte</t>
   </si>
   <si>
@@ -677,18 +668,6 @@
     <t>ehbv-avi.35-calypte</t>
   </si>
   <si>
-    <t>passeriformes</t>
-  </si>
-  <si>
-    <t>ara</t>
-  </si>
-  <si>
-    <t>psittaciformes</t>
-  </si>
-  <si>
-    <t>antrostomus</t>
-  </si>
-  <si>
     <t>ehbv-avi.48-podiceps</t>
   </si>
   <si>
@@ -701,15 +680,6 @@
     <t>ehbv-avi.28-alauda</t>
   </si>
   <si>
-    <t>Aauda</t>
-  </si>
-  <si>
-    <t>podiceps</t>
-  </si>
-  <si>
-    <t>melopsittacus</t>
-  </si>
-  <si>
     <t>Endogenous avihepadnavirus 52</t>
   </si>
   <si>
@@ -926,9 +896,6 @@
     <t>ehbv-avi.31-passeriformes</t>
   </si>
   <si>
-    <t>picoides</t>
-  </si>
-  <si>
     <t>ehbv-avi.49-psittaciformes</t>
   </si>
   <si>
@@ -1055,9 +1022,6 @@
     <t>Endogenous avihepadnavirus 43</t>
   </si>
   <si>
-    <t>gallirallus</t>
-  </si>
-  <si>
     <t>OBI1</t>
   </si>
   <si>
@@ -1097,9 +1061,6 @@
     <t>avi.14-gavia</t>
   </si>
   <si>
-    <t>gavia</t>
-  </si>
-  <si>
     <t>ehbv-avi.15-gavia</t>
   </si>
   <si>
@@ -1112,9 +1073,6 @@
     <t>avi.12-anatidae</t>
   </si>
   <si>
-    <t>anatidae</t>
-  </si>
-  <si>
     <t>ehbv-avi.30-anatidae-con</t>
   </si>
   <si>
@@ -1134,6 +1092,48 @@
   </si>
   <si>
     <t>Family</t>
+  </si>
+  <si>
+    <t>Clade</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Tyto alba</t>
+  </si>
+  <si>
+    <t>Anatidae</t>
+  </si>
+  <si>
+    <t>Gavia</t>
+  </si>
+  <si>
+    <t>Leptosomus</t>
+  </si>
+  <si>
+    <t>Picoides</t>
+  </si>
+  <si>
+    <t>Podiceps</t>
+  </si>
+  <si>
+    <t>Antrostomus</t>
+  </si>
+  <si>
+    <t>Gallirallus</t>
+  </si>
+  <si>
+    <t>Ara</t>
+  </si>
+  <si>
+    <t>Suborder</t>
+  </si>
+  <si>
+    <t>Sauropsida</t>
+  </si>
+  <si>
+    <t>Alauda</t>
   </si>
 </sst>
 </file>
@@ -2608,8 +2608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J45" sqref="A1:P61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2631,13 +2631,13 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -2646,2249 +2646,2337 @@
         <v>3</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="13">
+        <v>1</v>
+      </c>
+      <c r="G2" s="19" t="s">
         <v>277</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F2" s="13">
-        <v>1</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>287</v>
-      </c>
       <c r="H2" s="13" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="I2" s="13">
         <v>1</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="5"/>
+      <c r="M2" s="5" t="s">
+        <v>352</v>
+      </c>
       <c r="N2" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="O2" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F3" s="13">
         <v>2</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="5"/>
+      <c r="M3" s="5" t="s">
+        <v>351</v>
+      </c>
       <c r="N3" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P3" s="12" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F4" s="13">
         <v>3</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="5"/>
+      <c r="M4" s="5" t="s">
+        <v>350</v>
+      </c>
       <c r="N4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="O4" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F5" s="13">
         <v>4</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J5" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K5" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="5"/>
+      <c r="M5" s="5" t="s">
+        <v>350</v>
+      </c>
       <c r="N5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F6" s="13">
         <v>5</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M6" s="5"/>
+      <c r="M6" s="5" t="s">
+        <v>350</v>
+      </c>
       <c r="N6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P6" s="12" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F7" s="13">
         <v>6</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H7" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I7" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J7" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="K7" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="K7" s="13" t="s">
-        <v>99</v>
-      </c>
       <c r="L7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="5"/>
+      <c r="M7" s="5" t="s">
+        <v>350</v>
+      </c>
       <c r="N7" s="5" t="s">
         <v>13</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P7" s="12" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F8" s="13">
         <v>7</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H8" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I8" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M8" s="5"/>
+      <c r="M8" s="5" t="s">
+        <v>350</v>
+      </c>
       <c r="N8" s="5" t="s">
         <v>13</v>
       </c>
       <c r="O8" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P8" s="12" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F9" s="13">
         <v>8</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I9" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M9" s="5"/>
+      <c r="M9" s="5" t="s">
+        <v>352</v>
+      </c>
       <c r="N9" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="O9" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P9" s="12" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10" s="13">
         <v>9</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="I10" s="13">
         <v>1</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M10" s="5"/>
+      <c r="M10" s="5" t="s">
+        <v>353</v>
+      </c>
       <c r="N10" s="5" t="s">
         <v>6</v>
       </c>
       <c r="O10" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P10" s="13" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F11" s="13">
         <v>10</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="I11" s="13">
         <v>1</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M11" s="5"/>
+      <c r="M11" s="5" t="s">
+        <v>353</v>
+      </c>
       <c r="N11" s="5" t="s">
         <v>6</v>
       </c>
       <c r="O11" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P11" s="13" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F12" s="13">
         <v>11</v>
       </c>
       <c r="G12" s="19" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="I12" s="13">
         <v>1</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K12" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M12" s="5"/>
+      <c r="M12" s="5" t="s">
+        <v>353</v>
+      </c>
       <c r="N12" s="5" t="s">
-        <v>14</v>
+        <v>354</v>
       </c>
       <c r="O12" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P12" s="24" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>356</v>
+        <v>343</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>357</v>
+        <v>344</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>356</v>
+        <v>343</v>
       </c>
       <c r="F13" s="13">
         <v>12</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="I13" s="13">
         <v>1</v>
       </c>
       <c r="J13" s="26" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="K13" s="26" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M13" s="5"/>
+      <c r="M13" s="5" t="s">
+        <v>351</v>
+      </c>
       <c r="N13" s="5" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="O13" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P13" s="24" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F14" s="13">
         <v>13</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H14" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I14" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M14" s="5"/>
+      <c r="M14" s="5" t="s">
+        <v>352</v>
+      </c>
       <c r="N14" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O14" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P14" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="F15" s="13">
         <v>14</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="I15" s="13">
         <v>11</v>
       </c>
       <c r="J15" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="K15" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="K15" s="13" t="s">
-        <v>88</v>
-      </c>
       <c r="L15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M15" s="5"/>
+      <c r="M15" s="5" t="s">
+        <v>353</v>
+      </c>
       <c r="N15" s="5" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="O15" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P15" s="24" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>354</v>
+        <v>341</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>354</v>
+        <v>341</v>
       </c>
       <c r="F16" s="13">
         <v>15</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="I16" s="13">
         <v>1</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K16" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M16" s="5"/>
+      <c r="M16" s="5" t="s">
+        <v>353</v>
+      </c>
       <c r="N16" s="5" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="O16" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P16" s="24" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F17" s="13">
         <v>16</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H17" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I17" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J17" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="K17" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="K17" s="13" t="s">
-        <v>115</v>
-      </c>
       <c r="L17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M17" s="5"/>
+      <c r="M17" s="5" t="s">
+        <v>353</v>
+      </c>
       <c r="N17" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O17" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P17" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F18" s="13">
         <v>18</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="I18" s="13">
         <v>1</v>
       </c>
       <c r="J18" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="K18" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="K18" s="13" t="s">
-        <v>112</v>
-      </c>
       <c r="L18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M18" s="5"/>
+      <c r="M18" s="5" t="s">
+        <v>353</v>
+      </c>
       <c r="N18" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="O18" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P18" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F19" s="13">
         <v>19</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="I19" s="13">
         <v>1</v>
       </c>
       <c r="J19" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="K19" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="K19" s="13" t="s">
-        <v>86</v>
-      </c>
       <c r="L19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M19" s="5"/>
+      <c r="M19" s="5" t="s">
+        <v>353</v>
+      </c>
       <c r="N19" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="O19" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P19" s="13" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F20" s="13">
         <v>20</v>
       </c>
       <c r="G20" s="19" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="I20" s="13">
         <v>1</v>
       </c>
       <c r="J20" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="K20" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="K20" s="27" t="s">
-        <v>90</v>
-      </c>
       <c r="L20" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M20" s="5"/>
+      <c r="M20" s="5" t="s">
+        <v>353</v>
+      </c>
       <c r="N20" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="O20" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P20" s="17" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F21" s="13">
         <v>21</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H21" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I21" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L21" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M21" s="5"/>
+      <c r="M21" s="5" t="s">
+        <v>352</v>
+      </c>
       <c r="N21" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O21" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P21" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F22" s="13">
         <v>22</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H22" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I22" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J22" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="K22" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="K22" s="13" t="s">
-        <v>105</v>
-      </c>
       <c r="L22" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M22" s="5"/>
+      <c r="M22" s="5" t="s">
+        <v>353</v>
+      </c>
       <c r="N22" s="5" t="s">
-        <v>14</v>
+        <v>354</v>
       </c>
       <c r="O22" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P22" s="24" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="F23" s="13">
         <v>23</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="H23" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I23" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J23" s="28" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="K23" s="28" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="L23" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M23" s="5"/>
+      <c r="M23" s="5" t="s">
+        <v>350</v>
+      </c>
       <c r="N23" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="O23" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P23" s="14" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F24" s="13">
         <v>24</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H24" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I24" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J24" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K24" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L24" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M24" s="5"/>
+      <c r="M24" s="5" t="s">
+        <v>353</v>
+      </c>
       <c r="N24" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="O24" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P24" s="17" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F25" s="13">
         <v>25</v>
       </c>
       <c r="G25" s="19" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="I25" s="13">
         <v>523</v>
       </c>
       <c r="J25" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="K25" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="K25" s="13" t="s">
-        <v>110</v>
-      </c>
       <c r="L25" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M25" s="5"/>
+      <c r="M25" s="5" t="s">
+        <v>353</v>
+      </c>
       <c r="N25" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="O25" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P25" s="17" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F26" s="13">
         <v>26</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="H26" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I26" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J26" s="18" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="K26" s="18" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="L26" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M26" s="5" t="s">
-        <v>364</v>
+        <v>350</v>
       </c>
       <c r="N26" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="O26" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P26" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>361</v>
+        <v>347</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
       <c r="F27" s="13">
         <v>27</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="H27" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I27" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K27" s="13" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="L27" s="5" t="s">
         <v>9</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>365</v>
+        <v>351</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>363</v>
+        <v>349</v>
       </c>
       <c r="O27" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P27" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="F28" s="13">
         <v>28</v>
       </c>
       <c r="G28" s="19" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="I28" s="13">
         <v>745</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="K28" s="13" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="L28" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M28" s="5"/>
+      <c r="M28" s="5" t="s">
+        <v>353</v>
+      </c>
       <c r="N28" s="5" t="s">
-        <v>221</v>
+        <v>365</v>
       </c>
       <c r="O28" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P28" s="13" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F29" s="13">
         <v>29</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J29" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="K29" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="K29" s="13" t="s">
-        <v>108</v>
-      </c>
       <c r="L29" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M29" s="5"/>
+      <c r="M29" s="5" t="s">
+        <v>353</v>
+      </c>
       <c r="N29" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="O29" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P29" s="14" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
       <c r="F30" s="13">
         <v>30</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H30" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I30" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J30" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="K30" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="K30" s="26" t="s">
-        <v>103</v>
-      </c>
       <c r="L30" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M30" s="5"/>
+      <c r="M30" s="5" t="s">
+        <v>351</v>
+      </c>
       <c r="N30" s="5" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="O30" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P30" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F31" s="13">
         <v>31</v>
       </c>
       <c r="G31" s="19" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="I31" s="13">
         <v>1</v>
       </c>
       <c r="J31" s="25" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="K31" s="25" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="L31" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M31" s="5"/>
+      <c r="M31" s="5" t="s">
+        <v>350</v>
+      </c>
       <c r="N31" s="5" t="s">
         <v>13</v>
       </c>
       <c r="O31" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P31" s="14" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F32" s="13">
         <v>32</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H32" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I32" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K32" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L32" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M32" s="5"/>
+      <c r="M32" s="5" t="s">
+        <v>350</v>
+      </c>
       <c r="N32" s="5" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="O32" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P32" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F33" s="13">
         <v>34</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H33" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I33" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J33" s="13" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="K33" s="13" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="L33" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M33" s="5"/>
+      <c r="M33" s="5" t="s">
+        <v>353</v>
+      </c>
       <c r="N33" s="5" t="s">
-        <v>168</v>
+        <v>357</v>
       </c>
       <c r="O33" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P33" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F34" s="13">
         <v>35</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H34" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I34" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J34" s="25" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="K34" s="25" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="L34" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M34" s="5"/>
+      <c r="M34" s="5" t="s">
+        <v>353</v>
+      </c>
       <c r="N34" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="O34" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P34" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F35" s="13">
         <v>37</v>
       </c>
       <c r="G35" s="19" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I35" s="13" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J35" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K35" s="13" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="L35" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M35" s="5"/>
+      <c r="M35" s="5" t="s">
+        <v>353</v>
+      </c>
       <c r="N35" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O35" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P35" s="14" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F36" s="13">
         <v>38</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H36" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I36" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K36" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L36" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M36" s="5"/>
+      <c r="M36" s="5" t="s">
+        <v>350</v>
+      </c>
       <c r="N36" s="5" t="s">
-        <v>213</v>
+        <v>13</v>
       </c>
       <c r="O36" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P36" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="F37" s="13">
         <v>39</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H37" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I37" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="K37" s="13" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="L37" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M37" s="5"/>
+      <c r="M37" s="5" t="s">
+        <v>353</v>
+      </c>
       <c r="N37" s="5" t="s">
-        <v>214</v>
+        <v>362</v>
       </c>
       <c r="O37" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P37" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F38" s="13">
         <v>41</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H38" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I38" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="K38" s="13" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="L38" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M38" s="5"/>
+      <c r="M38" s="5" t="s">
+        <v>350</v>
+      </c>
       <c r="N38" s="5" t="s">
-        <v>215</v>
+        <v>147</v>
       </c>
       <c r="O38" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P38" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F39" s="13">
         <v>42</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H39" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I39" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="K39" s="13" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L39" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M39" s="5"/>
+      <c r="M39" s="5" t="s">
+        <v>350</v>
+      </c>
       <c r="N39" s="5" t="s">
-        <v>213</v>
+        <v>13</v>
       </c>
       <c r="O39" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P39" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="F40" s="13">
         <v>43</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H40" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I40" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J40" s="13" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="K40" s="13" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="L40" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M40" s="5"/>
+      <c r="M40" s="5" t="s">
+        <v>353</v>
+      </c>
       <c r="N40" s="5" t="s">
-        <v>339</v>
+        <v>361</v>
       </c>
       <c r="O40" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P40" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F41" s="13">
         <v>44</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H41" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I41" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J41" s="13" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="K41" s="13" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="L41" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M41" s="5"/>
+      <c r="M41" s="5" t="s">
+        <v>353</v>
+      </c>
       <c r="N41" s="5" t="s">
-        <v>216</v>
+        <v>360</v>
       </c>
       <c r="O41" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P41" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="F42" s="13">
         <v>45</v>
       </c>
       <c r="G42" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H42" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I42" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J42" s="13" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="K42" s="13" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="L42" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="5"/>
+      <c r="M42" s="5" t="s">
+        <v>350</v>
+      </c>
       <c r="N42" s="5" t="s">
-        <v>215</v>
+        <v>147</v>
       </c>
       <c r="O42" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P42" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F43" s="13">
         <v>46</v>
       </c>
       <c r="G43" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H43" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I43" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J43" s="27" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="K43" s="27" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="L43" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M43" s="5"/>
+      <c r="M43" s="5" t="s">
+        <v>350</v>
+      </c>
       <c r="N43" s="5" t="s">
-        <v>215</v>
+        <v>147</v>
       </c>
       <c r="O43" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P43" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="F44" s="13">
         <v>48</v>
       </c>
       <c r="G44" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H44" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I44" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J44" s="13" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="K44" s="13" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="L44" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M44" s="5"/>
+      <c r="M44" s="5" t="s">
+        <v>353</v>
+      </c>
       <c r="N44" s="5" t="s">
-        <v>222</v>
+        <v>359</v>
       </c>
       <c r="O44" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P44" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="F45" s="13">
         <v>49</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H45" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I45" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J45" s="13" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="K45" s="13" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="L45" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M45" s="5"/>
+      <c r="M45" s="5" t="s">
+        <v>350</v>
+      </c>
       <c r="N45" s="5" t="s">
-        <v>215</v>
+        <v>147</v>
       </c>
       <c r="O45" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P45" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="F46" s="13">
         <v>52</v>
       </c>
       <c r="G46" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H46" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I46" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J46" s="18" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="K46" s="18" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="L46" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M46" s="5"/>
+      <c r="M46" s="5" t="s">
+        <v>353</v>
+      </c>
       <c r="N46" s="5" t="s">
-        <v>223</v>
+        <v>6</v>
       </c>
       <c r="O46" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P46" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="F47" s="13">
         <v>53</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H47" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I47" s="21" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J47" s="13" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="K47" s="13" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="L47" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M47" s="5"/>
+      <c r="M47" s="5" t="s">
+        <v>353</v>
+      </c>
       <c r="N47" s="5" t="s">
-        <v>296</v>
+        <v>358</v>
       </c>
       <c r="O47" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P47" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -4896,13 +4984,13 @@
         <v>10</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>10</v>
@@ -4911,94 +4999,98 @@
         <v>1</v>
       </c>
       <c r="G48" s="23" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="H48" s="11" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I48" s="11" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J48" s="11" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="K48" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L48" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M48" s="4"/>
+      <c r="M48" s="4" t="s">
+        <v>363</v>
+      </c>
       <c r="N48" s="4" t="s">
         <v>4</v>
       </c>
       <c r="O48" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P48" s="11" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F49" s="11">
         <v>2</v>
       </c>
       <c r="G49" s="23" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="H49" s="11" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I49" s="11" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J49" s="11" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="K49" s="11" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="L49" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M49" s="4"/>
+      <c r="M49" s="4" t="s">
+        <v>363</v>
+      </c>
       <c r="N49" s="4" t="s">
         <v>4</v>
       </c>
       <c r="O49" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="P49" s="11" t="s">
         <v>178</v>
-      </c>
-      <c r="P49" s="11" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>11</v>
@@ -5007,80 +5099,84 @@
         <v>3</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H50" s="11" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J50" s="11" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="K50" s="11" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="L50" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M50" s="4"/>
+      <c r="M50" s="4" t="s">
+        <v>350</v>
+      </c>
       <c r="N50" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O50" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P50" s="11" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F51" s="11">
         <v>4</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H51" s="11" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I51" s="11" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J51" s="11" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="K51" s="11" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="L51" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M51" s="4"/>
+      <c r="M51" s="4" t="s">
+        <v>350</v>
+      </c>
       <c r="N51" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O51" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P51" s="11" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
@@ -5088,13 +5184,13 @@
         <v>12</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>12</v>
@@ -5103,464 +5199,484 @@
         <v>5</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H52" s="11" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I52" s="11" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J52" s="11" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
       <c r="K52" s="11" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
       <c r="L52" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M52" s="4"/>
+      <c r="M52" s="4" t="s">
+        <v>350</v>
+      </c>
       <c r="N52" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O52" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="P52" s="11" t="s">
         <v>178</v>
-      </c>
-      <c r="P52" s="11" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="F53" s="11">
         <v>6</v>
       </c>
       <c r="G53" s="11" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H53" s="11" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I53" s="11" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J53" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K53" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L53" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M53" s="4"/>
+      <c r="M53" s="4" t="s">
+        <v>353</v>
+      </c>
       <c r="N53" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O53" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P53" s="11" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="F54" s="11">
         <v>9</v>
       </c>
       <c r="G54" s="23" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="H54" s="11" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I54" s="11" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J54" s="28" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="K54" s="28" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="L54" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M54" s="4"/>
+      <c r="M54" s="4" t="s">
+        <v>363</v>
+      </c>
       <c r="N54" s="4" t="s">
         <v>4</v>
       </c>
       <c r="O54" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="P54" s="11" t="s">
         <v>178</v>
-      </c>
-      <c r="P54" s="11" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F55" s="11">
         <v>8</v>
       </c>
       <c r="G55" s="23" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="H55" s="11" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I55" s="11" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J55" s="11" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="K55" s="11" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="L55" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M55" s="4"/>
+      <c r="M55" s="4" t="s">
+        <v>363</v>
+      </c>
       <c r="N55" s="4" t="s">
         <v>4</v>
       </c>
       <c r="O55" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="P55" s="11" t="s">
         <v>178</v>
-      </c>
-      <c r="P55" s="11" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F56" s="12">
         <v>1</v>
       </c>
       <c r="G56" s="22" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="H56" s="12" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="I56" s="12">
         <v>1</v>
       </c>
       <c r="J56" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="K56" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L56" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M56" s="3"/>
+      <c r="M56" s="3" t="s">
+        <v>352</v>
+      </c>
       <c r="N56" s="3" t="s">
-        <v>123</v>
+        <v>364</v>
       </c>
       <c r="O56" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P56" s="12" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F57" s="12">
         <v>2</v>
       </c>
       <c r="G57" s="12" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H57" s="12" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I57" s="12" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J57" s="12" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="K57" s="12" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="L57" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M57" s="3"/>
+      <c r="M57" s="3" t="s">
+        <v>353</v>
+      </c>
       <c r="N57" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O57" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P57" s="12" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F58" s="12">
         <v>3</v>
       </c>
       <c r="G58" s="12" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H58" s="12" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I58" s="12" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J58" s="12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K58" s="12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="L58" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M58" s="3"/>
+      <c r="M58" s="3" t="s">
+        <v>353</v>
+      </c>
       <c r="N58" s="3" t="s">
         <v>7</v>
       </c>
       <c r="O58" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P58" s="12" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F59" s="12">
         <v>4</v>
       </c>
       <c r="G59" s="12" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H59" s="12" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I59" s="12" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J59" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="K59" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="K59" s="12" t="s">
-        <v>117</v>
-      </c>
       <c r="L59" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M59" s="3"/>
+      <c r="M59" s="3" t="s">
+        <v>353</v>
+      </c>
       <c r="N59" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="O59" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P59" s="12" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F60" s="12">
         <v>5</v>
       </c>
       <c r="G60" s="12" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H60" s="12" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I60" s="12" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J60" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="K60" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="K60" s="12" t="s">
-        <v>119</v>
-      </c>
       <c r="L60" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M60" s="3"/>
+      <c r="M60" s="3" t="s">
+        <v>353</v>
+      </c>
       <c r="N60" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="O60" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P60" s="12" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="C61" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="F61" s="12">
         <v>1</v>
       </c>
       <c r="G61" s="12" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="H61" s="12" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I61" s="12" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="J61" s="12" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="K61" s="12" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="L61" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M61" s="3"/>
+      <c r="M61" s="3" t="s">
+        <v>353</v>
+      </c>
       <c r="N61" s="3" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="O61" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P61" s="12" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor - final EVE names
</commit_message>
<xml_diff>
--- a/tabular/eve/ehbv-refseqs-side-data.xlsx
+++ b/tabular/eve/ehbv-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8640BE39-FF09-EE40-AACA-63AC6F95AC75}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01BCB8F4-96C0-524D-9981-17A5065DDB66}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12720" yWindow="1800" windowWidth="36120" windowHeight="22320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="368">
   <si>
     <t>Herpetohepadnavirus</t>
   </si>
@@ -1128,6 +1128,18 @@
   </si>
   <si>
     <t>ehbv-avi.12-anatidae</t>
+  </si>
+  <si>
+    <t>Endogenous avihepadnavirus 54</t>
+  </si>
+  <si>
+    <t>Corapipo_altera</t>
+  </si>
+  <si>
+    <t>ehbv-avi.54-corapipo</t>
+  </si>
+  <si>
+    <t>avi.54-corapipo</t>
   </si>
 </sst>
 </file>
@@ -2600,10 +2612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P62"/>
+  <dimension ref="A1:P63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:P62"/>
+    <sheetView tabSelected="1" topLeftCell="F25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K49" sqref="A1:P63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -5024,73 +5036,73 @@
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="F49" s="11">
-        <v>1</v>
-      </c>
-      <c r="G49" s="23" t="s">
-        <v>263</v>
-      </c>
-      <c r="H49" s="11" t="s">
-        <v>267</v>
-      </c>
-      <c r="I49" s="11" t="s">
-        <v>267</v>
-      </c>
-      <c r="J49" s="11" t="s">
-        <v>268</v>
-      </c>
-      <c r="K49" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="L49" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M49" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="N49" s="4" t="s">
-        <v>4</v>
+      <c r="A49" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="F49" s="13">
+        <v>54</v>
+      </c>
+      <c r="G49" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="H49" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="I49" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="J49" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="K49" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="L49" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M49" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="N49" s="5" t="s">
+        <v>365</v>
       </c>
       <c r="O49" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="P49" s="11" t="s">
+      <c r="P49" s="16" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F50" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G50" s="23" t="s">
         <v>263</v>
@@ -5102,10 +5114,10 @@
         <v>267</v>
       </c>
       <c r="J50" s="11" t="s">
-        <v>301</v>
+        <v>268</v>
       </c>
       <c r="K50" s="11" t="s">
-        <v>302</v>
+        <v>48</v>
       </c>
       <c r="L50" s="4" t="s">
         <v>9</v>
@@ -5120,30 +5132,30 @@
         <v>163</v>
       </c>
       <c r="P50" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>140</v>
+        <v>358</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>210</v>
+        <v>248</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>15</v>
+        <v>131</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>140</v>
+        <v>358</v>
       </c>
       <c r="F51" s="11">
-        <v>3</v>
-      </c>
-      <c r="G51" s="11" t="s">
-        <v>264</v>
+        <v>2</v>
+      </c>
+      <c r="G51" s="23" t="s">
+        <v>263</v>
       </c>
       <c r="H51" s="11" t="s">
         <v>267</v>
@@ -5152,45 +5164,45 @@
         <v>267</v>
       </c>
       <c r="J51" s="11" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="K51" s="11" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="L51" s="4" t="s">
         <v>9</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>332</v>
+        <v>345</v>
       </c>
       <c r="N51" s="4" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="O51" s="16" t="s">
         <v>163</v>
       </c>
       <c r="P51" s="11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>129</v>
+        <v>15</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F52" s="11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G52" s="11" t="s">
         <v>264</v>
@@ -5202,10 +5214,10 @@
         <v>267</v>
       </c>
       <c r="J52" s="11" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="K52" s="11" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="L52" s="4" t="s">
         <v>9</v>
@@ -5225,22 +5237,22 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>359</v>
+        <v>141</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>249</v>
+        <v>211</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>16</v>
+        <v>129</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>359</v>
+        <v>141</v>
       </c>
       <c r="F53" s="11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G53" s="11" t="s">
         <v>264</v>
@@ -5252,10 +5264,10 @@
         <v>267</v>
       </c>
       <c r="J53" s="11" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="K53" s="11" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="L53" s="4" t="s">
         <v>9</v>
@@ -5264,33 +5276,33 @@
         <v>332</v>
       </c>
       <c r="N53" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O53" s="16" t="s">
         <v>163</v>
       </c>
       <c r="P53" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>202</v>
+        <v>359</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>212</v>
+        <v>249</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>202</v>
+        <v>359</v>
       </c>
       <c r="F54" s="11">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G54" s="11" t="s">
         <v>264</v>
@@ -5302,48 +5314,48 @@
         <v>267</v>
       </c>
       <c r="J54" s="11" t="s">
-        <v>79</v>
+        <v>307</v>
       </c>
       <c r="K54" s="11" t="s">
-        <v>79</v>
+        <v>308</v>
       </c>
       <c r="L54" s="4" t="s">
         <v>9</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="N54" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O54" s="16" t="s">
         <v>163</v>
       </c>
       <c r="P54" s="11" t="s">
-        <v>206</v>
+        <v>166</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>361</v>
+        <v>202</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>250</v>
+        <v>212</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>160</v>
+        <v>17</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>361</v>
+        <v>202</v>
       </c>
       <c r="F55" s="11">
-        <v>9</v>
-      </c>
-      <c r="G55" s="23" t="s">
-        <v>263</v>
+        <v>6</v>
+      </c>
+      <c r="G55" s="11" t="s">
+        <v>264</v>
       </c>
       <c r="H55" s="11" t="s">
         <v>267</v>
@@ -5351,46 +5363,46 @@
       <c r="I55" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="J55" s="28" t="s">
-        <v>269</v>
-      </c>
-      <c r="K55" s="28" t="s">
-        <v>270</v>
+      <c r="J55" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="K55" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="L55" s="4" t="s">
         <v>9</v>
       </c>
       <c r="M55" s="4" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="N55" s="4" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="O55" s="16" t="s">
         <v>163</v>
       </c>
       <c r="P55" s="11" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="F56" s="11">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G56" s="23" t="s">
         <v>263</v>
@@ -5401,11 +5413,11 @@
       <c r="I56" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="J56" s="11" t="s">
-        <v>314</v>
-      </c>
-      <c r="K56" s="11" t="s">
-        <v>315</v>
+      <c r="J56" s="28" t="s">
+        <v>269</v>
+      </c>
+      <c r="K56" s="28" t="s">
+        <v>270</v>
       </c>
       <c r="L56" s="4" t="s">
         <v>9</v>
@@ -5424,123 +5436,123 @@
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="F57" s="12">
-        <v>1</v>
-      </c>
-      <c r="G57" s="22" t="s">
+      <c r="A57" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="F57" s="11">
+        <v>8</v>
+      </c>
+      <c r="G57" s="23" t="s">
         <v>263</v>
       </c>
-      <c r="H57" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="I57" s="12">
-        <v>1</v>
-      </c>
-      <c r="J57" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="K57" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="L57" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="M57" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="N57" s="3" t="s">
-        <v>346</v>
+      <c r="H57" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="I57" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="J57" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="K57" s="11" t="s">
+        <v>315</v>
+      </c>
+      <c r="L57" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M57" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="N57" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="O57" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="P57" s="12" t="s">
-        <v>167</v>
+      <c r="P57" s="11" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>51</v>
+        <v>119</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>213</v>
+        <v>252</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>51</v>
+        <v>119</v>
       </c>
       <c r="F58" s="12">
-        <v>2</v>
-      </c>
-      <c r="G58" s="12" t="s">
-        <v>264</v>
+        <v>1</v>
+      </c>
+      <c r="G58" s="22" t="s">
+        <v>263</v>
       </c>
       <c r="H58" s="12" t="s">
-        <v>267</v>
-      </c>
-      <c r="I58" s="12" t="s">
-        <v>267</v>
+        <v>261</v>
+      </c>
+      <c r="I58" s="12">
+        <v>1</v>
       </c>
       <c r="J58" s="12" t="s">
-        <v>309</v>
+        <v>143</v>
       </c>
       <c r="K58" s="12" t="s">
-        <v>310</v>
+        <v>144</v>
       </c>
       <c r="L58" s="3" t="s">
         <v>9</v>
       </c>
       <c r="M58" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N58" s="3" t="s">
-        <v>14</v>
+        <v>346</v>
       </c>
       <c r="O58" s="16" t="s">
         <v>163</v>
       </c>
       <c r="P58" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F59" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G59" s="12" t="s">
         <v>264</v>
@@ -5552,10 +5564,10 @@
         <v>267</v>
       </c>
       <c r="J59" s="12" t="s">
-        <v>142</v>
+        <v>309</v>
       </c>
       <c r="K59" s="12" t="s">
-        <v>142</v>
+        <v>310</v>
       </c>
       <c r="L59" s="3" t="s">
         <v>9</v>
@@ -5564,33 +5576,33 @@
         <v>335</v>
       </c>
       <c r="N59" s="3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="O59" s="16" t="s">
         <v>163</v>
       </c>
       <c r="P59" s="12" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="F60" s="12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G60" s="12" t="s">
         <v>264</v>
@@ -5602,10 +5614,10 @@
         <v>267</v>
       </c>
       <c r="J60" s="12" t="s">
-        <v>112</v>
+        <v>142</v>
       </c>
       <c r="K60" s="12" t="s">
-        <v>113</v>
+        <v>142</v>
       </c>
       <c r="L60" s="3" t="s">
         <v>9</v>
@@ -5614,7 +5626,7 @@
         <v>335</v>
       </c>
       <c r="N60" s="3" t="s">
-        <v>139</v>
+        <v>7</v>
       </c>
       <c r="O60" s="16" t="s">
         <v>163</v>
@@ -5625,22 +5637,22 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C61" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="F61" s="12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G61" s="12" t="s">
         <v>264</v>
@@ -5652,10 +5664,10 @@
         <v>267</v>
       </c>
       <c r="J61" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K61" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L61" s="3" t="s">
         <v>9</v>
@@ -5675,22 +5687,22 @@
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>322</v>
+        <v>50</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>323</v>
+        <v>216</v>
       </c>
       <c r="C62" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>322</v>
+        <v>50</v>
       </c>
       <c r="F62" s="12">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G62" s="12" t="s">
         <v>264</v>
@@ -5702,10 +5714,10 @@
         <v>267</v>
       </c>
       <c r="J62" s="12" t="s">
-        <v>267</v>
+        <v>114</v>
       </c>
       <c r="K62" s="12" t="s">
-        <v>267</v>
+        <v>115</v>
       </c>
       <c r="L62" s="3" t="s">
         <v>9</v>
@@ -5714,7 +5726,7 @@
         <v>335</v>
       </c>
       <c r="N62" s="3" t="s">
-        <v>324</v>
+        <v>139</v>
       </c>
       <c r="O62" s="16" t="s">
         <v>163</v>
@@ -5723,11 +5735,61 @@
         <v>164</v>
       </c>
     </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="F63" s="12">
+        <v>1</v>
+      </c>
+      <c r="G63" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="H63" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="I63" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="J63" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="K63" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="L63" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M63" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="N63" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="O63" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="P63" s="12" t="s">
+        <v>164</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:N1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P61">
-    <sortCondition ref="C2:C61"/>
-    <sortCondition ref="F2:F61"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P62">
+    <sortCondition ref="C2:C62"/>
+    <sortCondition ref="F2:F62"/>
   </sortState>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>